<commit_message>
Restore all old previous chapter advisor details
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516DBF59-9E75-054C-AFB0-23EA6C83F8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DB52921-185D-DE44-99B5-3E46D26D3D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="180" windowWidth="28800" windowHeight="16300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Overview" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1591" uniqueCount="910">
   <si>
     <t>2022 Zone Activity Review</t>
   </si>
@@ -2646,6 +2646,144 @@
   </si>
   <si>
     <t>2019;2021</t>
+  </si>
+  <si>
+    <t>Professor Rudra Kafle</t>
+  </si>
+  <si>
+    <t>Kristina A. Lynch</t>
+  </si>
+  <si>
+    <t>Robert Cordery</t>
+  </si>
+  <si>
+    <t>David Morin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joe Checkelsky
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spencer Smith
+</t>
+  </si>
+  <si>
+    <t>Professor William Karstens</t>
+  </si>
+  <si>
+    <t>Joyce Palmer-Fortune</t>
+  </si>
+  <si>
+    <t>Frank Dudish</t>
+  </si>
+  <si>
+    <t>Sumientra Rampersad</t>
+  </si>
+  <si>
+    <t>Dr. Benjamin Chandran</t>
+  </si>
+  <si>
+    <t>Rudra Kafle</t>
+  </si>
+  <si>
+    <t>Sarah Demers</t>
+  </si>
+  <si>
+    <t>William Loinaz</t>
+  </si>
+  <si>
+    <t>Robert Carey</t>
+  </si>
+  <si>
+    <t>Dr. Thayaparan Paramanathan</t>
+  </si>
+  <si>
+    <t>Thomas Burton</t>
+  </si>
+  <si>
+    <t>Joseph Ribaudo</t>
+  </si>
+  <si>
+    <t>Matt Guthrie</t>
+  </si>
+  <si>
+    <t>Ben Brau</t>
+  </si>
+  <si>
+    <t>John Smedley</t>
+  </si>
+  <si>
+    <t>Mark O. Battle</t>
+  </si>
+  <si>
+    <t>Richard Fell</t>
+  </si>
+  <si>
+    <t>Dr. Michael Boyer</t>
+  </si>
+  <si>
+    <t>Dr. Michael Weinstein</t>
+  </si>
+  <si>
+    <t>Dr. Cornely</t>
+  </si>
+  <si>
+    <t>Dr. Steven Harfenist</t>
+  </si>
+  <si>
+    <t>Richard Hyde</t>
+  </si>
+  <si>
+    <t>Nancy Lee</t>
+  </si>
+  <si>
+    <t>Sps Advisor</t>
+  </si>
+  <si>
+    <t>Loraine Allen</t>
+  </si>
+  <si>
+    <t>James McDonald</t>
+  </si>
+  <si>
+    <t>Gerald Darling</t>
+  </si>
+  <si>
+    <t>Paul Nakroshis</t>
+  </si>
+  <si>
+    <t>Candice Etson</t>
+  </si>
+  <si>
+    <t>Alica Chance</t>
+  </si>
+  <si>
+    <t>Kristina.A.Lynch@dartmouth.edu</t>
+  </si>
+  <si>
+    <t>checkelsky@mit.edu</t>
+  </si>
+  <si>
+    <t>smiths@mtholyoke.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ngugliucci@anselm.edu
+</t>
+  </si>
+  <si>
+    <t>frank.dudish@maine.edu</t>
+  </si>
+  <si>
+    <t>rpk101@wpi.edu</t>
+  </si>
+  <si>
+    <t>sarah.demers@yale.edu</t>
+  </si>
+  <si>
+    <t>TPARAMANATHAN@bridgew.edu</t>
+  </si>
+  <si>
+    <t>fell@brandeis.edu</t>
   </si>
 </sst>
 </file>
@@ -2664,49 +2802,58 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF1F1F1F"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2868,7 +3015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3003,18 +3150,54 @@
     <xf numFmtId="46" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFCCCCCC"/>
+          <bgColor rgb="FFCCCCCC"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3042,9 +3225,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Activity Report-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="secondRowStripe" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="secondRowStripe" dxfId="1"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3059,7 +3242,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AZ74" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AZ1048576" headerRowCount="0">
   <tableColumns count="52">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -3082,7 +3265,7 @@
     <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Column19"/>
     <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Column20"/>
     <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Column21"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Column22" dataDxfId="0"/>
     <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Column23"/>
     <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Column24"/>
     <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Column25"/>
@@ -3424,21 +3607,21 @@
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -4525,10 +4708,10 @@
   <dimension ref="A1:AZ1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF12" sqref="AF12"/>
+      <selection pane="bottomRight" activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4649,10 +4832,10 @@
       <c r="U1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="62" t="s">
+      <c r="V1" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="W1" s="62" t="s">
+      <c r="W1" s="16" t="s">
         <v>47</v>
       </c>
       <c r="X1" s="16" t="s">
@@ -4682,7 +4865,7 @@
       <c r="AF1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="AG1" s="62" t="s">
+      <c r="AG1" s="60" t="s">
         <v>57</v>
       </c>
       <c r="AH1" s="16" t="s">
@@ -4803,8 +4986,12 @@
       <c r="U2" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V2" s="24"/>
-      <c r="W2" s="23"/>
+      <c r="V2" s="39" t="s">
+        <v>865</v>
+      </c>
+      <c r="W2" s="63" t="s">
+        <v>77</v>
+      </c>
       <c r="X2" s="23" t="s">
         <v>85</v>
       </c>
@@ -4937,8 +5124,12 @@
       <c r="U3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
+      <c r="V3" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="W3" s="63" t="s">
+        <v>108</v>
+      </c>
       <c r="X3" s="23" t="s">
         <v>85</v>
       </c>
@@ -5057,8 +5248,12 @@
       <c r="U4" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27"/>
+      <c r="V4" s="64" t="s">
+        <v>866</v>
+      </c>
+      <c r="W4" s="64" t="s">
+        <v>901</v>
+      </c>
       <c r="X4" s="23" t="s">
         <v>85</v>
       </c>
@@ -5171,8 +5366,12 @@
       </c>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
+      <c r="V5" s="63" t="s">
+        <v>867</v>
+      </c>
+      <c r="W5" s="63" t="s">
+        <v>133</v>
+      </c>
       <c r="X5" s="23"/>
       <c r="Y5" s="23"/>
       <c r="Z5" s="23" t="s">
@@ -5279,8 +5478,12 @@
       <c r="U6" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
+      <c r="V6" s="63" t="s">
+        <v>868</v>
+      </c>
+      <c r="W6" s="63" t="s">
+        <v>145</v>
+      </c>
       <c r="X6" s="23"/>
       <c r="Y6" s="23"/>
       <c r="Z6" s="23" t="s">
@@ -5403,8 +5606,12 @@
       <c r="U7" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
+      <c r="V7" s="63" t="s">
+        <v>869</v>
+      </c>
+      <c r="W7" s="63" t="s">
+        <v>902</v>
+      </c>
       <c r="X7" s="23" t="s">
         <v>166</v>
       </c>
@@ -5541,8 +5748,12 @@
       <c r="U8" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="V8" s="26"/>
-      <c r="W8" s="26"/>
+      <c r="V8" s="26" t="s">
+        <v>870</v>
+      </c>
+      <c r="W8" s="26" t="s">
+        <v>903</v>
+      </c>
       <c r="X8" s="26" t="s">
         <v>85</v>
       </c>
@@ -5671,8 +5882,12 @@
       </c>
       <c r="T9" s="23"/>
       <c r="U9" s="23"/>
-      <c r="V9" s="26"/>
-      <c r="W9" s="26"/>
+      <c r="V9" s="26" t="s">
+        <v>206</v>
+      </c>
+      <c r="W9" s="26" t="s">
+        <v>904</v>
+      </c>
       <c r="X9" s="23"/>
       <c r="Y9" s="23"/>
       <c r="Z9" s="23" t="s">
@@ -5789,8 +6004,12 @@
       </c>
       <c r="T10" s="23"/>
       <c r="U10" s="23"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
+      <c r="V10" s="26" t="s">
+        <v>871</v>
+      </c>
+      <c r="W10" s="26" t="s">
+        <v>223</v>
+      </c>
       <c r="X10" s="23"/>
       <c r="Y10" s="23"/>
       <c r="Z10" s="23" t="s">
@@ -5907,8 +6126,12 @@
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
+      <c r="V11" s="63" t="s">
+        <v>872</v>
+      </c>
+      <c r="W11" s="63" t="s">
+        <v>238</v>
+      </c>
       <c r="X11" s="23"/>
       <c r="Y11" s="23"/>
       <c r="Z11" s="23" t="s">
@@ -6037,8 +6260,12 @@
       <c r="U12" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V12" s="23"/>
-      <c r="W12" s="23"/>
+      <c r="V12" s="63" t="s">
+        <v>262</v>
+      </c>
+      <c r="W12" s="63" t="s">
+        <v>263</v>
+      </c>
       <c r="X12" s="23" t="s">
         <v>85</v>
       </c>
@@ -6163,8 +6390,12 @@
       <c r="U13" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V13" s="23"/>
-      <c r="W13" s="23"/>
+      <c r="V13" s="63" t="s">
+        <v>276</v>
+      </c>
+      <c r="W13" s="63" t="s">
+        <v>277</v>
+      </c>
       <c r="X13" s="23" t="s">
         <v>85</v>
       </c>
@@ -6285,8 +6516,12 @@
       <c r="U14" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V14" s="23"/>
-      <c r="W14" s="23"/>
+      <c r="V14" s="63" t="s">
+        <v>289</v>
+      </c>
+      <c r="W14" s="63" t="s">
+        <v>290</v>
+      </c>
       <c r="X14" s="23"/>
       <c r="Y14" s="23"/>
       <c r="Z14" s="23" t="s">
@@ -6417,8 +6652,12 @@
       <c r="U15" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
+      <c r="V15" s="64" t="s">
+        <v>873</v>
+      </c>
+      <c r="W15" s="64" t="s">
+        <v>905</v>
+      </c>
       <c r="X15" s="23" t="s">
         <v>315</v>
       </c>
@@ -6559,8 +6798,12 @@
       <c r="U16" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
+      <c r="V16" s="64" t="s">
+        <v>874</v>
+      </c>
+      <c r="W16" s="64" t="s">
+        <v>334</v>
+      </c>
       <c r="X16" s="23" t="s">
         <v>85</v>
       </c>
@@ -6681,8 +6924,12 @@
       <c r="U17" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V17" s="23"/>
-      <c r="W17" s="23"/>
+      <c r="V17" s="63" t="s">
+        <v>352</v>
+      </c>
+      <c r="W17" s="63" t="s">
+        <v>353</v>
+      </c>
       <c r="X17" s="23" t="s">
         <v>85</v>
       </c>
@@ -6815,8 +7062,12 @@
       <c r="U18" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V18" s="23"/>
-      <c r="W18" s="23"/>
+      <c r="V18" s="63" t="s">
+        <v>875</v>
+      </c>
+      <c r="W18" s="63" t="s">
+        <v>368</v>
+      </c>
       <c r="X18" s="23" t="s">
         <v>85</v>
       </c>
@@ -6933,8 +7184,12 @@
       <c r="U19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
+      <c r="V19" s="63" t="s">
+        <v>385</v>
+      </c>
+      <c r="W19" s="63" t="s">
+        <v>386</v>
+      </c>
       <c r="X19" s="23" t="s">
         <v>85</v>
       </c>
@@ -7065,8 +7320,12 @@
       </c>
       <c r="T20" s="23"/>
       <c r="U20" s="23"/>
-      <c r="V20" s="26"/>
-      <c r="W20" s="26"/>
+      <c r="V20" s="26" t="s">
+        <v>876</v>
+      </c>
+      <c r="W20" s="26" t="s">
+        <v>906</v>
+      </c>
       <c r="X20" s="23"/>
       <c r="Y20" s="23"/>
       <c r="Z20" s="23" t="s">
@@ -7195,8 +7454,12 @@
       </c>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
+      <c r="V21" s="64" t="s">
+        <v>877</v>
+      </c>
+      <c r="W21" s="64" t="s">
+        <v>907</v>
+      </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
       <c r="Z21" s="24" t="s">
@@ -7311,8 +7574,12 @@
       <c r="S22" s="45"/>
       <c r="T22" s="45"/>
       <c r="U22" s="45"/>
-      <c r="V22" s="45"/>
-      <c r="W22" s="45"/>
+      <c r="V22" s="65" t="s">
+        <v>878</v>
+      </c>
+      <c r="W22" s="65" t="s">
+        <v>444</v>
+      </c>
       <c r="X22" s="45"/>
       <c r="Y22" s="45"/>
       <c r="Z22" s="45"/>
@@ -7417,8 +7684,12 @@
       <c r="U23" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V23" s="50"/>
-      <c r="W23" s="50"/>
+      <c r="V23" s="66" t="s">
+        <v>879</v>
+      </c>
+      <c r="W23" s="66" t="s">
+        <v>453</v>
+      </c>
       <c r="X23" s="50"/>
       <c r="Y23" s="50"/>
       <c r="Z23" s="50" t="s">
@@ -7541,8 +7812,12 @@
       <c r="U24" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V24" s="50"/>
-      <c r="W24" s="50"/>
+      <c r="V24" s="66" t="s">
+        <v>880</v>
+      </c>
+      <c r="W24" s="66" t="s">
+        <v>908</v>
+      </c>
       <c r="X24" s="50"/>
       <c r="Y24" s="50"/>
       <c r="Z24" s="50" t="s">
@@ -7667,8 +7942,12 @@
       <c r="U25" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V25" s="50"/>
-      <c r="W25" s="50"/>
+      <c r="V25" s="66" t="s">
+        <v>881</v>
+      </c>
+      <c r="W25" s="66" t="s">
+        <v>499</v>
+      </c>
       <c r="X25" s="50"/>
       <c r="Y25" s="50"/>
       <c r="Z25" s="50" t="s">
@@ -7797,8 +8076,12 @@
       <c r="U26" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V26" s="50"/>
-      <c r="W26" s="50"/>
+      <c r="V26" s="66" t="s">
+        <v>882</v>
+      </c>
+      <c r="W26" s="66" t="s">
+        <v>518</v>
+      </c>
       <c r="X26" s="50" t="s">
         <v>85</v>
       </c>
@@ -7917,8 +8200,12 @@
       <c r="U27" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="V27" s="45"/>
-      <c r="W27" s="45"/>
+      <c r="V27" s="65" t="s">
+        <v>883</v>
+      </c>
+      <c r="W27" s="65" t="s">
+        <v>525</v>
+      </c>
       <c r="X27" s="45" t="s">
         <v>85</v>
       </c>
@@ -8027,8 +8314,12 @@
       <c r="U28" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
+      <c r="V28" s="51" t="s">
+        <v>884</v>
+      </c>
+      <c r="W28" s="51" t="s">
+        <v>538</v>
+      </c>
       <c r="X28" s="51" t="s">
         <v>85</v>
       </c>
@@ -8235,8 +8526,8 @@
       <c r="S30" s="55"/>
       <c r="T30" s="55"/>
       <c r="U30" s="55"/>
-      <c r="V30" s="55"/>
-      <c r="W30" s="55"/>
+      <c r="V30" s="67"/>
+      <c r="W30" s="67"/>
       <c r="X30" s="55"/>
       <c r="Y30" s="55"/>
       <c r="Z30" s="55" t="s">
@@ -8309,8 +8600,8 @@
       <c r="S31" s="55"/>
       <c r="T31" s="55"/>
       <c r="U31" s="55"/>
-      <c r="V31" s="55"/>
-      <c r="W31" s="55"/>
+      <c r="V31" s="67"/>
+      <c r="W31" s="67"/>
       <c r="X31" s="55"/>
       <c r="Y31" s="55"/>
       <c r="Z31" s="55" t="s">
@@ -8397,8 +8688,12 @@
       <c r="S32" s="55"/>
       <c r="T32" s="55"/>
       <c r="U32" s="55"/>
-      <c r="V32" s="55"/>
-      <c r="W32" s="55"/>
+      <c r="V32" s="67" t="s">
+        <v>885</v>
+      </c>
+      <c r="W32" s="67" t="s">
+        <v>569</v>
+      </c>
       <c r="X32" s="55"/>
       <c r="Y32" s="55"/>
       <c r="Z32" s="55" t="s">
@@ -8475,8 +8770,8 @@
       <c r="S33" s="55"/>
       <c r="T33" s="55"/>
       <c r="U33" s="55"/>
-      <c r="V33" s="55"/>
-      <c r="W33" s="55"/>
+      <c r="V33" s="67"/>
+      <c r="W33" s="67"/>
       <c r="X33" s="55"/>
       <c r="Y33" s="55"/>
       <c r="Z33" s="55" t="s">
@@ -8549,8 +8844,8 @@
       <c r="S34" s="55"/>
       <c r="T34" s="55"/>
       <c r="U34" s="55"/>
-      <c r="V34" s="55"/>
-      <c r="W34" s="55"/>
+      <c r="V34" s="67"/>
+      <c r="W34" s="67"/>
       <c r="X34" s="55"/>
       <c r="Y34" s="55"/>
       <c r="Z34" s="55" t="s">
@@ -8639,8 +8934,12 @@
       <c r="S35" s="55"/>
       <c r="T35" s="55"/>
       <c r="U35" s="55"/>
-      <c r="V35" s="55"/>
-      <c r="W35" s="55"/>
+      <c r="V35" s="67" t="s">
+        <v>886</v>
+      </c>
+      <c r="W35" s="67" t="s">
+        <v>581</v>
+      </c>
       <c r="X35" s="55"/>
       <c r="Y35" s="55"/>
       <c r="Z35" s="55" t="s">
@@ -8743,8 +9042,12 @@
       <c r="U36" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V36" s="55"/>
-      <c r="W36" s="55"/>
+      <c r="V36" s="67" t="s">
+        <v>887</v>
+      </c>
+      <c r="W36" s="67" t="s">
+        <v>909</v>
+      </c>
       <c r="X36" s="55" t="s">
         <v>85</v>
       </c>
@@ -8825,8 +9128,8 @@
       <c r="S37" s="55"/>
       <c r="T37" s="55"/>
       <c r="U37" s="55"/>
-      <c r="V37" s="55"/>
-      <c r="W37" s="55"/>
+      <c r="V37" s="67"/>
+      <c r="W37" s="67"/>
       <c r="X37" s="55"/>
       <c r="Y37" s="55"/>
       <c r="Z37" s="55" t="s">
@@ -8925,8 +9228,12 @@
       <c r="U38" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V38" s="55"/>
-      <c r="W38" s="55"/>
+      <c r="V38" s="67" t="s">
+        <v>606</v>
+      </c>
+      <c r="W38" s="67" t="s">
+        <v>601</v>
+      </c>
       <c r="X38" s="55" t="s">
         <v>85</v>
       </c>
@@ -9041,8 +9348,12 @@
       <c r="U39" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V39" s="55"/>
-      <c r="W39" s="55"/>
+      <c r="V39" s="67" t="s">
+        <v>888</v>
+      </c>
+      <c r="W39" s="67" t="s">
+        <v>612</v>
+      </c>
       <c r="X39" s="55" t="s">
         <v>85</v>
       </c>
@@ -9151,8 +9462,12 @@
       </c>
       <c r="T40" s="55"/>
       <c r="U40" s="55"/>
-      <c r="V40" s="55"/>
-      <c r="W40" s="55"/>
+      <c r="V40" s="67" t="s">
+        <v>627</v>
+      </c>
+      <c r="W40" s="67" t="s">
+        <v>628</v>
+      </c>
       <c r="X40" s="55"/>
       <c r="Y40" s="55"/>
       <c r="Z40" s="55" t="s">
@@ -9261,8 +9576,12 @@
       <c r="U41" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V41" s="55"/>
-      <c r="W41" s="55"/>
+      <c r="V41" s="67" t="s">
+        <v>634</v>
+      </c>
+      <c r="W41" s="67" t="s">
+        <v>630</v>
+      </c>
       <c r="X41" s="55" t="s">
         <v>85</v>
       </c>
@@ -9375,8 +9694,12 @@
       <c r="U42" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V42" s="55"/>
-      <c r="W42" s="55"/>
+      <c r="V42" s="67" t="s">
+        <v>889</v>
+      </c>
+      <c r="W42" s="67" t="s">
+        <v>638</v>
+      </c>
       <c r="X42" s="55" t="s">
         <v>85</v>
       </c>
@@ -9481,8 +9804,12 @@
       <c r="U43" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V43" s="55"/>
-      <c r="W43" s="55"/>
+      <c r="V43" s="67" t="s">
+        <v>890</v>
+      </c>
+      <c r="W43" s="67" t="s">
+        <v>647</v>
+      </c>
       <c r="X43" s="55" t="s">
         <v>85</v>
       </c>
@@ -9563,8 +9890,8 @@
       <c r="S44" s="55"/>
       <c r="T44" s="55"/>
       <c r="U44" s="55"/>
-      <c r="V44" s="55"/>
-      <c r="W44" s="55"/>
+      <c r="V44" s="67"/>
+      <c r="W44" s="67"/>
       <c r="X44" s="55"/>
       <c r="Y44" s="55"/>
       <c r="Z44" s="55" t="s">
@@ -9635,8 +9962,8 @@
       <c r="S45" s="55"/>
       <c r="T45" s="55"/>
       <c r="U45" s="55"/>
-      <c r="V45" s="55"/>
-      <c r="W45" s="55"/>
+      <c r="V45" s="67"/>
+      <c r="W45" s="67"/>
       <c r="X45" s="55"/>
       <c r="Y45" s="55"/>
       <c r="Z45" s="55" t="s">
@@ -9709,8 +10036,8 @@
       <c r="S46" s="55"/>
       <c r="T46" s="55"/>
       <c r="U46" s="55"/>
-      <c r="V46" s="55"/>
-      <c r="W46" s="55"/>
+      <c r="V46" s="67"/>
+      <c r="W46" s="67"/>
       <c r="X46" s="55"/>
       <c r="Y46" s="55"/>
       <c r="Z46" s="55" t="s">
@@ -9807,8 +10134,12 @@
       <c r="U47" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V47" s="55"/>
-      <c r="W47" s="55"/>
+      <c r="V47" s="67" t="s">
+        <v>664</v>
+      </c>
+      <c r="W47" s="67" t="s">
+        <v>659</v>
+      </c>
       <c r="X47" s="55" t="s">
         <v>85</v>
       </c>
@@ -9909,8 +10240,8 @@
       <c r="S48" s="55"/>
       <c r="T48" s="55"/>
       <c r="U48" s="55"/>
-      <c r="V48" s="55"/>
-      <c r="W48" s="55"/>
+      <c r="V48" s="67"/>
+      <c r="W48" s="67"/>
       <c r="X48" s="55"/>
       <c r="Y48" s="55"/>
       <c r="Z48" s="55" t="s">
@@ -10009,8 +10340,12 @@
       <c r="U49" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V49" s="55"/>
-      <c r="W49" s="55"/>
+      <c r="V49" s="67" t="s">
+        <v>891</v>
+      </c>
+      <c r="W49" s="67" t="s">
+        <v>677</v>
+      </c>
       <c r="X49" s="55" t="s">
         <v>85</v>
       </c>
@@ -10103,8 +10438,8 @@
       <c r="S50" s="55"/>
       <c r="T50" s="55"/>
       <c r="U50" s="55"/>
-      <c r="V50" s="55"/>
-      <c r="W50" s="55"/>
+      <c r="V50" s="67"/>
+      <c r="W50" s="67"/>
       <c r="X50" s="55"/>
       <c r="Y50" s="55"/>
       <c r="Z50" s="55" t="s">
@@ -10187,8 +10522,8 @@
       <c r="S51" s="55"/>
       <c r="T51" s="55"/>
       <c r="U51" s="55"/>
-      <c r="V51" s="55"/>
-      <c r="W51" s="55"/>
+      <c r="V51" s="67"/>
+      <c r="W51" s="67"/>
       <c r="X51" s="55"/>
       <c r="Y51" s="55"/>
       <c r="Z51" s="55" t="s">
@@ -10277,8 +10612,8 @@
       <c r="S52" s="55"/>
       <c r="T52" s="55"/>
       <c r="U52" s="55"/>
-      <c r="V52" s="55"/>
-      <c r="W52" s="55"/>
+      <c r="V52" s="67"/>
+      <c r="W52" s="67"/>
       <c r="X52" s="55"/>
       <c r="Y52" s="55"/>
       <c r="Z52" s="55" t="s">
@@ -10379,8 +10714,12 @@
       <c r="U53" s="55" t="s">
         <v>709</v>
       </c>
-      <c r="V53" s="55"/>
-      <c r="W53" s="55"/>
+      <c r="V53" s="67" t="s">
+        <v>708</v>
+      </c>
+      <c r="W53" s="67" t="s">
+        <v>704</v>
+      </c>
       <c r="X53" s="55" t="s">
         <v>85</v>
       </c>
@@ -10483,8 +10822,12 @@
       <c r="S54" s="55"/>
       <c r="T54" s="55"/>
       <c r="U54" s="55"/>
-      <c r="V54" s="55"/>
-      <c r="W54" s="55"/>
+      <c r="V54" s="67" t="s">
+        <v>892</v>
+      </c>
+      <c r="W54" s="67" t="s">
+        <v>714</v>
+      </c>
       <c r="X54" s="55"/>
       <c r="Y54" s="55"/>
       <c r="Z54" s="55" t="s">
@@ -10563,8 +10906,8 @@
       <c r="S55" s="55"/>
       <c r="T55" s="55"/>
       <c r="U55" s="55"/>
-      <c r="V55" s="55"/>
-      <c r="W55" s="55"/>
+      <c r="V55" s="67"/>
+      <c r="W55" s="67"/>
       <c r="X55" s="55"/>
       <c r="Y55" s="55"/>
       <c r="Z55" s="55" t="s">
@@ -10651,8 +10994,12 @@
       <c r="U56" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V56" s="55"/>
-      <c r="W56" s="55"/>
+      <c r="V56" s="67" t="s">
+        <v>893</v>
+      </c>
+      <c r="W56" s="67" t="s">
+        <v>724</v>
+      </c>
       <c r="X56" s="55" t="s">
         <v>85</v>
       </c>
@@ -10737,8 +11084,8 @@
       <c r="S57" s="55"/>
       <c r="T57" s="55"/>
       <c r="U57" s="55"/>
-      <c r="V57" s="55"/>
-      <c r="W57" s="55"/>
+      <c r="V57" s="67"/>
+      <c r="W57" s="67"/>
       <c r="X57" s="55"/>
       <c r="Y57" s="55"/>
       <c r="Z57" s="55" t="s">
@@ -10831,8 +11178,12 @@
       <c r="U58" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V58" s="55"/>
-      <c r="W58" s="55"/>
+      <c r="V58" s="67" t="s">
+        <v>737</v>
+      </c>
+      <c r="W58" s="67" t="s">
+        <v>734</v>
+      </c>
       <c r="X58" s="55" t="s">
         <v>85</v>
       </c>
@@ -10937,8 +11288,12 @@
       <c r="S59" s="55"/>
       <c r="T59" s="55"/>
       <c r="U59" s="55"/>
-      <c r="V59" s="55"/>
-      <c r="W59" s="55"/>
+      <c r="V59" s="67" t="s">
+        <v>894</v>
+      </c>
+      <c r="W59" s="67" t="s">
+        <v>740</v>
+      </c>
       <c r="X59" s="55"/>
       <c r="Y59" s="55"/>
       <c r="Z59" s="55" t="s">
@@ -11037,8 +11392,12 @@
       <c r="U60" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V60" s="55"/>
-      <c r="W60" s="55"/>
+      <c r="V60" s="67" t="s">
+        <v>895</v>
+      </c>
+      <c r="W60" s="67" t="s">
+        <v>752</v>
+      </c>
       <c r="X60" s="55" t="s">
         <v>85</v>
       </c>
@@ -11135,8 +11494,8 @@
       <c r="U61" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V61" s="55"/>
-      <c r="W61" s="55"/>
+      <c r="V61" s="67"/>
+      <c r="W61" s="67"/>
       <c r="X61" s="55" t="s">
         <v>85</v>
       </c>
@@ -11233,8 +11592,12 @@
       <c r="U62" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V62" s="55"/>
-      <c r="W62" s="55"/>
+      <c r="V62" s="67" t="s">
+        <v>896</v>
+      </c>
+      <c r="W62" s="67" t="s">
+        <v>761</v>
+      </c>
       <c r="X62" s="55" t="s">
         <v>85</v>
       </c>
@@ -11319,8 +11682,8 @@
       <c r="S63" s="55"/>
       <c r="T63" s="55"/>
       <c r="U63" s="55"/>
-      <c r="V63" s="55"/>
-      <c r="W63" s="55"/>
+      <c r="V63" s="67"/>
+      <c r="W63" s="67"/>
       <c r="X63" s="55"/>
       <c r="Y63" s="55"/>
       <c r="Z63" s="55" t="s">
@@ -11417,8 +11780,12 @@
       <c r="U64" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V64" s="55"/>
-      <c r="W64" s="55"/>
+      <c r="V64" s="67" t="s">
+        <v>776</v>
+      </c>
+      <c r="W64" s="67" t="s">
+        <v>771</v>
+      </c>
       <c r="X64" s="55" t="s">
         <v>85</v>
       </c>
@@ -11523,8 +11890,12 @@
       <c r="U65" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V65" s="55"/>
-      <c r="W65" s="55"/>
+      <c r="V65" s="67" t="s">
+        <v>787</v>
+      </c>
+      <c r="W65" s="67" t="s">
+        <v>783</v>
+      </c>
       <c r="X65" s="55" t="s">
         <v>85</v>
       </c>
@@ -11637,8 +12008,12 @@
       <c r="U66" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V66" s="55"/>
-      <c r="W66" s="55"/>
+      <c r="V66" s="67" t="s">
+        <v>796</v>
+      </c>
+      <c r="W66" s="67" t="s">
+        <v>791</v>
+      </c>
       <c r="X66" s="55" t="s">
         <v>85</v>
       </c>
@@ -11743,8 +12118,12 @@
       </c>
       <c r="T67" s="55"/>
       <c r="U67" s="55"/>
-      <c r="V67" s="55"/>
-      <c r="W67" s="55"/>
+      <c r="V67" s="67" t="s">
+        <v>897</v>
+      </c>
+      <c r="W67" s="67" t="s">
+        <v>800</v>
+      </c>
       <c r="X67" s="55"/>
       <c r="Y67" s="55"/>
       <c r="Z67" s="55" t="s">
@@ -11833,8 +12212,12 @@
       <c r="U68" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V68" s="55"/>
-      <c r="W68" s="55"/>
+      <c r="V68" s="67" t="s">
+        <v>898</v>
+      </c>
+      <c r="W68" s="67" t="s">
+        <v>806</v>
+      </c>
       <c r="X68" s="55" t="s">
         <v>85</v>
       </c>
@@ -11943,8 +12326,12 @@
       <c r="U69" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V69" s="55"/>
-      <c r="W69" s="55"/>
+      <c r="V69" s="67" t="s">
+        <v>819</v>
+      </c>
+      <c r="W69" s="67" t="s">
+        <v>814</v>
+      </c>
       <c r="X69" s="55" t="s">
         <v>85</v>
       </c>
@@ -12073,8 +12460,12 @@
       <c r="U70" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V70" s="55"/>
-      <c r="W70" s="55"/>
+      <c r="V70" s="67" t="s">
+        <v>899</v>
+      </c>
+      <c r="W70" s="67" t="s">
+        <v>836</v>
+      </c>
       <c r="X70" s="55" t="s">
         <v>840</v>
       </c>
@@ -12181,8 +12572,12 @@
       <c r="U71" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V71" s="55"/>
-      <c r="W71" s="55"/>
+      <c r="V71" s="67" t="s">
+        <v>900</v>
+      </c>
+      <c r="W71" s="67" t="s">
+        <v>848</v>
+      </c>
       <c r="X71" s="55" t="s">
         <v>85</v>
       </c>
@@ -12265,8 +12660,8 @@
       <c r="S72" s="55"/>
       <c r="T72" s="55"/>
       <c r="U72" s="55"/>
-      <c r="V72" s="55"/>
-      <c r="W72" s="55"/>
+      <c r="V72" s="67"/>
+      <c r="W72" s="67"/>
       <c r="X72" s="55"/>
       <c r="Y72" s="55"/>
       <c r="Z72" s="55" t="s">
@@ -12351,8 +12746,12 @@
       <c r="S73" s="55"/>
       <c r="T73" s="55"/>
       <c r="U73" s="55"/>
-      <c r="V73" s="55"/>
-      <c r="W73" s="55"/>
+      <c r="V73" s="67" t="s">
+        <v>861</v>
+      </c>
+      <c r="W73" s="67" t="s">
+        <v>856</v>
+      </c>
       <c r="X73" s="55"/>
       <c r="Y73" s="55"/>
       <c r="Z73" s="55"/>
@@ -12429,8 +12828,8 @@
       <c r="S74" s="55"/>
       <c r="T74" s="55"/>
       <c r="U74" s="55"/>
-      <c r="V74" s="55"/>
-      <c r="W74" s="55"/>
+      <c r="V74" s="67"/>
+      <c r="W74" s="67"/>
       <c r="X74" s="55"/>
       <c r="Y74" s="55"/>
       <c r="Z74" s="55" t="s">

</xml_diff>

<commit_message>
Test: delete all induction dates
For testing purposes, I deleted the induction dates to see if my extra implementation for handling induction dates is going to work.
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96859764-448E-C641-9870-036797EEC7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{663ACADE-BA21-5742-95A3-687CC530524D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3153,10 +3153,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3168,6 +3164,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3607,21 +3607,21 @@
       <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
@@ -4708,10 +4708,10 @@
   <dimension ref="A1:AZ1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL17" sqref="AL17"/>
+      <selection pane="bottomRight" activeCell="AU11" sqref="AU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4989,7 +4989,7 @@
       <c r="V2" s="39" t="s">
         <v>864</v>
       </c>
-      <c r="W2" s="63" t="s">
+      <c r="W2" s="61" t="s">
         <v>77</v>
       </c>
       <c r="X2" s="23" t="s">
@@ -5054,9 +5054,7 @@
       </c>
       <c r="AT2" s="23"/>
       <c r="AU2" s="23"/>
-      <c r="AV2" s="23">
-        <v>2022</v>
-      </c>
+      <c r="AV2" s="23"/>
       <c r="AW2" s="23"/>
       <c r="AX2" s="24" t="s">
         <v>99</v>
@@ -5124,10 +5122,10 @@
       <c r="U3" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V3" s="63" t="s">
+      <c r="V3" s="61" t="s">
         <v>107</v>
       </c>
-      <c r="W3" s="63" t="s">
+      <c r="W3" s="61" t="s">
         <v>108</v>
       </c>
       <c r="X3" s="23" t="s">
@@ -5178,9 +5176,7 @@
         <v>114</v>
       </c>
       <c r="AU3" s="23"/>
-      <c r="AV3" s="23">
-        <v>2021</v>
-      </c>
+      <c r="AV3" s="23"/>
       <c r="AW3" s="23" t="s">
         <v>115</v>
       </c>
@@ -5248,10 +5244,10 @@
       <c r="U4" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V4" s="64" t="s">
+      <c r="V4" s="62" t="s">
         <v>865</v>
       </c>
-      <c r="W4" s="64" t="s">
+      <c r="W4" s="62" t="s">
         <v>900</v>
       </c>
       <c r="X4" s="23" t="s">
@@ -5276,24 +5272,24 @@
       <c r="AG4" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="AH4" s="64" t="s">
+      <c r="AH4" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="AI4" s="64" t="s">
+      <c r="AI4" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="AJ4" s="64" t="s">
+      <c r="AJ4" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="AK4" s="64" t="s">
+      <c r="AK4" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="AL4" s="63"/>
-      <c r="AM4" s="63"/>
-      <c r="AN4" s="63"/>
-      <c r="AO4" s="63"/>
-      <c r="AP4" s="63"/>
-      <c r="AQ4" s="63"/>
+      <c r="AL4" s="61"/>
+      <c r="AM4" s="61"/>
+      <c r="AN4" s="61"/>
+      <c r="AO4" s="61"/>
+      <c r="AP4" s="61"/>
+      <c r="AQ4" s="61"/>
       <c r="AR4" s="23"/>
       <c r="AS4" s="23"/>
       <c r="AT4" s="23"/>
@@ -5366,10 +5362,10 @@
       </c>
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
-      <c r="V5" s="63" t="s">
+      <c r="V5" s="61" t="s">
         <v>866</v>
       </c>
-      <c r="W5" s="63" t="s">
+      <c r="W5" s="61" t="s">
         <v>133</v>
       </c>
       <c r="X5" s="23"/>
@@ -5412,9 +5408,7 @@
       <c r="AS5" s="23"/>
       <c r="AT5" s="23"/>
       <c r="AU5" s="23"/>
-      <c r="AV5" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV5" s="23"/>
       <c r="AW5" s="23"/>
       <c r="AX5" s="24" t="s">
         <v>99</v>
@@ -5478,10 +5472,10 @@
       <c r="U6" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V6" s="63" t="s">
+      <c r="V6" s="61" t="s">
         <v>867</v>
       </c>
-      <c r="W6" s="63" t="s">
+      <c r="W6" s="61" t="s">
         <v>145</v>
       </c>
       <c r="X6" s="23"/>
@@ -5508,24 +5502,24 @@
       <c r="AG6" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="AH6" s="63" t="s">
+      <c r="AH6" s="61" t="s">
         <v>154</v>
       </c>
-      <c r="AI6" s="63" t="s">
+      <c r="AI6" s="61" t="s">
         <v>155</v>
       </c>
-      <c r="AJ6" s="63" t="s">
+      <c r="AJ6" s="61" t="s">
         <v>156</v>
       </c>
-      <c r="AK6" s="63" t="s">
+      <c r="AK6" s="61" t="s">
         <v>157</v>
       </c>
       <c r="AL6" s="26"/>
       <c r="AM6" s="26"/>
-      <c r="AN6" s="63"/>
-      <c r="AO6" s="63"/>
-      <c r="AP6" s="63"/>
-      <c r="AQ6" s="63" t="s">
+      <c r="AN6" s="61"/>
+      <c r="AO6" s="61"/>
+      <c r="AP6" s="61"/>
+      <c r="AQ6" s="61" t="s">
         <v>158</v>
       </c>
       <c r="AR6" s="23">
@@ -5606,10 +5600,10 @@
       <c r="U7" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="V7" s="63" t="s">
+      <c r="V7" s="61" t="s">
         <v>868</v>
       </c>
-      <c r="W7" s="63" t="s">
+      <c r="W7" s="61" t="s">
         <v>901</v>
       </c>
       <c r="X7" s="23" t="s">
@@ -5640,16 +5634,16 @@
       <c r="AG7" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="AH7" s="63" t="s">
+      <c r="AH7" s="61" t="s">
         <v>172</v>
       </c>
-      <c r="AI7" s="63" t="s">
+      <c r="AI7" s="61" t="s">
         <v>173</v>
       </c>
-      <c r="AJ7" s="63" t="s">
+      <c r="AJ7" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="AK7" s="63" t="s">
+      <c r="AK7" s="61" t="s">
         <v>175</v>
       </c>
       <c r="AL7" s="30" t="s">
@@ -5658,10 +5652,10 @@
       <c r="AM7" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="AN7" s="63" t="s">
+      <c r="AN7" s="61" t="s">
         <v>178</v>
       </c>
-      <c r="AO7" s="63" t="s">
+      <c r="AO7" s="61" t="s">
         <v>179</v>
       </c>
       <c r="AP7" s="26"/>
@@ -5674,9 +5668,7 @@
       </c>
       <c r="AT7" s="23"/>
       <c r="AU7" s="23"/>
-      <c r="AV7" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV7" s="23"/>
       <c r="AW7" s="23"/>
       <c r="AX7" s="24" t="s">
         <v>181</v>
@@ -5814,9 +5806,7 @@
       </c>
       <c r="AT8" s="26"/>
       <c r="AU8" s="26"/>
-      <c r="AV8" s="26">
-        <v>2023</v>
-      </c>
+      <c r="AV8" s="26"/>
       <c r="AW8" s="26"/>
       <c r="AX8" s="32"/>
       <c r="AY8" s="26">
@@ -5932,9 +5922,7 @@
       <c r="AU9" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="AV9" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV9" s="23"/>
       <c r="AW9" s="23" t="s">
         <v>212</v>
       </c>
@@ -6068,9 +6056,7 @@
       <c r="AU10" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="AV10" s="23">
-        <v>2021</v>
-      </c>
+      <c r="AV10" s="23"/>
       <c r="AW10" s="23"/>
       <c r="AX10" s="24"/>
       <c r="AY10" s="23">
@@ -6126,10 +6112,10 @@
       <c r="S11" s="23"/>
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
-      <c r="V11" s="63" t="s">
+      <c r="V11" s="61" t="s">
         <v>871</v>
       </c>
-      <c r="W11" s="63" t="s">
+      <c r="W11" s="61" t="s">
         <v>238</v>
       </c>
       <c r="X11" s="23"/>
@@ -6260,10 +6246,10 @@
       <c r="U12" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V12" s="63" t="s">
+      <c r="V12" s="61" t="s">
         <v>262</v>
       </c>
-      <c r="W12" s="63" t="s">
+      <c r="W12" s="61" t="s">
         <v>263</v>
       </c>
       <c r="X12" s="23" t="s">
@@ -6316,9 +6302,7 @@
       <c r="AU12" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="AV12" s="23">
-        <v>2010</v>
-      </c>
+      <c r="AV12" s="23"/>
       <c r="AW12" s="23"/>
       <c r="AX12" s="24" t="s">
         <v>269</v>
@@ -6390,10 +6374,10 @@
       <c r="U13" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V13" s="63" t="s">
+      <c r="V13" s="61" t="s">
         <v>276</v>
       </c>
-      <c r="W13" s="63" t="s">
+      <c r="W13" s="61" t="s">
         <v>277</v>
       </c>
       <c r="X13" s="23" t="s">
@@ -6440,9 +6424,7 @@
       <c r="AS13" s="23"/>
       <c r="AT13" s="23"/>
       <c r="AU13" s="23"/>
-      <c r="AV13" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV13" s="23"/>
       <c r="AW13" s="23"/>
       <c r="AX13" s="24" t="s">
         <v>99</v>
@@ -6516,10 +6498,10 @@
       <c r="U14" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V14" s="63" t="s">
+      <c r="V14" s="61" t="s">
         <v>289</v>
       </c>
-      <c r="W14" s="63" t="s">
+      <c r="W14" s="61" t="s">
         <v>290</v>
       </c>
       <c r="X14" s="23"/>
@@ -6542,34 +6524,34 @@
       <c r="AG14" s="23" t="s">
         <v>282</v>
       </c>
-      <c r="AH14" s="63" t="s">
+      <c r="AH14" s="61" t="s">
         <v>293</v>
       </c>
-      <c r="AI14" s="63" t="s">
+      <c r="AI14" s="61" t="s">
         <v>294</v>
       </c>
-      <c r="AJ14" s="64" t="s">
+      <c r="AJ14" s="62" t="s">
         <v>295</v>
       </c>
-      <c r="AK14" s="63" t="s">
+      <c r="AK14" s="61" t="s">
         <v>283</v>
       </c>
-      <c r="AL14" s="64" t="s">
+      <c r="AL14" s="62" t="s">
         <v>296</v>
       </c>
-      <c r="AM14" s="64" t="s">
+      <c r="AM14" s="62" t="s">
         <v>297</v>
       </c>
-      <c r="AN14" s="64" t="s">
+      <c r="AN14" s="62" t="s">
         <v>298</v>
       </c>
-      <c r="AO14" s="64" t="s">
+      <c r="AO14" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="AP14" s="64" t="s">
+      <c r="AP14" s="62" t="s">
         <v>300</v>
       </c>
-      <c r="AQ14" s="64" t="s">
+      <c r="AQ14" s="62" t="s">
         <v>301</v>
       </c>
       <c r="AR14" s="23"/>
@@ -6578,9 +6560,7 @@
       </c>
       <c r="AT14" s="23"/>
       <c r="AU14" s="23"/>
-      <c r="AV14" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV14" s="23"/>
       <c r="AW14" s="23"/>
       <c r="AX14" s="24" t="s">
         <v>303</v>
@@ -6652,10 +6632,10 @@
       <c r="U15" s="23" t="s">
         <v>314</v>
       </c>
-      <c r="V15" s="64" t="s">
+      <c r="V15" s="62" t="s">
         <v>872</v>
       </c>
-      <c r="W15" s="64" t="s">
+      <c r="W15" s="62" t="s">
         <v>904</v>
       </c>
       <c r="X15" s="23" t="s">
@@ -6688,16 +6668,16 @@
       <c r="AG15" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="AH15" s="64" t="s">
+      <c r="AH15" s="62" t="s">
         <v>321</v>
       </c>
-      <c r="AI15" s="64" t="s">
+      <c r="AI15" s="62" t="s">
         <v>322</v>
       </c>
-      <c r="AJ15" s="64" t="s">
+      <c r="AJ15" s="62" t="s">
         <v>323</v>
       </c>
-      <c r="AK15" s="64" t="s">
+      <c r="AK15" s="62" t="s">
         <v>324</v>
       </c>
       <c r="AL15" s="39" t="s">
@@ -6724,9 +6704,7 @@
         <v>2017</v>
       </c>
       <c r="AU15" s="23"/>
-      <c r="AV15" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV15" s="23"/>
       <c r="AW15" s="23" t="s">
         <v>330</v>
       </c>
@@ -6798,10 +6776,10 @@
       <c r="U16" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V16" s="64" t="s">
+      <c r="V16" s="62" t="s">
         <v>873</v>
       </c>
-      <c r="W16" s="64" t="s">
+      <c r="W16" s="62" t="s">
         <v>333</v>
       </c>
       <c r="X16" s="23" t="s">
@@ -6836,7 +6814,7 @@
       <c r="AI16" s="30" t="s">
         <v>342</v>
       </c>
-      <c r="AJ16" s="63"/>
+      <c r="AJ16" s="61"/>
       <c r="AK16" s="26"/>
       <c r="AL16" s="26"/>
       <c r="AM16" s="26"/>
@@ -6852,9 +6830,7 @@
         <v>343</v>
       </c>
       <c r="AU16" s="23"/>
-      <c r="AV16" s="23">
-        <v>1977</v>
-      </c>
+      <c r="AV16" s="23"/>
       <c r="AW16" s="23"/>
       <c r="AX16" s="24"/>
       <c r="AY16" s="23" t="s">
@@ -6924,10 +6900,10 @@
       <c r="U17" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V17" s="63" t="s">
+      <c r="V17" s="61" t="s">
         <v>351</v>
       </c>
-      <c r="W17" s="63" t="s">
+      <c r="W17" s="61" t="s">
         <v>352</v>
       </c>
       <c r="X17" s="23" t="s">
@@ -6956,43 +6932,41 @@
       <c r="AG17" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="AH17" s="64" t="s">
+      <c r="AH17" s="62" t="s">
         <v>356</v>
       </c>
-      <c r="AI17" s="64" t="s">
+      <c r="AI17" s="62" t="s">
         <v>357</v>
       </c>
-      <c r="AJ17" s="63" t="s">
+      <c r="AJ17" s="61" t="s">
         <v>358</v>
       </c>
-      <c r="AK17" s="64" t="s">
+      <c r="AK17" s="62" t="s">
         <v>359</v>
       </c>
-      <c r="AL17" s="64" t="s">
+      <c r="AL17" s="62" t="s">
         <v>360</v>
       </c>
-      <c r="AM17" s="64" t="s">
+      <c r="AM17" s="62" t="s">
         <v>361</v>
       </c>
-      <c r="AN17" s="64" t="s">
+      <c r="AN17" s="62" t="s">
         <v>362</v>
       </c>
-      <c r="AO17" s="64" t="s">
+      <c r="AO17" s="62" t="s">
         <v>363</v>
       </c>
-      <c r="AP17" s="64" t="s">
+      <c r="AP17" s="62" t="s">
         <v>364</v>
       </c>
-      <c r="AQ17" s="64" t="s">
+      <c r="AQ17" s="62" t="s">
         <v>365</v>
       </c>
       <c r="AR17" s="23"/>
       <c r="AS17" s="23"/>
       <c r="AT17" s="23"/>
       <c r="AU17" s="23"/>
-      <c r="AV17" s="23">
-        <v>2018</v>
-      </c>
+      <c r="AV17" s="23"/>
       <c r="AW17" s="23"/>
       <c r="AX17" s="24"/>
       <c r="AY17" s="23">
@@ -7062,10 +7036,10 @@
       <c r="U18" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V18" s="63" t="s">
+      <c r="V18" s="61" t="s">
         <v>874</v>
       </c>
-      <c r="W18" s="63" t="s">
+      <c r="W18" s="61" t="s">
         <v>367</v>
       </c>
       <c r="X18" s="23" t="s">
@@ -7094,25 +7068,23 @@
       <c r="AG18" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="AH18" s="63"/>
-      <c r="AI18" s="63"/>
-      <c r="AJ18" s="63"/>
-      <c r="AK18" s="63"/>
-      <c r="AL18" s="63"/>
-      <c r="AM18" s="63"/>
-      <c r="AN18" s="63"/>
-      <c r="AO18" s="63"/>
-      <c r="AP18" s="63"/>
-      <c r="AQ18" s="63"/>
+      <c r="AH18" s="61"/>
+      <c r="AI18" s="61"/>
+      <c r="AJ18" s="61"/>
+      <c r="AK18" s="61"/>
+      <c r="AL18" s="61"/>
+      <c r="AM18" s="61"/>
+      <c r="AN18" s="61"/>
+      <c r="AO18" s="61"/>
+      <c r="AP18" s="61"/>
+      <c r="AQ18" s="61"/>
       <c r="AR18" s="23">
         <v>2012</v>
       </c>
       <c r="AS18" s="23"/>
       <c r="AT18" s="23"/>
       <c r="AU18" s="23"/>
-      <c r="AV18" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV18" s="23"/>
       <c r="AW18" s="23"/>
       <c r="AX18" s="24" t="s">
         <v>377</v>
@@ -7184,10 +7156,10 @@
       <c r="U19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="V19" s="63" t="s">
+      <c r="V19" s="61" t="s">
         <v>384</v>
       </c>
-      <c r="W19" s="63" t="s">
+      <c r="W19" s="61" t="s">
         <v>385</v>
       </c>
       <c r="X19" s="23" t="s">
@@ -7216,16 +7188,16 @@
       <c r="AG19" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="AH19" s="64" t="s">
+      <c r="AH19" s="62" t="s">
         <v>390</v>
       </c>
-      <c r="AI19" s="64" t="s">
+      <c r="AI19" s="62" t="s">
         <v>391</v>
       </c>
       <c r="AJ19" s="30" t="s">
         <v>392</v>
       </c>
-      <c r="AK19" s="64" t="s">
+      <c r="AK19" s="62" t="s">
         <v>393</v>
       </c>
       <c r="AL19" s="30" t="s">
@@ -7250,9 +7222,7 @@
       <c r="AS19" s="23"/>
       <c r="AT19" s="23"/>
       <c r="AU19" s="23"/>
-      <c r="AV19" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV19" s="23"/>
       <c r="AW19" s="23"/>
       <c r="AX19" s="24" t="s">
         <v>400</v>
@@ -7360,10 +7330,10 @@
       <c r="AK20" s="32" t="s">
         <v>415</v>
       </c>
-      <c r="AL20" s="64" t="s">
+      <c r="AL20" s="62" t="s">
         <v>416</v>
       </c>
-      <c r="AM20" s="64" t="s">
+      <c r="AM20" s="62" t="s">
         <v>417</v>
       </c>
       <c r="AN20" s="39" t="s">
@@ -7372,10 +7342,10 @@
       <c r="AO20" s="39" t="s">
         <v>419</v>
       </c>
-      <c r="AP20" s="64" t="s">
+      <c r="AP20" s="62" t="s">
         <v>420</v>
       </c>
-      <c r="AQ20" s="64" t="s">
+      <c r="AQ20" s="62" t="s">
         <v>421</v>
       </c>
       <c r="AR20" s="23">
@@ -7386,9 +7356,7 @@
         <v>2014</v>
       </c>
       <c r="AU20" s="23"/>
-      <c r="AV20" s="23">
-        <v>2023</v>
-      </c>
+      <c r="AV20" s="23"/>
       <c r="AW20" s="23"/>
       <c r="AX20" s="24" t="s">
         <v>99</v>
@@ -7454,10 +7422,10 @@
       </c>
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
-      <c r="V21" s="64" t="s">
+      <c r="V21" s="62" t="s">
         <v>876</v>
       </c>
-      <c r="W21" s="64" t="s">
+      <c r="W21" s="62" t="s">
         <v>906</v>
       </c>
       <c r="X21" s="24"/>
@@ -7514,9 +7482,7 @@
       <c r="AS21" s="24"/>
       <c r="AT21" s="24"/>
       <c r="AU21" s="24"/>
-      <c r="AV21" s="24">
-        <v>2023</v>
-      </c>
+      <c r="AV21" s="24"/>
       <c r="AW21" s="24" t="s">
         <v>115</v>
       </c>
@@ -7574,10 +7540,10 @@
       <c r="S22" s="45"/>
       <c r="T22" s="45"/>
       <c r="U22" s="45"/>
-      <c r="V22" s="65" t="s">
+      <c r="V22" s="63" t="s">
         <v>877</v>
       </c>
-      <c r="W22" s="65" t="s">
+      <c r="W22" s="63" t="s">
         <v>443</v>
       </c>
       <c r="X22" s="45"/>
@@ -7600,16 +7566,16 @@
       <c r="AG22" s="45" t="s">
         <v>442</v>
       </c>
-      <c r="AH22" s="65"/>
-      <c r="AI22" s="65"/>
-      <c r="AJ22" s="65"/>
-      <c r="AK22" s="65"/>
-      <c r="AL22" s="65"/>
-      <c r="AM22" s="65"/>
-      <c r="AN22" s="65"/>
-      <c r="AO22" s="65"/>
-      <c r="AP22" s="65"/>
-      <c r="AQ22" s="65"/>
+      <c r="AH22" s="63"/>
+      <c r="AI22" s="63"/>
+      <c r="AJ22" s="63"/>
+      <c r="AK22" s="63"/>
+      <c r="AL22" s="63"/>
+      <c r="AM22" s="63"/>
+      <c r="AN22" s="63"/>
+      <c r="AO22" s="63"/>
+      <c r="AP22" s="63"/>
+      <c r="AQ22" s="63"/>
       <c r="AR22" s="45"/>
       <c r="AS22" s="45">
         <v>2014</v>
@@ -7684,10 +7650,10 @@
       <c r="U23" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V23" s="66" t="s">
+      <c r="V23" s="64" t="s">
         <v>878</v>
       </c>
-      <c r="W23" s="66" t="s">
+      <c r="W23" s="64" t="s">
         <v>452</v>
       </c>
       <c r="X23" s="50"/>
@@ -7714,34 +7680,34 @@
       <c r="AG23" s="50" t="s">
         <v>451</v>
       </c>
-      <c r="AH23" s="66" t="s">
+      <c r="AH23" s="64" t="s">
         <v>461</v>
       </c>
-      <c r="AI23" s="66" t="s">
+      <c r="AI23" s="64" t="s">
         <v>462</v>
       </c>
-      <c r="AJ23" s="66" t="s">
+      <c r="AJ23" s="64" t="s">
         <v>463</v>
       </c>
-      <c r="AK23" s="66" t="s">
+      <c r="AK23" s="64" t="s">
         <v>464</v>
       </c>
-      <c r="AL23" s="66" t="s">
+      <c r="AL23" s="64" t="s">
         <v>465</v>
       </c>
-      <c r="AM23" s="66" t="s">
+      <c r="AM23" s="64" t="s">
         <v>466</v>
       </c>
-      <c r="AN23" s="66" t="s">
+      <c r="AN23" s="64" t="s">
         <v>467</v>
       </c>
-      <c r="AO23" s="66" t="s">
+      <c r="AO23" s="64" t="s">
         <v>468</v>
       </c>
-      <c r="AP23" s="66" t="s">
+      <c r="AP23" s="64" t="s">
         <v>469</v>
       </c>
-      <c r="AQ23" s="66" t="s">
+      <c r="AQ23" s="64" t="s">
         <v>470</v>
       </c>
       <c r="AR23" s="50" t="s">
@@ -7750,9 +7716,7 @@
       <c r="AS23" s="50"/>
       <c r="AT23" s="50"/>
       <c r="AU23" s="50"/>
-      <c r="AV23" s="50">
-        <v>1987</v>
-      </c>
+      <c r="AV23" s="50"/>
       <c r="AW23" s="50"/>
       <c r="AX23" s="45" t="s">
         <v>472</v>
@@ -7812,10 +7776,10 @@
       <c r="U24" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V24" s="66" t="s">
+      <c r="V24" s="64" t="s">
         <v>879</v>
       </c>
-      <c r="W24" s="66" t="s">
+      <c r="W24" s="64" t="s">
         <v>907</v>
       </c>
       <c r="X24" s="50"/>
@@ -7840,32 +7804,32 @@
       <c r="AG24" s="50" t="s">
         <v>481</v>
       </c>
-      <c r="AH24" s="66" t="s">
+      <c r="AH24" s="64" t="s">
         <v>482</v>
       </c>
-      <c r="AI24" s="66" t="s">
+      <c r="AI24" s="64" t="s">
         <v>483</v>
       </c>
-      <c r="AJ24" s="66" t="s">
+      <c r="AJ24" s="64" t="s">
         <v>484</v>
       </c>
-      <c r="AK24" s="66" t="s">
+      <c r="AK24" s="64" t="s">
         <v>485</v>
       </c>
-      <c r="AL24" s="66" t="s">
+      <c r="AL24" s="64" t="s">
         <v>486</v>
       </c>
-      <c r="AM24" s="66" t="s">
+      <c r="AM24" s="64" t="s">
         <v>487</v>
       </c>
-      <c r="AN24" s="66" t="s">
+      <c r="AN24" s="64" t="s">
         <v>488</v>
       </c>
-      <c r="AO24" s="66" t="s">
+      <c r="AO24" s="64" t="s">
         <v>489</v>
       </c>
-      <c r="AP24" s="66"/>
-      <c r="AQ24" s="66"/>
+      <c r="AP24" s="64"/>
+      <c r="AQ24" s="64"/>
       <c r="AR24" s="50">
         <v>2019</v>
       </c>
@@ -7942,10 +7906,10 @@
       <c r="U25" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V25" s="66" t="s">
+      <c r="V25" s="64" t="s">
         <v>880</v>
       </c>
-      <c r="W25" s="66" t="s">
+      <c r="W25" s="64" t="s">
         <v>498</v>
       </c>
       <c r="X25" s="50"/>
@@ -7970,32 +7934,32 @@
       <c r="AG25" s="50" t="s">
         <v>491</v>
       </c>
-      <c r="AH25" s="66" t="s">
+      <c r="AH25" s="64" t="s">
         <v>502</v>
       </c>
-      <c r="AI25" s="66" t="s">
+      <c r="AI25" s="64" t="s">
         <v>503</v>
       </c>
-      <c r="AJ25" s="66" t="s">
+      <c r="AJ25" s="64" t="s">
         <v>504</v>
       </c>
-      <c r="AK25" s="66" t="s">
+      <c r="AK25" s="64" t="s">
         <v>505</v>
       </c>
-      <c r="AL25" s="66" t="s">
+      <c r="AL25" s="64" t="s">
         <v>506</v>
       </c>
-      <c r="AM25" s="66" t="s">
+      <c r="AM25" s="64" t="s">
         <v>507</v>
       </c>
-      <c r="AN25" s="66" t="s">
+      <c r="AN25" s="64" t="s">
         <v>508</v>
       </c>
-      <c r="AO25" s="66" t="s">
+      <c r="AO25" s="64" t="s">
         <v>509</v>
       </c>
-      <c r="AP25" s="66"/>
-      <c r="AQ25" s="66"/>
+      <c r="AP25" s="64"/>
+      <c r="AQ25" s="64"/>
       <c r="AR25" s="50">
         <v>2019</v>
       </c>
@@ -8004,9 +7968,7 @@
       </c>
       <c r="AT25" s="50"/>
       <c r="AU25" s="50"/>
-      <c r="AV25" s="50">
-        <v>2018</v>
-      </c>
+      <c r="AV25" s="50"/>
       <c r="AW25" s="50"/>
       <c r="AX25" s="45"/>
       <c r="AY25" s="50" t="s">
@@ -8076,10 +8038,10 @@
       <c r="U26" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="V26" s="66" t="s">
+      <c r="V26" s="64" t="s">
         <v>881</v>
       </c>
-      <c r="W26" s="66" t="s">
+      <c r="W26" s="64" t="s">
         <v>517</v>
       </c>
       <c r="X26" s="50" t="s">
@@ -8106,31 +8068,29 @@
       <c r="AG26" s="50" t="s">
         <v>511</v>
       </c>
-      <c r="AH26" s="66" t="s">
+      <c r="AH26" s="64" t="s">
         <v>520</v>
       </c>
-      <c r="AI26" s="66" t="s">
+      <c r="AI26" s="64" t="s">
         <v>512</v>
       </c>
-      <c r="AJ26" s="66" t="s">
+      <c r="AJ26" s="64" t="s">
         <v>521</v>
       </c>
-      <c r="AK26" s="66" t="s">
+      <c r="AK26" s="64" t="s">
         <v>522</v>
       </c>
-      <c r="AL26" s="66"/>
-      <c r="AM26" s="66"/>
-      <c r="AN26" s="66"/>
-      <c r="AO26" s="66"/>
-      <c r="AP26" s="66"/>
-      <c r="AQ26" s="66"/>
+      <c r="AL26" s="64"/>
+      <c r="AM26" s="64"/>
+      <c r="AN26" s="64"/>
+      <c r="AO26" s="64"/>
+      <c r="AP26" s="64"/>
+      <c r="AQ26" s="64"/>
       <c r="AR26" s="50"/>
       <c r="AS26" s="50"/>
       <c r="AT26" s="50"/>
       <c r="AU26" s="50"/>
-      <c r="AV26" s="50">
-        <v>2023</v>
-      </c>
+      <c r="AV26" s="50"/>
       <c r="AW26" s="50"/>
       <c r="AX26" s="45" t="s">
         <v>99</v>
@@ -8200,10 +8160,10 @@
       <c r="U27" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="V27" s="65" t="s">
+      <c r="V27" s="63" t="s">
         <v>882</v>
       </c>
-      <c r="W27" s="65" t="s">
+      <c r="W27" s="63" t="s">
         <v>524</v>
       </c>
       <c r="X27" s="45" t="s">
@@ -8234,25 +8194,23 @@
       <c r="AG27" s="45" t="s">
         <v>523</v>
       </c>
-      <c r="AH27" s="65"/>
-      <c r="AI27" s="65"/>
-      <c r="AJ27" s="65"/>
-      <c r="AK27" s="65"/>
-      <c r="AL27" s="65"/>
-      <c r="AM27" s="65"/>
-      <c r="AN27" s="65"/>
-      <c r="AO27" s="65"/>
-      <c r="AP27" s="65"/>
-      <c r="AQ27" s="65"/>
+      <c r="AH27" s="63"/>
+      <c r="AI27" s="63"/>
+      <c r="AJ27" s="63"/>
+      <c r="AK27" s="63"/>
+      <c r="AL27" s="63"/>
+      <c r="AM27" s="63"/>
+      <c r="AN27" s="63"/>
+      <c r="AO27" s="63"/>
+      <c r="AP27" s="63"/>
+      <c r="AQ27" s="63"/>
       <c r="AR27" s="45" t="s">
         <v>471</v>
       </c>
       <c r="AS27" s="45"/>
       <c r="AT27" s="45"/>
       <c r="AU27" s="45"/>
-      <c r="AV27" s="45">
-        <v>2023</v>
-      </c>
+      <c r="AV27" s="45"/>
       <c r="AW27" s="45"/>
       <c r="AX27" s="45" t="s">
         <v>99</v>
@@ -8480,9 +8438,7 @@
       <c r="AS29" s="51"/>
       <c r="AT29" s="51"/>
       <c r="AU29" s="51"/>
-      <c r="AV29" s="51">
-        <v>2021</v>
-      </c>
+      <c r="AV29" s="51"/>
       <c r="AW29" s="51"/>
       <c r="AX29" s="48" t="s">
         <v>99</v>
@@ -8526,8 +8482,8 @@
       <c r="S30" s="55"/>
       <c r="T30" s="55"/>
       <c r="U30" s="55"/>
-      <c r="V30" s="67"/>
-      <c r="W30" s="67"/>
+      <c r="V30" s="65"/>
+      <c r="W30" s="65"/>
       <c r="X30" s="55"/>
       <c r="Y30" s="55"/>
       <c r="Z30" s="55" t="s">
@@ -8542,16 +8498,16 @@
       <c r="AG30" s="55" t="s">
         <v>565</v>
       </c>
-      <c r="AH30" s="67"/>
-      <c r="AI30" s="67"/>
-      <c r="AJ30" s="67"/>
-      <c r="AK30" s="67"/>
-      <c r="AL30" s="67"/>
-      <c r="AM30" s="67"/>
-      <c r="AN30" s="67"/>
-      <c r="AO30" s="67"/>
-      <c r="AP30" s="67"/>
-      <c r="AQ30" s="67"/>
+      <c r="AH30" s="65"/>
+      <c r="AI30" s="65"/>
+      <c r="AJ30" s="65"/>
+      <c r="AK30" s="65"/>
+      <c r="AL30" s="65"/>
+      <c r="AM30" s="65"/>
+      <c r="AN30" s="65"/>
+      <c r="AO30" s="65"/>
+      <c r="AP30" s="65"/>
+      <c r="AQ30" s="65"/>
       <c r="AR30" s="55"/>
       <c r="AS30" s="55"/>
       <c r="AT30" s="55"/>
@@ -8600,8 +8556,8 @@
       <c r="S31" s="55"/>
       <c r="T31" s="55"/>
       <c r="U31" s="55"/>
-      <c r="V31" s="67"/>
-      <c r="W31" s="67"/>
+      <c r="V31" s="65"/>
+      <c r="W31" s="65"/>
       <c r="X31" s="55"/>
       <c r="Y31" s="55"/>
       <c r="Z31" s="55" t="s">
@@ -8616,16 +8572,16 @@
       <c r="AG31" s="55" t="s">
         <v>566</v>
       </c>
-      <c r="AH31" s="67"/>
-      <c r="AI31" s="67"/>
-      <c r="AJ31" s="67"/>
-      <c r="AK31" s="67"/>
-      <c r="AL31" s="67"/>
-      <c r="AM31" s="67"/>
-      <c r="AN31" s="67"/>
-      <c r="AO31" s="67"/>
-      <c r="AP31" s="67"/>
-      <c r="AQ31" s="67"/>
+      <c r="AH31" s="65"/>
+      <c r="AI31" s="65"/>
+      <c r="AJ31" s="65"/>
+      <c r="AK31" s="65"/>
+      <c r="AL31" s="65"/>
+      <c r="AM31" s="65"/>
+      <c r="AN31" s="65"/>
+      <c r="AO31" s="65"/>
+      <c r="AP31" s="65"/>
+      <c r="AQ31" s="65"/>
       <c r="AR31" s="55"/>
       <c r="AS31" s="55"/>
       <c r="AT31" s="55"/>
@@ -8688,10 +8644,10 @@
       <c r="S32" s="55"/>
       <c r="T32" s="55"/>
       <c r="U32" s="55"/>
-      <c r="V32" s="67" t="s">
+      <c r="V32" s="65" t="s">
         <v>884</v>
       </c>
-      <c r="W32" s="67" t="s">
+      <c r="W32" s="65" t="s">
         <v>568</v>
       </c>
       <c r="X32" s="55"/>
@@ -8714,16 +8670,16 @@
       <c r="AG32" s="55" t="s">
         <v>567</v>
       </c>
-      <c r="AH32" s="67"/>
-      <c r="AI32" s="67"/>
-      <c r="AJ32" s="67"/>
-      <c r="AK32" s="67"/>
-      <c r="AL32" s="67"/>
-      <c r="AM32" s="67"/>
-      <c r="AN32" s="67"/>
-      <c r="AO32" s="67"/>
-      <c r="AP32" s="67"/>
-      <c r="AQ32" s="67"/>
+      <c r="AH32" s="65"/>
+      <c r="AI32" s="65"/>
+      <c r="AJ32" s="65"/>
+      <c r="AK32" s="65"/>
+      <c r="AL32" s="65"/>
+      <c r="AM32" s="65"/>
+      <c r="AN32" s="65"/>
+      <c r="AO32" s="65"/>
+      <c r="AP32" s="65"/>
+      <c r="AQ32" s="65"/>
       <c r="AR32" s="55"/>
       <c r="AS32" s="55"/>
       <c r="AT32" s="55"/>
@@ -8770,8 +8726,8 @@
       <c r="S33" s="55"/>
       <c r="T33" s="55"/>
       <c r="U33" s="55"/>
-      <c r="V33" s="67"/>
-      <c r="W33" s="67"/>
+      <c r="V33" s="65"/>
+      <c r="W33" s="65"/>
       <c r="X33" s="55"/>
       <c r="Y33" s="55"/>
       <c r="Z33" s="55" t="s">
@@ -8786,16 +8742,16 @@
       <c r="AG33" s="55" t="s">
         <v>576</v>
       </c>
-      <c r="AH33" s="67"/>
-      <c r="AI33" s="67"/>
-      <c r="AJ33" s="67"/>
-      <c r="AK33" s="67"/>
-      <c r="AL33" s="67"/>
-      <c r="AM33" s="67"/>
-      <c r="AN33" s="67"/>
-      <c r="AO33" s="67"/>
-      <c r="AP33" s="67"/>
-      <c r="AQ33" s="67"/>
+      <c r="AH33" s="65"/>
+      <c r="AI33" s="65"/>
+      <c r="AJ33" s="65"/>
+      <c r="AK33" s="65"/>
+      <c r="AL33" s="65"/>
+      <c r="AM33" s="65"/>
+      <c r="AN33" s="65"/>
+      <c r="AO33" s="65"/>
+      <c r="AP33" s="65"/>
+      <c r="AQ33" s="65"/>
       <c r="AR33" s="55"/>
       <c r="AS33" s="55"/>
       <c r="AT33" s="55"/>
@@ -8844,8 +8800,8 @@
       <c r="S34" s="55"/>
       <c r="T34" s="55"/>
       <c r="U34" s="55"/>
-      <c r="V34" s="67"/>
-      <c r="W34" s="67"/>
+      <c r="V34" s="65"/>
+      <c r="W34" s="65"/>
       <c r="X34" s="55"/>
       <c r="Y34" s="55"/>
       <c r="Z34" s="55" t="s">
@@ -8860,16 +8816,16 @@
       <c r="AG34" s="55" t="s">
         <v>577</v>
       </c>
-      <c r="AH34" s="67"/>
-      <c r="AI34" s="67"/>
-      <c r="AJ34" s="67"/>
-      <c r="AK34" s="67"/>
-      <c r="AL34" s="67"/>
-      <c r="AM34" s="67"/>
-      <c r="AN34" s="67"/>
-      <c r="AO34" s="67"/>
-      <c r="AP34" s="67"/>
-      <c r="AQ34" s="67"/>
+      <c r="AH34" s="65"/>
+      <c r="AI34" s="65"/>
+      <c r="AJ34" s="65"/>
+      <c r="AK34" s="65"/>
+      <c r="AL34" s="65"/>
+      <c r="AM34" s="65"/>
+      <c r="AN34" s="65"/>
+      <c r="AO34" s="65"/>
+      <c r="AP34" s="65"/>
+      <c r="AQ34" s="65"/>
       <c r="AR34" s="55"/>
       <c r="AS34" s="55"/>
       <c r="AT34" s="55"/>
@@ -8934,10 +8890,10 @@
       <c r="S35" s="55"/>
       <c r="T35" s="55"/>
       <c r="U35" s="55"/>
-      <c r="V35" s="67" t="s">
+      <c r="V35" s="65" t="s">
         <v>885</v>
       </c>
-      <c r="W35" s="67" t="s">
+      <c r="W35" s="65" t="s">
         <v>580</v>
       </c>
       <c r="X35" s="55"/>
@@ -8960,16 +8916,16 @@
       <c r="AG35" s="55" t="s">
         <v>579</v>
       </c>
-      <c r="AH35" s="67"/>
-      <c r="AI35" s="67"/>
-      <c r="AJ35" s="67"/>
-      <c r="AK35" s="67"/>
-      <c r="AL35" s="67"/>
-      <c r="AM35" s="67"/>
-      <c r="AN35" s="67"/>
-      <c r="AO35" s="67"/>
-      <c r="AP35" s="67"/>
-      <c r="AQ35" s="67"/>
+      <c r="AH35" s="65"/>
+      <c r="AI35" s="65"/>
+      <c r="AJ35" s="65"/>
+      <c r="AK35" s="65"/>
+      <c r="AL35" s="65"/>
+      <c r="AM35" s="65"/>
+      <c r="AN35" s="65"/>
+      <c r="AO35" s="65"/>
+      <c r="AP35" s="65"/>
+      <c r="AQ35" s="65"/>
       <c r="AR35" s="55" t="s">
         <v>439</v>
       </c>
@@ -9042,10 +8998,10 @@
       <c r="U36" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V36" s="67" t="s">
+      <c r="V36" s="65" t="s">
         <v>886</v>
       </c>
-      <c r="W36" s="67" t="s">
+      <c r="W36" s="65" t="s">
         <v>908</v>
       </c>
       <c r="X36" s="55" t="s">
@@ -9072,16 +9028,16 @@
       <c r="AG36" s="55" t="s">
         <v>590</v>
       </c>
-      <c r="AH36" s="67"/>
-      <c r="AI36" s="67"/>
-      <c r="AJ36" s="67"/>
-      <c r="AK36" s="67"/>
-      <c r="AL36" s="67"/>
-      <c r="AM36" s="67"/>
-      <c r="AN36" s="67"/>
-      <c r="AO36" s="67"/>
-      <c r="AP36" s="67"/>
-      <c r="AQ36" s="67"/>
+      <c r="AH36" s="65"/>
+      <c r="AI36" s="65"/>
+      <c r="AJ36" s="65"/>
+      <c r="AK36" s="65"/>
+      <c r="AL36" s="65"/>
+      <c r="AM36" s="65"/>
+      <c r="AN36" s="65"/>
+      <c r="AO36" s="65"/>
+      <c r="AP36" s="65"/>
+      <c r="AQ36" s="65"/>
       <c r="AR36" s="55"/>
       <c r="AS36" s="55"/>
       <c r="AT36" s="55"/>
@@ -9128,8 +9084,8 @@
       <c r="S37" s="55"/>
       <c r="T37" s="55"/>
       <c r="U37" s="55"/>
-      <c r="V37" s="67"/>
-      <c r="W37" s="67"/>
+      <c r="V37" s="65"/>
+      <c r="W37" s="65"/>
       <c r="X37" s="55"/>
       <c r="Y37" s="55"/>
       <c r="Z37" s="55" t="s">
@@ -9144,16 +9100,16 @@
       <c r="AG37" s="55" t="s">
         <v>598</v>
       </c>
-      <c r="AH37" s="67"/>
-      <c r="AI37" s="67"/>
-      <c r="AJ37" s="67"/>
-      <c r="AK37" s="67"/>
-      <c r="AL37" s="67"/>
-      <c r="AM37" s="67"/>
-      <c r="AN37" s="67"/>
-      <c r="AO37" s="67"/>
-      <c r="AP37" s="67"/>
-      <c r="AQ37" s="67"/>
+      <c r="AH37" s="65"/>
+      <c r="AI37" s="65"/>
+      <c r="AJ37" s="65"/>
+      <c r="AK37" s="65"/>
+      <c r="AL37" s="65"/>
+      <c r="AM37" s="65"/>
+      <c r="AN37" s="65"/>
+      <c r="AO37" s="65"/>
+      <c r="AP37" s="65"/>
+      <c r="AQ37" s="65"/>
       <c r="AR37" s="55"/>
       <c r="AS37" s="55"/>
       <c r="AT37" s="55"/>
@@ -9228,10 +9184,10 @@
       <c r="U38" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V38" s="67" t="s">
+      <c r="V38" s="65" t="s">
         <v>605</v>
       </c>
-      <c r="W38" s="67" t="s">
+      <c r="W38" s="65" t="s">
         <v>600</v>
       </c>
       <c r="X38" s="55" t="s">
@@ -9260,25 +9216,23 @@
       <c r="AG38" s="55" t="s">
         <v>599</v>
       </c>
-      <c r="AH38" s="67"/>
-      <c r="AI38" s="67"/>
-      <c r="AJ38" s="67"/>
-      <c r="AK38" s="67"/>
-      <c r="AL38" s="67"/>
-      <c r="AM38" s="67"/>
-      <c r="AN38" s="67"/>
-      <c r="AO38" s="67"/>
-      <c r="AP38" s="67"/>
-      <c r="AQ38" s="67"/>
+      <c r="AH38" s="65"/>
+      <c r="AI38" s="65"/>
+      <c r="AJ38" s="65"/>
+      <c r="AK38" s="65"/>
+      <c r="AL38" s="65"/>
+      <c r="AM38" s="65"/>
+      <c r="AN38" s="65"/>
+      <c r="AO38" s="65"/>
+      <c r="AP38" s="65"/>
+      <c r="AQ38" s="65"/>
       <c r="AR38" s="55" t="s">
         <v>608</v>
       </c>
       <c r="AS38" s="55"/>
       <c r="AT38" s="55"/>
       <c r="AU38" s="55"/>
-      <c r="AV38" s="55">
-        <v>2023</v>
-      </c>
+      <c r="AV38" s="55"/>
       <c r="AW38" s="55"/>
       <c r="AX38" s="56" t="s">
         <v>609</v>
@@ -9348,10 +9302,10 @@
       <c r="U39" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V39" s="67" t="s">
+      <c r="V39" s="65" t="s">
         <v>887</v>
       </c>
-      <c r="W39" s="67" t="s">
+      <c r="W39" s="65" t="s">
         <v>611</v>
       </c>
       <c r="X39" s="55" t="s">
@@ -9380,25 +9334,23 @@
       <c r="AG39" s="55" t="s">
         <v>610</v>
       </c>
-      <c r="AH39" s="67"/>
-      <c r="AI39" s="67"/>
-      <c r="AJ39" s="67"/>
-      <c r="AK39" s="67"/>
-      <c r="AL39" s="67"/>
-      <c r="AM39" s="67"/>
-      <c r="AN39" s="67"/>
-      <c r="AO39" s="67"/>
-      <c r="AP39" s="67"/>
-      <c r="AQ39" s="67"/>
+      <c r="AH39" s="65"/>
+      <c r="AI39" s="65"/>
+      <c r="AJ39" s="65"/>
+      <c r="AK39" s="65"/>
+      <c r="AL39" s="65"/>
+      <c r="AM39" s="65"/>
+      <c r="AN39" s="65"/>
+      <c r="AO39" s="65"/>
+      <c r="AP39" s="65"/>
+      <c r="AQ39" s="65"/>
       <c r="AR39" s="55" t="s">
         <v>619</v>
       </c>
       <c r="AS39" s="55"/>
       <c r="AT39" s="55"/>
       <c r="AU39" s="55"/>
-      <c r="AV39" s="55">
-        <v>1994</v>
-      </c>
+      <c r="AV39" s="55"/>
       <c r="AW39" s="55"/>
       <c r="AX39" s="56"/>
       <c r="AY39" s="55"/>
@@ -9462,10 +9414,10 @@
       </c>
       <c r="T40" s="55"/>
       <c r="U40" s="55"/>
-      <c r="V40" s="67" t="s">
+      <c r="V40" s="65" t="s">
         <v>626</v>
       </c>
-      <c r="W40" s="67" t="s">
+      <c r="W40" s="65" t="s">
         <v>627</v>
       </c>
       <c r="X40" s="55"/>
@@ -9488,23 +9440,21 @@
       <c r="AG40" s="55" t="s">
         <v>620</v>
       </c>
-      <c r="AH40" s="67"/>
-      <c r="AI40" s="67"/>
-      <c r="AJ40" s="67"/>
-      <c r="AK40" s="67"/>
-      <c r="AL40" s="67"/>
-      <c r="AM40" s="67"/>
-      <c r="AN40" s="67"/>
-      <c r="AO40" s="67"/>
-      <c r="AP40" s="67"/>
-      <c r="AQ40" s="67"/>
+      <c r="AH40" s="65"/>
+      <c r="AI40" s="65"/>
+      <c r="AJ40" s="65"/>
+      <c r="AK40" s="65"/>
+      <c r="AL40" s="65"/>
+      <c r="AM40" s="65"/>
+      <c r="AN40" s="65"/>
+      <c r="AO40" s="65"/>
+      <c r="AP40" s="65"/>
+      <c r="AQ40" s="65"/>
       <c r="AR40" s="55"/>
       <c r="AS40" s="55"/>
       <c r="AT40" s="55"/>
       <c r="AU40" s="55"/>
-      <c r="AV40" s="55">
-        <v>2023</v>
-      </c>
+      <c r="AV40" s="55"/>
       <c r="AW40" s="55"/>
       <c r="AX40" s="56" t="s">
         <v>99</v>
@@ -9576,10 +9526,10 @@
       <c r="U41" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V41" s="67" t="s">
+      <c r="V41" s="65" t="s">
         <v>633</v>
       </c>
-      <c r="W41" s="67" t="s">
+      <c r="W41" s="65" t="s">
         <v>629</v>
       </c>
       <c r="X41" s="55" t="s">
@@ -9608,25 +9558,23 @@
       <c r="AG41" s="55" t="s">
         <v>628</v>
       </c>
-      <c r="AH41" s="67"/>
-      <c r="AI41" s="67"/>
-      <c r="AJ41" s="67" t="s">
+      <c r="AH41" s="65"/>
+      <c r="AI41" s="65"/>
+      <c r="AJ41" s="65" t="s">
         <v>635</v>
       </c>
-      <c r="AK41" s="67"/>
-      <c r="AL41" s="67"/>
-      <c r="AM41" s="67"/>
-      <c r="AN41" s="67"/>
-      <c r="AO41" s="67"/>
-      <c r="AP41" s="67"/>
-      <c r="AQ41" s="67"/>
+      <c r="AK41" s="65"/>
+      <c r="AL41" s="65"/>
+      <c r="AM41" s="65"/>
+      <c r="AN41" s="65"/>
+      <c r="AO41" s="65"/>
+      <c r="AP41" s="65"/>
+      <c r="AQ41" s="65"/>
       <c r="AR41" s="55"/>
       <c r="AS41" s="55"/>
       <c r="AT41" s="55"/>
       <c r="AU41" s="55"/>
-      <c r="AV41" s="55">
-        <v>2023</v>
-      </c>
+      <c r="AV41" s="55"/>
       <c r="AW41" s="55"/>
       <c r="AX41" s="56"/>
       <c r="AY41" s="55"/>
@@ -9694,10 +9642,10 @@
       <c r="U42" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V42" s="67" t="s">
+      <c r="V42" s="65" t="s">
         <v>888</v>
       </c>
-      <c r="W42" s="67" t="s">
+      <c r="W42" s="65" t="s">
         <v>637</v>
       </c>
       <c r="X42" s="55" t="s">
@@ -9726,23 +9674,21 @@
       <c r="AG42" s="55" t="s">
         <v>636</v>
       </c>
-      <c r="AH42" s="67"/>
-      <c r="AI42" s="67"/>
-      <c r="AJ42" s="67"/>
-      <c r="AK42" s="67"/>
-      <c r="AL42" s="67"/>
-      <c r="AM42" s="67"/>
-      <c r="AN42" s="67"/>
-      <c r="AO42" s="67"/>
-      <c r="AP42" s="67"/>
-      <c r="AQ42" s="67"/>
+      <c r="AH42" s="65"/>
+      <c r="AI42" s="65"/>
+      <c r="AJ42" s="65"/>
+      <c r="AK42" s="65"/>
+      <c r="AL42" s="65"/>
+      <c r="AM42" s="65"/>
+      <c r="AN42" s="65"/>
+      <c r="AO42" s="65"/>
+      <c r="AP42" s="65"/>
+      <c r="AQ42" s="65"/>
       <c r="AR42" s="55"/>
       <c r="AS42" s="55"/>
       <c r="AT42" s="55"/>
       <c r="AU42" s="55"/>
-      <c r="AV42" s="55">
-        <v>2023</v>
-      </c>
+      <c r="AV42" s="55"/>
       <c r="AW42" s="55"/>
       <c r="AX42" s="56" t="s">
         <v>472</v>
@@ -9804,10 +9750,10 @@
       <c r="U43" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V43" s="67" t="s">
+      <c r="V43" s="65" t="s">
         <v>889</v>
       </c>
-      <c r="W43" s="67" t="s">
+      <c r="W43" s="65" t="s">
         <v>646</v>
       </c>
       <c r="X43" s="55" t="s">
@@ -9834,16 +9780,16 @@
       <c r="AG43" s="55" t="s">
         <v>652</v>
       </c>
-      <c r="AH43" s="67"/>
-      <c r="AI43" s="67"/>
-      <c r="AJ43" s="67"/>
-      <c r="AK43" s="67"/>
-      <c r="AL43" s="67"/>
-      <c r="AM43" s="67"/>
-      <c r="AN43" s="67"/>
-      <c r="AO43" s="67"/>
-      <c r="AP43" s="67"/>
-      <c r="AQ43" s="67"/>
+      <c r="AH43" s="65"/>
+      <c r="AI43" s="65"/>
+      <c r="AJ43" s="65"/>
+      <c r="AK43" s="65"/>
+      <c r="AL43" s="65"/>
+      <c r="AM43" s="65"/>
+      <c r="AN43" s="65"/>
+      <c r="AO43" s="65"/>
+      <c r="AP43" s="65"/>
+      <c r="AQ43" s="65"/>
       <c r="AR43" s="55"/>
       <c r="AS43" s="55"/>
       <c r="AT43" s="55"/>
@@ -9890,8 +9836,8 @@
       <c r="S44" s="55"/>
       <c r="T44" s="55"/>
       <c r="U44" s="55"/>
-      <c r="V44" s="67"/>
-      <c r="W44" s="67"/>
+      <c r="V44" s="65"/>
+      <c r="W44" s="65"/>
       <c r="X44" s="55"/>
       <c r="Y44" s="55"/>
       <c r="Z44" s="55" t="s">
@@ -9906,16 +9852,16 @@
       <c r="AG44" s="55" t="s">
         <v>653</v>
       </c>
-      <c r="AH44" s="67"/>
-      <c r="AI44" s="67"/>
-      <c r="AJ44" s="67"/>
-      <c r="AK44" s="67"/>
-      <c r="AL44" s="67"/>
-      <c r="AM44" s="67"/>
-      <c r="AN44" s="67"/>
-      <c r="AO44" s="67"/>
-      <c r="AP44" s="67"/>
-      <c r="AQ44" s="67"/>
+      <c r="AH44" s="65"/>
+      <c r="AI44" s="65"/>
+      <c r="AJ44" s="65"/>
+      <c r="AK44" s="65"/>
+      <c r="AL44" s="65"/>
+      <c r="AM44" s="65"/>
+      <c r="AN44" s="65"/>
+      <c r="AO44" s="65"/>
+      <c r="AP44" s="65"/>
+      <c r="AQ44" s="65"/>
       <c r="AR44" s="55"/>
       <c r="AS44" s="55"/>
       <c r="AT44" s="55"/>
@@ -9962,8 +9908,8 @@
       <c r="S45" s="55"/>
       <c r="T45" s="55"/>
       <c r="U45" s="55"/>
-      <c r="V45" s="67"/>
-      <c r="W45" s="67"/>
+      <c r="V45" s="65"/>
+      <c r="W45" s="65"/>
       <c r="X45" s="55"/>
       <c r="Y45" s="55"/>
       <c r="Z45" s="55" t="s">
@@ -9978,16 +9924,16 @@
       <c r="AG45" s="55" t="s">
         <v>654</v>
       </c>
-      <c r="AH45" s="67"/>
-      <c r="AI45" s="67"/>
-      <c r="AJ45" s="67"/>
-      <c r="AK45" s="67"/>
-      <c r="AL45" s="67"/>
-      <c r="AM45" s="67"/>
-      <c r="AN45" s="67"/>
-      <c r="AO45" s="67"/>
-      <c r="AP45" s="67"/>
-      <c r="AQ45" s="67"/>
+      <c r="AH45" s="65"/>
+      <c r="AI45" s="65"/>
+      <c r="AJ45" s="65"/>
+      <c r="AK45" s="65"/>
+      <c r="AL45" s="65"/>
+      <c r="AM45" s="65"/>
+      <c r="AN45" s="65"/>
+      <c r="AO45" s="65"/>
+      <c r="AP45" s="65"/>
+      <c r="AQ45" s="65"/>
       <c r="AR45" s="55"/>
       <c r="AS45" s="55"/>
       <c r="AT45" s="55"/>
@@ -10036,8 +9982,8 @@
       <c r="S46" s="55"/>
       <c r="T46" s="55"/>
       <c r="U46" s="55"/>
-      <c r="V46" s="67"/>
-      <c r="W46" s="67"/>
+      <c r="V46" s="65"/>
+      <c r="W46" s="65"/>
       <c r="X46" s="55"/>
       <c r="Y46" s="55"/>
       <c r="Z46" s="55" t="s">
@@ -10052,16 +9998,16 @@
       <c r="AG46" s="55" t="s">
         <v>655</v>
       </c>
-      <c r="AH46" s="67"/>
-      <c r="AI46" s="67"/>
-      <c r="AJ46" s="67"/>
-      <c r="AK46" s="67"/>
-      <c r="AL46" s="67"/>
-      <c r="AM46" s="67"/>
-      <c r="AN46" s="67"/>
-      <c r="AO46" s="67"/>
-      <c r="AP46" s="67"/>
-      <c r="AQ46" s="67"/>
+      <c r="AH46" s="65"/>
+      <c r="AI46" s="65"/>
+      <c r="AJ46" s="65"/>
+      <c r="AK46" s="65"/>
+      <c r="AL46" s="65"/>
+      <c r="AM46" s="65"/>
+      <c r="AN46" s="65"/>
+      <c r="AO46" s="65"/>
+      <c r="AP46" s="65"/>
+      <c r="AQ46" s="65"/>
       <c r="AR46" s="55"/>
       <c r="AS46" s="55"/>
       <c r="AT46" s="55"/>
@@ -10134,10 +10080,10 @@
       <c r="U47" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V47" s="67" t="s">
+      <c r="V47" s="65" t="s">
         <v>663</v>
       </c>
-      <c r="W47" s="67" t="s">
+      <c r="W47" s="65" t="s">
         <v>658</v>
       </c>
       <c r="X47" s="55" t="s">
@@ -10168,25 +10114,23 @@
       <c r="AG47" s="55" t="s">
         <v>657</v>
       </c>
-      <c r="AH47" s="67"/>
-      <c r="AI47" s="67"/>
-      <c r="AJ47" s="67" t="s">
+      <c r="AH47" s="65"/>
+      <c r="AI47" s="65"/>
+      <c r="AJ47" s="65" t="s">
         <v>666</v>
       </c>
-      <c r="AK47" s="67"/>
-      <c r="AL47" s="67"/>
-      <c r="AM47" s="67"/>
-      <c r="AN47" s="67"/>
-      <c r="AO47" s="67"/>
-      <c r="AP47" s="67"/>
-      <c r="AQ47" s="67"/>
+      <c r="AK47" s="65"/>
+      <c r="AL47" s="65"/>
+      <c r="AM47" s="65"/>
+      <c r="AN47" s="65"/>
+      <c r="AO47" s="65"/>
+      <c r="AP47" s="65"/>
+      <c r="AQ47" s="65"/>
       <c r="AR47" s="55"/>
       <c r="AS47" s="55"/>
       <c r="AT47" s="55"/>
       <c r="AU47" s="55"/>
-      <c r="AV47" s="55">
-        <v>2017</v>
-      </c>
+      <c r="AV47" s="55"/>
       <c r="AW47" s="55"/>
       <c r="AX47" s="56" t="s">
         <v>667</v>
@@ -10240,8 +10184,8 @@
       <c r="S48" s="55"/>
       <c r="T48" s="55"/>
       <c r="U48" s="55"/>
-      <c r="V48" s="67"/>
-      <c r="W48" s="67"/>
+      <c r="V48" s="65"/>
+      <c r="W48" s="65"/>
       <c r="X48" s="55"/>
       <c r="Y48" s="55"/>
       <c r="Z48" s="55" t="s">
@@ -10260,16 +10204,16 @@
       <c r="AG48" s="55" t="s">
         <v>669</v>
       </c>
-      <c r="AH48" s="67"/>
-      <c r="AI48" s="67"/>
-      <c r="AJ48" s="67"/>
-      <c r="AK48" s="67"/>
-      <c r="AL48" s="67"/>
-      <c r="AM48" s="67"/>
-      <c r="AN48" s="67"/>
-      <c r="AO48" s="67"/>
-      <c r="AP48" s="67"/>
-      <c r="AQ48" s="67"/>
+      <c r="AH48" s="65"/>
+      <c r="AI48" s="65"/>
+      <c r="AJ48" s="65"/>
+      <c r="AK48" s="65"/>
+      <c r="AL48" s="65"/>
+      <c r="AM48" s="65"/>
+      <c r="AN48" s="65"/>
+      <c r="AO48" s="65"/>
+      <c r="AP48" s="65"/>
+      <c r="AQ48" s="65"/>
       <c r="AR48" s="55"/>
       <c r="AS48" s="55"/>
       <c r="AT48" s="55"/>
@@ -10340,10 +10284,10 @@
       <c r="U49" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V49" s="67" t="s">
+      <c r="V49" s="65" t="s">
         <v>890</v>
       </c>
-      <c r="W49" s="67" t="s">
+      <c r="W49" s="65" t="s">
         <v>676</v>
       </c>
       <c r="X49" s="55" t="s">
@@ -10370,23 +10314,21 @@
       <c r="AG49" s="55" t="s">
         <v>675</v>
       </c>
-      <c r="AH49" s="67"/>
-      <c r="AI49" s="67"/>
-      <c r="AJ49" s="67"/>
-      <c r="AK49" s="67"/>
-      <c r="AL49" s="67"/>
-      <c r="AM49" s="67"/>
-      <c r="AN49" s="67"/>
-      <c r="AO49" s="67"/>
-      <c r="AP49" s="67"/>
-      <c r="AQ49" s="67"/>
+      <c r="AH49" s="65"/>
+      <c r="AI49" s="65"/>
+      <c r="AJ49" s="65"/>
+      <c r="AK49" s="65"/>
+      <c r="AL49" s="65"/>
+      <c r="AM49" s="65"/>
+      <c r="AN49" s="65"/>
+      <c r="AO49" s="65"/>
+      <c r="AP49" s="65"/>
+      <c r="AQ49" s="65"/>
       <c r="AR49" s="55"/>
       <c r="AS49" s="55"/>
       <c r="AT49" s="55"/>
       <c r="AU49" s="55"/>
-      <c r="AV49" s="55">
-        <v>1998</v>
-      </c>
+      <c r="AV49" s="55"/>
       <c r="AW49" s="55"/>
       <c r="AX49" s="56" t="s">
         <v>683</v>
@@ -10438,8 +10380,8 @@
       <c r="S50" s="55"/>
       <c r="T50" s="55"/>
       <c r="U50" s="55"/>
-      <c r="V50" s="67"/>
-      <c r="W50" s="67"/>
+      <c r="V50" s="65"/>
+      <c r="W50" s="65"/>
       <c r="X50" s="55"/>
       <c r="Y50" s="55"/>
       <c r="Z50" s="55" t="s">
@@ -10458,16 +10400,16 @@
       <c r="AG50" s="55" t="s">
         <v>684</v>
       </c>
-      <c r="AH50" s="67"/>
-      <c r="AI50" s="67"/>
-      <c r="AJ50" s="67"/>
-      <c r="AK50" s="67"/>
-      <c r="AL50" s="67"/>
-      <c r="AM50" s="67"/>
-      <c r="AN50" s="67"/>
-      <c r="AO50" s="67"/>
-      <c r="AP50" s="67"/>
-      <c r="AQ50" s="67"/>
+      <c r="AH50" s="65"/>
+      <c r="AI50" s="65"/>
+      <c r="AJ50" s="65"/>
+      <c r="AK50" s="65"/>
+      <c r="AL50" s="65"/>
+      <c r="AM50" s="65"/>
+      <c r="AN50" s="65"/>
+      <c r="AO50" s="65"/>
+      <c r="AP50" s="65"/>
+      <c r="AQ50" s="65"/>
       <c r="AR50" s="55"/>
       <c r="AS50" s="55"/>
       <c r="AT50" s="55"/>
@@ -10522,8 +10464,8 @@
       <c r="S51" s="55"/>
       <c r="T51" s="55"/>
       <c r="U51" s="55"/>
-      <c r="V51" s="67"/>
-      <c r="W51" s="67"/>
+      <c r="V51" s="65"/>
+      <c r="W51" s="65"/>
       <c r="X51" s="55"/>
       <c r="Y51" s="55"/>
       <c r="Z51" s="55" t="s">
@@ -10542,16 +10484,16 @@
       <c r="AG51" s="55" t="s">
         <v>689</v>
       </c>
-      <c r="AH51" s="67"/>
-      <c r="AI51" s="67"/>
-      <c r="AJ51" s="67"/>
-      <c r="AK51" s="67"/>
-      <c r="AL51" s="67"/>
-      <c r="AM51" s="67"/>
-      <c r="AN51" s="67"/>
-      <c r="AO51" s="67"/>
-      <c r="AP51" s="67"/>
-      <c r="AQ51" s="67"/>
+      <c r="AH51" s="65"/>
+      <c r="AI51" s="65"/>
+      <c r="AJ51" s="65"/>
+      <c r="AK51" s="65"/>
+      <c r="AL51" s="65"/>
+      <c r="AM51" s="65"/>
+      <c r="AN51" s="65"/>
+      <c r="AO51" s="65"/>
+      <c r="AP51" s="65"/>
+      <c r="AQ51" s="65"/>
       <c r="AR51" s="55"/>
       <c r="AS51" s="55"/>
       <c r="AT51" s="55"/>
@@ -10612,8 +10554,8 @@
       <c r="S52" s="55"/>
       <c r="T52" s="55"/>
       <c r="U52" s="55"/>
-      <c r="V52" s="67"/>
-      <c r="W52" s="67"/>
+      <c r="V52" s="65"/>
+      <c r="W52" s="65"/>
       <c r="X52" s="55"/>
       <c r="Y52" s="55"/>
       <c r="Z52" s="55" t="s">
@@ -10632,16 +10574,16 @@
       <c r="AG52" s="55" t="s">
         <v>697</v>
       </c>
-      <c r="AH52" s="67"/>
-      <c r="AI52" s="67"/>
-      <c r="AJ52" s="67"/>
-      <c r="AK52" s="67"/>
-      <c r="AL52" s="67"/>
-      <c r="AM52" s="67"/>
-      <c r="AN52" s="67"/>
-      <c r="AO52" s="67"/>
-      <c r="AP52" s="67"/>
-      <c r="AQ52" s="67"/>
+      <c r="AH52" s="65"/>
+      <c r="AI52" s="65"/>
+      <c r="AJ52" s="65"/>
+      <c r="AK52" s="65"/>
+      <c r="AL52" s="65"/>
+      <c r="AM52" s="65"/>
+      <c r="AN52" s="65"/>
+      <c r="AO52" s="65"/>
+      <c r="AP52" s="65"/>
+      <c r="AQ52" s="65"/>
       <c r="AR52" s="55"/>
       <c r="AS52" s="55"/>
       <c r="AT52" s="55"/>
@@ -10714,10 +10656,10 @@
       <c r="U53" s="55" t="s">
         <v>708</v>
       </c>
-      <c r="V53" s="67" t="s">
+      <c r="V53" s="65" t="s">
         <v>707</v>
       </c>
-      <c r="W53" s="67" t="s">
+      <c r="W53" s="65" t="s">
         <v>703</v>
       </c>
       <c r="X53" s="55" t="s">
@@ -10746,16 +10688,16 @@
       <c r="AG53" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="AH53" s="67"/>
-      <c r="AI53" s="67"/>
-      <c r="AJ53" s="67"/>
-      <c r="AK53" s="67"/>
-      <c r="AL53" s="67"/>
-      <c r="AM53" s="67"/>
-      <c r="AN53" s="67"/>
-      <c r="AO53" s="67"/>
-      <c r="AP53" s="67"/>
-      <c r="AQ53" s="67"/>
+      <c r="AH53" s="65"/>
+      <c r="AI53" s="65"/>
+      <c r="AJ53" s="65"/>
+      <c r="AK53" s="65"/>
+      <c r="AL53" s="65"/>
+      <c r="AM53" s="65"/>
+      <c r="AN53" s="65"/>
+      <c r="AO53" s="65"/>
+      <c r="AP53" s="65"/>
+      <c r="AQ53" s="65"/>
       <c r="AR53" s="59">
         <v>85.404166666666669</v>
       </c>
@@ -10764,9 +10706,7 @@
         <v>578</v>
       </c>
       <c r="AU53" s="55"/>
-      <c r="AV53" s="55">
-        <v>2007</v>
-      </c>
+      <c r="AV53" s="55"/>
       <c r="AW53" s="55"/>
       <c r="AX53" s="56" t="s">
         <v>99</v>
@@ -10822,10 +10762,10 @@
       <c r="S54" s="55"/>
       <c r="T54" s="55"/>
       <c r="U54" s="55"/>
-      <c r="V54" s="67" t="s">
+      <c r="V54" s="65" t="s">
         <v>891</v>
       </c>
-      <c r="W54" s="67" t="s">
+      <c r="W54" s="65" t="s">
         <v>713</v>
       </c>
       <c r="X54" s="55"/>
@@ -10846,18 +10786,18 @@
       <c r="AG54" s="55" t="s">
         <v>712</v>
       </c>
-      <c r="AH54" s="67"/>
-      <c r="AI54" s="67"/>
-      <c r="AJ54" s="67" t="s">
+      <c r="AH54" s="65"/>
+      <c r="AI54" s="65"/>
+      <c r="AJ54" s="65" t="s">
         <v>720</v>
       </c>
-      <c r="AK54" s="67"/>
-      <c r="AL54" s="67"/>
-      <c r="AM54" s="67"/>
-      <c r="AN54" s="67"/>
-      <c r="AO54" s="67"/>
-      <c r="AP54" s="67"/>
-      <c r="AQ54" s="67"/>
+      <c r="AK54" s="65"/>
+      <c r="AL54" s="65"/>
+      <c r="AM54" s="65"/>
+      <c r="AN54" s="65"/>
+      <c r="AO54" s="65"/>
+      <c r="AP54" s="65"/>
+      <c r="AQ54" s="65"/>
       <c r="AR54" s="55"/>
       <c r="AS54" s="55"/>
       <c r="AT54" s="55"/>
@@ -10906,8 +10846,8 @@
       <c r="S55" s="55"/>
       <c r="T55" s="55"/>
       <c r="U55" s="55"/>
-      <c r="V55" s="67"/>
-      <c r="W55" s="67"/>
+      <c r="V55" s="65"/>
+      <c r="W55" s="65"/>
       <c r="X55" s="55"/>
       <c r="Y55" s="55"/>
       <c r="Z55" s="55" t="s">
@@ -10922,16 +10862,16 @@
       <c r="AG55" s="55" t="s">
         <v>721</v>
       </c>
-      <c r="AH55" s="67"/>
-      <c r="AI55" s="67"/>
-      <c r="AJ55" s="67"/>
-      <c r="AK55" s="67"/>
-      <c r="AL55" s="67"/>
-      <c r="AM55" s="67"/>
-      <c r="AN55" s="67"/>
-      <c r="AO55" s="67"/>
-      <c r="AP55" s="67"/>
-      <c r="AQ55" s="67"/>
+      <c r="AH55" s="65"/>
+      <c r="AI55" s="65"/>
+      <c r="AJ55" s="65"/>
+      <c r="AK55" s="65"/>
+      <c r="AL55" s="65"/>
+      <c r="AM55" s="65"/>
+      <c r="AN55" s="65"/>
+      <c r="AO55" s="65"/>
+      <c r="AP55" s="65"/>
+      <c r="AQ55" s="65"/>
       <c r="AR55" s="55"/>
       <c r="AS55" s="55"/>
       <c r="AT55" s="55"/>
@@ -10994,10 +10934,10 @@
       <c r="U56" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V56" s="67" t="s">
+      <c r="V56" s="65" t="s">
         <v>892</v>
       </c>
-      <c r="W56" s="67" t="s">
+      <c r="W56" s="65" t="s">
         <v>723</v>
       </c>
       <c r="X56" s="55" t="s">
@@ -11026,16 +10966,16 @@
       <c r="AG56" s="55" t="s">
         <v>722</v>
       </c>
-      <c r="AH56" s="67"/>
-      <c r="AI56" s="67"/>
-      <c r="AJ56" s="67"/>
-      <c r="AK56" s="67"/>
-      <c r="AL56" s="67"/>
-      <c r="AM56" s="67"/>
-      <c r="AN56" s="67"/>
-      <c r="AO56" s="67"/>
-      <c r="AP56" s="67"/>
-      <c r="AQ56" s="67"/>
+      <c r="AH56" s="65"/>
+      <c r="AI56" s="65"/>
+      <c r="AJ56" s="65"/>
+      <c r="AK56" s="65"/>
+      <c r="AL56" s="65"/>
+      <c r="AM56" s="65"/>
+      <c r="AN56" s="65"/>
+      <c r="AO56" s="65"/>
+      <c r="AP56" s="65"/>
+      <c r="AQ56" s="65"/>
       <c r="AR56" s="55"/>
       <c r="AS56" s="55"/>
       <c r="AT56" s="55"/>
@@ -11084,8 +11024,8 @@
       <c r="S57" s="55"/>
       <c r="T57" s="55"/>
       <c r="U57" s="55"/>
-      <c r="V57" s="67"/>
-      <c r="W57" s="67"/>
+      <c r="V57" s="65"/>
+      <c r="W57" s="65"/>
       <c r="X57" s="55"/>
       <c r="Y57" s="55"/>
       <c r="Z57" s="55" t="s">
@@ -11100,16 +11040,16 @@
       <c r="AG57" s="55" t="s">
         <v>730</v>
       </c>
-      <c r="AH57" s="67"/>
-      <c r="AI57" s="67"/>
-      <c r="AJ57" s="67"/>
-      <c r="AK57" s="67"/>
-      <c r="AL57" s="67"/>
-      <c r="AM57" s="67"/>
-      <c r="AN57" s="67"/>
-      <c r="AO57" s="67"/>
-      <c r="AP57" s="67"/>
-      <c r="AQ57" s="67"/>
+      <c r="AH57" s="65"/>
+      <c r="AI57" s="65"/>
+      <c r="AJ57" s="65"/>
+      <c r="AK57" s="65"/>
+      <c r="AL57" s="65"/>
+      <c r="AM57" s="65"/>
+      <c r="AN57" s="65"/>
+      <c r="AO57" s="65"/>
+      <c r="AP57" s="65"/>
+      <c r="AQ57" s="65"/>
       <c r="AR57" s="55"/>
       <c r="AS57" s="55"/>
       <c r="AT57" s="55"/>
@@ -11178,10 +11118,10 @@
       <c r="U58" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V58" s="67" t="s">
+      <c r="V58" s="65" t="s">
         <v>736</v>
       </c>
-      <c r="W58" s="67" t="s">
+      <c r="W58" s="65" t="s">
         <v>733</v>
       </c>
       <c r="X58" s="55" t="s">
@@ -11208,16 +11148,16 @@
       <c r="AG58" s="55" t="s">
         <v>732</v>
       </c>
-      <c r="AH58" s="67"/>
-      <c r="AI58" s="67"/>
-      <c r="AJ58" s="67"/>
-      <c r="AK58" s="67"/>
-      <c r="AL58" s="67"/>
-      <c r="AM58" s="67"/>
-      <c r="AN58" s="67"/>
-      <c r="AO58" s="67"/>
-      <c r="AP58" s="67"/>
-      <c r="AQ58" s="67"/>
+      <c r="AH58" s="65"/>
+      <c r="AI58" s="65"/>
+      <c r="AJ58" s="65"/>
+      <c r="AK58" s="65"/>
+      <c r="AL58" s="65"/>
+      <c r="AM58" s="65"/>
+      <c r="AN58" s="65"/>
+      <c r="AO58" s="65"/>
+      <c r="AP58" s="65"/>
+      <c r="AQ58" s="65"/>
       <c r="AR58" s="55" t="s">
         <v>737</v>
       </c>
@@ -11288,10 +11228,10 @@
       <c r="S59" s="55"/>
       <c r="T59" s="55"/>
       <c r="U59" s="55"/>
-      <c r="V59" s="67" t="s">
+      <c r="V59" s="65" t="s">
         <v>893</v>
       </c>
-      <c r="W59" s="67" t="s">
+      <c r="W59" s="65" t="s">
         <v>739</v>
       </c>
       <c r="X59" s="55"/>
@@ -11316,20 +11256,20 @@
       <c r="AG59" s="55" t="s">
         <v>738</v>
       </c>
-      <c r="AH59" s="67" t="s">
+      <c r="AH59" s="65" t="s">
         <v>748</v>
       </c>
-      <c r="AI59" s="67" t="s">
+      <c r="AI59" s="65" t="s">
         <v>749</v>
       </c>
-      <c r="AJ59" s="67"/>
-      <c r="AK59" s="67"/>
-      <c r="AL59" s="67"/>
-      <c r="AM59" s="67"/>
-      <c r="AN59" s="67"/>
-      <c r="AO59" s="67"/>
-      <c r="AP59" s="67"/>
-      <c r="AQ59" s="67"/>
+      <c r="AJ59" s="65"/>
+      <c r="AK59" s="65"/>
+      <c r="AL59" s="65"/>
+      <c r="AM59" s="65"/>
+      <c r="AN59" s="65"/>
+      <c r="AO59" s="65"/>
+      <c r="AP59" s="65"/>
+      <c r="AQ59" s="65"/>
       <c r="AR59" s="55"/>
       <c r="AS59" s="55"/>
       <c r="AT59" s="55"/>
@@ -11392,10 +11332,10 @@
       <c r="U60" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V60" s="67" t="s">
+      <c r="V60" s="65" t="s">
         <v>894</v>
       </c>
-      <c r="W60" s="67" t="s">
+      <c r="W60" s="65" t="s">
         <v>751</v>
       </c>
       <c r="X60" s="55" t="s">
@@ -11424,16 +11364,16 @@
       <c r="AG60" s="55" t="s">
         <v>750</v>
       </c>
-      <c r="AH60" s="67"/>
-      <c r="AI60" s="67"/>
-      <c r="AJ60" s="67"/>
-      <c r="AK60" s="67"/>
-      <c r="AL60" s="67"/>
-      <c r="AM60" s="67"/>
-      <c r="AN60" s="67"/>
-      <c r="AO60" s="67"/>
-      <c r="AP60" s="67"/>
-      <c r="AQ60" s="67"/>
+      <c r="AH60" s="65"/>
+      <c r="AI60" s="65"/>
+      <c r="AJ60" s="65"/>
+      <c r="AK60" s="65"/>
+      <c r="AL60" s="65"/>
+      <c r="AM60" s="65"/>
+      <c r="AN60" s="65"/>
+      <c r="AO60" s="65"/>
+      <c r="AP60" s="65"/>
+      <c r="AQ60" s="65"/>
       <c r="AR60" s="55"/>
       <c r="AS60" s="55"/>
       <c r="AT60" s="55"/>
@@ -11494,8 +11434,8 @@
       <c r="U61" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V61" s="67"/>
-      <c r="W61" s="67"/>
+      <c r="V61" s="65"/>
+      <c r="W61" s="65"/>
       <c r="X61" s="55" t="s">
         <v>85</v>
       </c>
@@ -11516,23 +11456,21 @@
       <c r="AG61" s="55" t="s">
         <v>758</v>
       </c>
-      <c r="AH61" s="67"/>
-      <c r="AI61" s="67"/>
-      <c r="AJ61" s="67"/>
-      <c r="AK61" s="67"/>
-      <c r="AL61" s="67"/>
-      <c r="AM61" s="67"/>
-      <c r="AN61" s="67"/>
-      <c r="AO61" s="67"/>
-      <c r="AP61" s="67"/>
-      <c r="AQ61" s="67"/>
+      <c r="AH61" s="65"/>
+      <c r="AI61" s="65"/>
+      <c r="AJ61" s="65"/>
+      <c r="AK61" s="65"/>
+      <c r="AL61" s="65"/>
+      <c r="AM61" s="65"/>
+      <c r="AN61" s="65"/>
+      <c r="AO61" s="65"/>
+      <c r="AP61" s="65"/>
+      <c r="AQ61" s="65"/>
       <c r="AR61" s="55"/>
       <c r="AS61" s="55"/>
       <c r="AT61" s="55"/>
       <c r="AU61" s="55"/>
-      <c r="AV61" s="55">
-        <v>1986</v>
-      </c>
+      <c r="AV61" s="55"/>
       <c r="AW61" s="55"/>
       <c r="AX61" s="56" t="s">
         <v>99</v>
@@ -11592,10 +11530,10 @@
       <c r="U62" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V62" s="67" t="s">
+      <c r="V62" s="65" t="s">
         <v>895</v>
       </c>
-      <c r="W62" s="67" t="s">
+      <c r="W62" s="65" t="s">
         <v>760</v>
       </c>
       <c r="X62" s="55" t="s">
@@ -11622,16 +11560,16 @@
       <c r="AG62" s="55" t="s">
         <v>759</v>
       </c>
-      <c r="AH62" s="67"/>
-      <c r="AI62" s="67"/>
-      <c r="AJ62" s="67"/>
-      <c r="AK62" s="67"/>
-      <c r="AL62" s="67"/>
-      <c r="AM62" s="67"/>
-      <c r="AN62" s="67"/>
-      <c r="AO62" s="67"/>
-      <c r="AP62" s="67"/>
-      <c r="AQ62" s="67"/>
+      <c r="AH62" s="65"/>
+      <c r="AI62" s="65"/>
+      <c r="AJ62" s="65"/>
+      <c r="AK62" s="65"/>
+      <c r="AL62" s="65"/>
+      <c r="AM62" s="65"/>
+      <c r="AN62" s="65"/>
+      <c r="AO62" s="65"/>
+      <c r="AP62" s="65"/>
+      <c r="AQ62" s="65"/>
       <c r="AR62" s="55"/>
       <c r="AS62" s="55"/>
       <c r="AT62" s="55"/>
@@ -11682,8 +11620,8 @@
       <c r="S63" s="55"/>
       <c r="T63" s="55"/>
       <c r="U63" s="55"/>
-      <c r="V63" s="67"/>
-      <c r="W63" s="67"/>
+      <c r="V63" s="65"/>
+      <c r="W63" s="65"/>
       <c r="X63" s="55"/>
       <c r="Y63" s="55"/>
       <c r="Z63" s="55" t="s">
@@ -11698,16 +11636,16 @@
       <c r="AG63" s="55" t="s">
         <v>768</v>
       </c>
-      <c r="AH63" s="67"/>
-      <c r="AI63" s="67"/>
-      <c r="AJ63" s="67"/>
-      <c r="AK63" s="67"/>
-      <c r="AL63" s="67"/>
-      <c r="AM63" s="67"/>
-      <c r="AN63" s="67"/>
-      <c r="AO63" s="67"/>
-      <c r="AP63" s="67"/>
-      <c r="AQ63" s="67"/>
+      <c r="AH63" s="65"/>
+      <c r="AI63" s="65"/>
+      <c r="AJ63" s="65"/>
+      <c r="AK63" s="65"/>
+      <c r="AL63" s="65"/>
+      <c r="AM63" s="65"/>
+      <c r="AN63" s="65"/>
+      <c r="AO63" s="65"/>
+      <c r="AP63" s="65"/>
+      <c r="AQ63" s="65"/>
       <c r="AR63" s="55"/>
       <c r="AS63" s="55"/>
       <c r="AT63" s="55"/>
@@ -11780,10 +11718,10 @@
       <c r="U64" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V64" s="67" t="s">
+      <c r="V64" s="65" t="s">
         <v>775</v>
       </c>
-      <c r="W64" s="67" t="s">
+      <c r="W64" s="65" t="s">
         <v>770</v>
       </c>
       <c r="X64" s="55" t="s">
@@ -11810,29 +11748,27 @@
       <c r="AG64" s="55" t="s">
         <v>778</v>
       </c>
-      <c r="AH64" s="67" t="s">
+      <c r="AH64" s="65" t="s">
         <v>779</v>
       </c>
-      <c r="AI64" s="67" t="s">
+      <c r="AI64" s="65" t="s">
         <v>780</v>
       </c>
-      <c r="AJ64" s="67"/>
-      <c r="AK64" s="67"/>
-      <c r="AL64" s="67"/>
-      <c r="AM64" s="67"/>
-      <c r="AN64" s="67"/>
-      <c r="AO64" s="67"/>
-      <c r="AP64" s="67"/>
-      <c r="AQ64" s="67"/>
+      <c r="AJ64" s="65"/>
+      <c r="AK64" s="65"/>
+      <c r="AL64" s="65"/>
+      <c r="AM64" s="65"/>
+      <c r="AN64" s="65"/>
+      <c r="AO64" s="65"/>
+      <c r="AP64" s="65"/>
+      <c r="AQ64" s="65"/>
       <c r="AR64" s="55"/>
       <c r="AS64" s="55"/>
       <c r="AT64" s="55">
         <v>2013</v>
       </c>
       <c r="AU64" s="55"/>
-      <c r="AV64" s="55">
-        <v>1998</v>
-      </c>
+      <c r="AV64" s="55"/>
       <c r="AW64" s="55"/>
       <c r="AX64" s="56"/>
       <c r="AY64" s="55"/>
@@ -11890,10 +11826,10 @@
       <c r="U65" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V65" s="67" t="s">
+      <c r="V65" s="65" t="s">
         <v>786</v>
       </c>
-      <c r="W65" s="67" t="s">
+      <c r="W65" s="65" t="s">
         <v>782</v>
       </c>
       <c r="X65" s="55" t="s">
@@ -11922,16 +11858,16 @@
       <c r="AG65" s="55" t="s">
         <v>781</v>
       </c>
-      <c r="AH65" s="67"/>
-      <c r="AI65" s="67"/>
-      <c r="AJ65" s="67"/>
-      <c r="AK65" s="67"/>
-      <c r="AL65" s="67"/>
-      <c r="AM65" s="67"/>
-      <c r="AN65" s="67"/>
-      <c r="AO65" s="67"/>
-      <c r="AP65" s="67"/>
-      <c r="AQ65" s="67"/>
+      <c r="AH65" s="65"/>
+      <c r="AI65" s="65"/>
+      <c r="AJ65" s="65"/>
+      <c r="AK65" s="65"/>
+      <c r="AL65" s="65"/>
+      <c r="AM65" s="65"/>
+      <c r="AN65" s="65"/>
+      <c r="AO65" s="65"/>
+      <c r="AP65" s="65"/>
+      <c r="AQ65" s="65"/>
       <c r="AR65" s="55"/>
       <c r="AS65" s="55"/>
       <c r="AT65" s="55"/>
@@ -12008,10 +11944,10 @@
       <c r="U66" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V66" s="67" t="s">
+      <c r="V66" s="65" t="s">
         <v>795</v>
       </c>
-      <c r="W66" s="67" t="s">
+      <c r="W66" s="65" t="s">
         <v>790</v>
       </c>
       <c r="X66" s="55" t="s">
@@ -12038,25 +11974,23 @@
       <c r="AG66" s="55" t="s">
         <v>789</v>
       </c>
-      <c r="AH66" s="67"/>
-      <c r="AI66" s="67"/>
-      <c r="AJ66" s="67"/>
-      <c r="AK66" s="67"/>
-      <c r="AL66" s="67"/>
-      <c r="AM66" s="67"/>
-      <c r="AN66" s="67"/>
-      <c r="AO66" s="67"/>
-      <c r="AP66" s="67"/>
-      <c r="AQ66" s="67"/>
+      <c r="AH66" s="65"/>
+      <c r="AI66" s="65"/>
+      <c r="AJ66" s="65"/>
+      <c r="AK66" s="65"/>
+      <c r="AL66" s="65"/>
+      <c r="AM66" s="65"/>
+      <c r="AN66" s="65"/>
+      <c r="AO66" s="65"/>
+      <c r="AP66" s="65"/>
+      <c r="AQ66" s="65"/>
       <c r="AR66" s="55">
         <v>2019</v>
       </c>
       <c r="AS66" s="55"/>
       <c r="AT66" s="55"/>
       <c r="AU66" s="55"/>
-      <c r="AV66" s="55">
-        <v>2012</v>
-      </c>
+      <c r="AV66" s="55"/>
       <c r="AW66" s="55"/>
       <c r="AX66" s="56" t="s">
         <v>99</v>
@@ -12118,10 +12052,10 @@
       </c>
       <c r="T67" s="55"/>
       <c r="U67" s="55"/>
-      <c r="V67" s="67" t="s">
+      <c r="V67" s="65" t="s">
         <v>896</v>
       </c>
-      <c r="W67" s="67" t="s">
+      <c r="W67" s="65" t="s">
         <v>799</v>
       </c>
       <c r="X67" s="55"/>
@@ -12140,16 +12074,16 @@
       <c r="AG67" s="55" t="s">
         <v>798</v>
       </c>
-      <c r="AH67" s="67"/>
-      <c r="AI67" s="67"/>
-      <c r="AJ67" s="67"/>
-      <c r="AK67" s="67"/>
-      <c r="AL67" s="67"/>
-      <c r="AM67" s="67"/>
-      <c r="AN67" s="67"/>
-      <c r="AO67" s="67"/>
-      <c r="AP67" s="67"/>
-      <c r="AQ67" s="67"/>
+      <c r="AH67" s="65"/>
+      <c r="AI67" s="65"/>
+      <c r="AJ67" s="65"/>
+      <c r="AK67" s="65"/>
+      <c r="AL67" s="65"/>
+      <c r="AM67" s="65"/>
+      <c r="AN67" s="65"/>
+      <c r="AO67" s="65"/>
+      <c r="AP67" s="65"/>
+      <c r="AQ67" s="65"/>
       <c r="AR67" s="55"/>
       <c r="AS67" s="55"/>
       <c r="AT67" s="55"/>
@@ -12212,10 +12146,10 @@
       <c r="U68" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V68" s="67" t="s">
+      <c r="V68" s="65" t="s">
         <v>897</v>
       </c>
-      <c r="W68" s="67" t="s">
+      <c r="W68" s="65" t="s">
         <v>805</v>
       </c>
       <c r="X68" s="55" t="s">
@@ -12242,16 +12176,16 @@
       <c r="AG68" s="55" t="s">
         <v>804</v>
       </c>
-      <c r="AH68" s="67"/>
-      <c r="AI68" s="67"/>
-      <c r="AJ68" s="67"/>
-      <c r="AK68" s="67"/>
-      <c r="AL68" s="67"/>
-      <c r="AM68" s="67"/>
-      <c r="AN68" s="67"/>
-      <c r="AO68" s="67"/>
-      <c r="AP68" s="67"/>
-      <c r="AQ68" s="67"/>
+      <c r="AH68" s="65"/>
+      <c r="AI68" s="65"/>
+      <c r="AJ68" s="65"/>
+      <c r="AK68" s="65"/>
+      <c r="AL68" s="65"/>
+      <c r="AM68" s="65"/>
+      <c r="AN68" s="65"/>
+      <c r="AO68" s="65"/>
+      <c r="AP68" s="65"/>
+      <c r="AQ68" s="65"/>
       <c r="AR68" s="55"/>
       <c r="AS68" s="55"/>
       <c r="AT68" s="55"/>
@@ -12326,10 +12260,10 @@
       <c r="U69" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V69" s="67" t="s">
+      <c r="V69" s="65" t="s">
         <v>818</v>
       </c>
-      <c r="W69" s="67" t="s">
+      <c r="W69" s="65" t="s">
         <v>813</v>
       </c>
       <c r="X69" s="55" t="s">
@@ -12358,34 +12292,34 @@
       <c r="AG69" s="55" t="s">
         <v>812</v>
       </c>
-      <c r="AH69" s="67" t="s">
+      <c r="AH69" s="65" t="s">
         <v>822</v>
       </c>
-      <c r="AI69" s="67" t="s">
+      <c r="AI69" s="65" t="s">
         <v>823</v>
       </c>
-      <c r="AJ69" s="67" t="s">
+      <c r="AJ69" s="65" t="s">
         <v>824</v>
       </c>
-      <c r="AK69" s="67" t="s">
+      <c r="AK69" s="65" t="s">
         <v>825</v>
       </c>
-      <c r="AL69" s="67" t="s">
+      <c r="AL69" s="65" t="s">
         <v>826</v>
       </c>
-      <c r="AM69" s="67" t="s">
+      <c r="AM69" s="65" t="s">
         <v>827</v>
       </c>
-      <c r="AN69" s="67" t="s">
+      <c r="AN69" s="65" t="s">
         <v>828</v>
       </c>
-      <c r="AO69" s="67" t="s">
+      <c r="AO69" s="65" t="s">
         <v>829</v>
       </c>
-      <c r="AP69" s="67" t="s">
+      <c r="AP69" s="65" t="s">
         <v>830</v>
       </c>
-      <c r="AQ69" s="67" t="s">
+      <c r="AQ69" s="65" t="s">
         <v>831</v>
       </c>
       <c r="AR69" s="55" t="s">
@@ -12396,9 +12330,7 @@
       </c>
       <c r="AT69" s="55"/>
       <c r="AU69" s="55"/>
-      <c r="AV69" s="55">
-        <v>1988</v>
-      </c>
+      <c r="AV69" s="55"/>
       <c r="AW69" s="55"/>
       <c r="AX69" s="56" t="s">
         <v>833</v>
@@ -12460,10 +12392,10 @@
       <c r="U70" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V70" s="67" t="s">
+      <c r="V70" s="65" t="s">
         <v>898</v>
       </c>
-      <c r="W70" s="67" t="s">
+      <c r="W70" s="65" t="s">
         <v>835</v>
       </c>
       <c r="X70" s="55" t="s">
@@ -12494,18 +12426,18 @@
       <c r="AG70" s="55" t="s">
         <v>834</v>
       </c>
-      <c r="AH70" s="67"/>
-      <c r="AI70" s="67"/>
-      <c r="AJ70" s="67" t="s">
+      <c r="AH70" s="65"/>
+      <c r="AI70" s="65"/>
+      <c r="AJ70" s="65" t="s">
         <v>844</v>
       </c>
-      <c r="AK70" s="67"/>
-      <c r="AL70" s="67"/>
-      <c r="AM70" s="67"/>
-      <c r="AN70" s="67"/>
-      <c r="AO70" s="67"/>
-      <c r="AP70" s="67"/>
-      <c r="AQ70" s="67"/>
+      <c r="AK70" s="65"/>
+      <c r="AL70" s="65"/>
+      <c r="AM70" s="65"/>
+      <c r="AN70" s="65"/>
+      <c r="AO70" s="65"/>
+      <c r="AP70" s="65"/>
+      <c r="AQ70" s="65"/>
       <c r="AR70" s="55"/>
       <c r="AS70" s="55">
         <v>2016</v>
@@ -12572,10 +12504,10 @@
       <c r="U71" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V71" s="67" t="s">
+      <c r="V71" s="65" t="s">
         <v>899</v>
       </c>
-      <c r="W71" s="67" t="s">
+      <c r="W71" s="65" t="s">
         <v>847</v>
       </c>
       <c r="X71" s="55" t="s">
@@ -12602,16 +12534,16 @@
       <c r="AG71" s="55" t="s">
         <v>846</v>
       </c>
-      <c r="AH71" s="67"/>
-      <c r="AI71" s="67"/>
-      <c r="AJ71" s="67"/>
-      <c r="AK71" s="67"/>
-      <c r="AL71" s="67"/>
-      <c r="AM71" s="67"/>
-      <c r="AN71" s="67"/>
-      <c r="AO71" s="67"/>
-      <c r="AP71" s="67"/>
-      <c r="AQ71" s="67"/>
+      <c r="AH71" s="65"/>
+      <c r="AI71" s="65"/>
+      <c r="AJ71" s="65"/>
+      <c r="AK71" s="65"/>
+      <c r="AL71" s="65"/>
+      <c r="AM71" s="65"/>
+      <c r="AN71" s="65"/>
+      <c r="AO71" s="65"/>
+      <c r="AP71" s="65"/>
+      <c r="AQ71" s="65"/>
       <c r="AR71" s="55"/>
       <c r="AS71" s="55"/>
       <c r="AT71" s="55"/>
@@ -12660,8 +12592,8 @@
       <c r="S72" s="55"/>
       <c r="T72" s="55"/>
       <c r="U72" s="55"/>
-      <c r="V72" s="67"/>
-      <c r="W72" s="67"/>
+      <c r="V72" s="65"/>
+      <c r="W72" s="65"/>
       <c r="X72" s="55"/>
       <c r="Y72" s="55"/>
       <c r="Z72" s="55" t="s">
@@ -12676,16 +12608,16 @@
       <c r="AG72" s="55" t="s">
         <v>853</v>
       </c>
-      <c r="AH72" s="67"/>
-      <c r="AI72" s="67"/>
-      <c r="AJ72" s="67"/>
-      <c r="AK72" s="67"/>
-      <c r="AL72" s="67"/>
-      <c r="AM72" s="67"/>
-      <c r="AN72" s="67"/>
-      <c r="AO72" s="67"/>
-      <c r="AP72" s="67"/>
-      <c r="AQ72" s="67"/>
+      <c r="AH72" s="65"/>
+      <c r="AI72" s="65"/>
+      <c r="AJ72" s="65"/>
+      <c r="AK72" s="65"/>
+      <c r="AL72" s="65"/>
+      <c r="AM72" s="65"/>
+      <c r="AN72" s="65"/>
+      <c r="AO72" s="65"/>
+      <c r="AP72" s="65"/>
+      <c r="AQ72" s="65"/>
       <c r="AR72" s="55"/>
       <c r="AS72" s="55"/>
       <c r="AT72" s="55"/>
@@ -12746,10 +12678,10 @@
       <c r="S73" s="55"/>
       <c r="T73" s="55"/>
       <c r="U73" s="55"/>
-      <c r="V73" s="67" t="s">
+      <c r="V73" s="65" t="s">
         <v>860</v>
       </c>
-      <c r="W73" s="67" t="s">
+      <c r="W73" s="65" t="s">
         <v>855</v>
       </c>
       <c r="X73" s="55"/>
@@ -12770,16 +12702,16 @@
       <c r="AG73" s="55" t="s">
         <v>854</v>
       </c>
-      <c r="AH73" s="67"/>
-      <c r="AI73" s="67"/>
-      <c r="AJ73" s="67"/>
-      <c r="AK73" s="67"/>
-      <c r="AL73" s="67"/>
-      <c r="AM73" s="67"/>
-      <c r="AN73" s="67"/>
-      <c r="AO73" s="67"/>
-      <c r="AP73" s="67"/>
-      <c r="AQ73" s="67"/>
+      <c r="AH73" s="65"/>
+      <c r="AI73" s="65"/>
+      <c r="AJ73" s="65"/>
+      <c r="AK73" s="65"/>
+      <c r="AL73" s="65"/>
+      <c r="AM73" s="65"/>
+      <c r="AN73" s="65"/>
+      <c r="AO73" s="65"/>
+      <c r="AP73" s="65"/>
+      <c r="AQ73" s="65"/>
       <c r="AR73" s="55"/>
       <c r="AS73" s="55"/>
       <c r="AT73" s="55"/>
@@ -12828,8 +12760,8 @@
       <c r="S74" s="55"/>
       <c r="T74" s="55"/>
       <c r="U74" s="55"/>
-      <c r="V74" s="67"/>
-      <c r="W74" s="67"/>
+      <c r="V74" s="65"/>
+      <c r="W74" s="65"/>
       <c r="X74" s="55"/>
       <c r="Y74" s="55"/>
       <c r="Z74" s="55" t="s">
@@ -12844,16 +12776,16 @@
       <c r="AG74" s="55" t="s">
         <v>862</v>
       </c>
-      <c r="AH74" s="67"/>
-      <c r="AI74" s="67"/>
-      <c r="AJ74" s="67"/>
-      <c r="AK74" s="67"/>
-      <c r="AL74" s="67"/>
-      <c r="AM74" s="67"/>
-      <c r="AN74" s="67"/>
-      <c r="AO74" s="67"/>
-      <c r="AP74" s="67"/>
-      <c r="AQ74" s="67"/>
+      <c r="AH74" s="65"/>
+      <c r="AI74" s="65"/>
+      <c r="AJ74" s="65"/>
+      <c r="AK74" s="65"/>
+      <c r="AL74" s="65"/>
+      <c r="AM74" s="65"/>
+      <c r="AN74" s="65"/>
+      <c r="AO74" s="65"/>
+      <c r="AP74" s="65"/>
+      <c r="AQ74" s="65"/>
       <c r="AR74" s="55"/>
       <c r="AS74" s="55"/>
       <c r="AT74" s="55"/>

</xml_diff>

<commit_message>
Refactor city extraction logic and handle missing city in target file
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C6B8BB-73C9-C441-870F-52226363808D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957B5CA7-6628-E14D-92BF-F99CA37CA19D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-3220" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Overview" sheetId="1" r:id="rId1"/>
@@ -4708,10 +4708,10 @@
   <dimension ref="A1:AZ1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Delete Harvard University - Division of Engineering and Applied Physics row
I noticed that in the Zone 1 Activity Excel sheet, the target sheet for updates, there are two different entries for Harvard College: ‘Harvard University’ (highlighted in green, indicating a chapter report submission within the last 5 years) and ‘Harvard University - Division of Engineering and Applied Physics’ (in gray for the opposite reason). To simplify comparisons and reduce confusion, I have decided to delete the latter row and keep the most recently updated one. Don’t worry, I have the original Excel sheet saved, and the deleted row contains no meaningful information, not even recent SPS awards.
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BFB1DA-8CAE-0647-A0D6-20D8679DBC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13795DA8-0833-4543-8172-424BA1664941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-3220" windowWidth="38400" windowHeight="24000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1545" uniqueCount="870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="865">
   <si>
     <t>2022 Zone Activity Review</t>
   </si>
@@ -1945,21 +1945,6 @@
   </si>
   <si>
     <t>2015; 2016; 2018; 2019; 2021</t>
-  </si>
-  <si>
-    <t>Harvard University - Division of Engineering and Applied Physics</t>
-  </si>
-  <si>
-    <t>29 Oxford Street</t>
-  </si>
-  <si>
-    <t>02138-2902</t>
-  </si>
-  <si>
-    <t>Eric Mazur</t>
-  </si>
-  <si>
-    <t>mazur@seas.harvard.edu</t>
   </si>
   <si>
     <t>2016; 2017; 2018; 2019</t>
@@ -3098,7 +3083,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AZ1048576" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:AZ1048575" headerRowCount="0">
   <tableColumns count="52">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -4559,13 +4544,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AZ1000"/>
+  <dimension ref="A1:AZ999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AT2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV10" sqref="AV10"/>
+      <selection pane="bottomRight" activeCell="AF52" sqref="AF52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4841,7 +4826,7 @@
         <v>85</v>
       </c>
       <c r="V2" s="39" t="s">
-        <v>825</v>
+        <v>820</v>
       </c>
       <c r="W2" s="62" t="s">
         <v>77</v>
@@ -5093,10 +5078,10 @@
         <v>85</v>
       </c>
       <c r="V4" s="63" t="s">
-        <v>826</v>
+        <v>821</v>
       </c>
       <c r="W4" s="63" t="s">
-        <v>861</v>
+        <v>856</v>
       </c>
       <c r="X4" s="23" t="s">
         <v>85</v>
@@ -5207,7 +5192,7 @@
       <c r="T5" s="23"/>
       <c r="U5" s="23"/>
       <c r="V5" s="62" t="s">
-        <v>827</v>
+        <v>822</v>
       </c>
       <c r="W5" s="62" t="s">
         <v>130</v>
@@ -5317,7 +5302,7 @@
         <v>85</v>
       </c>
       <c r="V6" s="62" t="s">
-        <v>828</v>
+        <v>823</v>
       </c>
       <c r="W6" s="62" t="s">
         <v>142</v>
@@ -5441,10 +5426,10 @@
         <v>162</v>
       </c>
       <c r="V7" s="62" t="s">
-        <v>829</v>
+        <v>824</v>
       </c>
       <c r="W7" s="62" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
       <c r="X7" s="23" t="s">
         <v>161</v>
@@ -5577,10 +5562,10 @@
         <v>85</v>
       </c>
       <c r="V8" s="26" t="s">
-        <v>830</v>
+        <v>825</v>
       </c>
       <c r="W8" s="26" t="s">
-        <v>863</v>
+        <v>858</v>
       </c>
       <c r="X8" s="26" t="s">
         <v>85</v>
@@ -5708,7 +5693,7 @@
         <v>197</v>
       </c>
       <c r="W9" s="26" t="s">
-        <v>864</v>
+        <v>859</v>
       </c>
       <c r="X9" s="23"/>
       <c r="Y9" s="23"/>
@@ -5825,7 +5810,7 @@
       <c r="T10" s="23"/>
       <c r="U10" s="23"/>
       <c r="V10" s="26" t="s">
-        <v>831</v>
+        <v>826</v>
       </c>
       <c r="W10" s="26" t="s">
         <v>214</v>
@@ -5941,7 +5926,7 @@
       <c r="T11" s="23"/>
       <c r="U11" s="23"/>
       <c r="V11" s="62" t="s">
-        <v>832</v>
+        <v>827</v>
       </c>
       <c r="W11" s="62" t="s">
         <v>227</v>
@@ -6453,10 +6438,10 @@
         <v>299</v>
       </c>
       <c r="V15" s="63" t="s">
-        <v>833</v>
+        <v>828</v>
       </c>
       <c r="W15" s="63" t="s">
-        <v>865</v>
+        <v>860</v>
       </c>
       <c r="X15" s="23" t="s">
         <v>300</v>
@@ -6593,7 +6578,7 @@
         <v>85</v>
       </c>
       <c r="V16" s="63" t="s">
-        <v>834</v>
+        <v>829</v>
       </c>
       <c r="W16" s="63" t="s">
         <v>317</v>
@@ -6843,7 +6828,7 @@
         <v>85</v>
       </c>
       <c r="V18" s="62" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="W18" s="62" t="s">
         <v>347</v>
@@ -7093,10 +7078,10 @@
       <c r="T20" s="23"/>
       <c r="U20" s="23"/>
       <c r="V20" s="26" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
       <c r="W20" s="26" t="s">
-        <v>866</v>
+        <v>861</v>
       </c>
       <c r="X20" s="23"/>
       <c r="Y20" s="23"/>
@@ -7221,10 +7206,10 @@
       <c r="T21" s="24"/>
       <c r="U21" s="24"/>
       <c r="V21" s="63" t="s">
-        <v>837</v>
+        <v>832</v>
       </c>
       <c r="W21" s="63" t="s">
-        <v>867</v>
+        <v>862</v>
       </c>
       <c r="X21" s="24"/>
       <c r="Y21" s="24"/>
@@ -7335,7 +7320,7 @@
       <c r="T22" s="45"/>
       <c r="U22" s="45"/>
       <c r="V22" s="64" t="s">
-        <v>838</v>
+        <v>833</v>
       </c>
       <c r="W22" s="64" t="s">
         <v>419</v>
@@ -7445,7 +7430,7 @@
         <v>85</v>
       </c>
       <c r="V23" s="65" t="s">
-        <v>839</v>
+        <v>834</v>
       </c>
       <c r="W23" s="65" t="s">
         <v>428</v>
@@ -7567,10 +7552,10 @@
         <v>85</v>
       </c>
       <c r="V24" s="65" t="s">
-        <v>840</v>
+        <v>835</v>
       </c>
       <c r="W24" s="65" t="s">
-        <v>868</v>
+        <v>863</v>
       </c>
       <c r="X24" s="50"/>
       <c r="Y24" s="50"/>
@@ -7693,7 +7678,7 @@
         <v>85</v>
       </c>
       <c r="V25" s="65" t="s">
-        <v>841</v>
+        <v>836</v>
       </c>
       <c r="W25" s="65" t="s">
         <v>470</v>
@@ -7821,7 +7806,7 @@
         <v>85</v>
       </c>
       <c r="V26" s="65" t="s">
-        <v>842</v>
+        <v>837</v>
       </c>
       <c r="W26" s="65" t="s">
         <v>487</v>
@@ -7939,7 +7924,7 @@
         <v>85</v>
       </c>
       <c r="V27" s="64" t="s">
-        <v>843</v>
+        <v>838</v>
       </c>
       <c r="W27" s="64" t="s">
         <v>493</v>
@@ -8051,7 +8036,7 @@
         <v>85</v>
       </c>
       <c r="V28" s="51" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
       <c r="W28" s="51" t="s">
         <v>506</v>
@@ -8419,7 +8404,7 @@
       <c r="T32" s="55"/>
       <c r="U32" s="55"/>
       <c r="V32" s="66" t="s">
-        <v>845</v>
+        <v>840</v>
       </c>
       <c r="W32" s="66" t="s">
         <v>535</v>
@@ -8665,7 +8650,7 @@
       <c r="T35" s="55"/>
       <c r="U35" s="55"/>
       <c r="V35" s="66" t="s">
-        <v>846</v>
+        <v>841</v>
       </c>
       <c r="W35" s="66" t="s">
         <v>547</v>
@@ -8773,10 +8758,10 @@
         <v>85</v>
       </c>
       <c r="V36" s="66" t="s">
-        <v>847</v>
+        <v>842</v>
       </c>
       <c r="W36" s="66" t="s">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="X36" s="55" t="s">
         <v>85</v>
@@ -9077,7 +9062,7 @@
         <v>85</v>
       </c>
       <c r="V39" s="66" t="s">
-        <v>848</v>
+        <v>843</v>
       </c>
       <c r="W39" s="66" t="s">
         <v>578</v>
@@ -9417,7 +9402,7 @@
         <v>85</v>
       </c>
       <c r="V42" s="66" t="s">
-        <v>849</v>
+        <v>844</v>
       </c>
       <c r="W42" s="66" t="s">
         <v>604</v>
@@ -9525,7 +9510,7 @@
         <v>85</v>
       </c>
       <c r="V43" s="66" t="s">
-        <v>850</v>
+        <v>845</v>
       </c>
       <c r="W43" s="66" t="s">
         <v>613</v>
@@ -9916,25 +9901,29 @@
     </row>
     <row r="48" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="54" t="s">
-        <v>636</v>
-      </c>
-      <c r="B48" s="55"/>
+        <v>637</v>
+      </c>
+      <c r="B48" s="55" t="s">
+        <v>638</v>
+      </c>
       <c r="C48" s="55" t="s">
-        <v>637</v>
+        <v>639</v>
       </c>
       <c r="D48" s="55"/>
       <c r="E48" s="55" t="s">
-        <v>144</v>
+        <v>640</v>
       </c>
       <c r="F48" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="G48" s="55"/>
+        <v>120</v>
+      </c>
+      <c r="G48" s="55" t="s">
+        <v>641</v>
+      </c>
       <c r="H48" s="55">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="I48" s="55" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="J48" s="55" t="s">
         <v>83</v>
@@ -9942,41 +9931,61 @@
       <c r="K48" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L48" s="56"/>
+      <c r="L48" s="56">
+        <v>3490</v>
+      </c>
       <c r="M48" s="56">
-        <v>36581668</v>
+        <v>25539814</v>
       </c>
       <c r="N48" s="56">
         <v>1</v>
       </c>
       <c r="O48" s="56">
-        <v>2740</v>
-      </c>
-      <c r="P48" s="56"/>
-      <c r="Q48" s="56"/>
+        <v>3490</v>
+      </c>
+      <c r="P48" s="56">
+        <v>430</v>
+      </c>
+      <c r="Q48" s="58">
+        <v>33700</v>
+      </c>
       <c r="R48" s="55"/>
       <c r="S48" s="55"/>
-      <c r="T48" s="55"/>
-      <c r="U48" s="55"/>
-      <c r="V48" s="66"/>
-      <c r="W48" s="66"/>
-      <c r="X48" s="55"/>
-      <c r="Y48" s="55"/>
-      <c r="Z48" s="55" t="s">
+      <c r="T48" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="U48" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="V48" s="66" t="s">
+        <v>846</v>
+      </c>
+      <c r="W48" s="66" t="s">
+        <v>638</v>
+      </c>
+      <c r="X48" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y48" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z48" s="55"/>
+      <c r="AA48" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="AA48" s="55"/>
       <c r="AB48" s="55" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="AC48" s="55" t="s">
-        <v>640</v>
-      </c>
-      <c r="AD48" s="55"/>
+        <v>638</v>
+      </c>
+      <c r="AD48" s="55" t="s">
+        <v>644</v>
+      </c>
       <c r="AE48" s="55"/>
       <c r="AF48" s="55"/>
       <c r="AG48" s="55" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="AH48" s="55"/>
       <c r="AI48" s="55"/>
@@ -9994,37 +10003,33 @@
       <c r="AU48" s="55"/>
       <c r="AV48" s="55"/>
       <c r="AW48" s="55"/>
-      <c r="AX48" s="56"/>
+      <c r="AX48" s="56" t="s">
+        <v>645</v>
+      </c>
       <c r="AY48" s="55" t="s">
-        <v>641</v>
+        <v>504</v>
       </c>
       <c r="AZ48" s="57"/>
     </row>
     <row r="49" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="54" t="s">
-        <v>642</v>
-      </c>
-      <c r="B49" s="55" t="s">
-        <v>643</v>
-      </c>
-      <c r="C49" s="55" t="s">
-        <v>644</v>
-      </c>
+        <v>646</v>
+      </c>
+      <c r="B49" s="55"/>
+      <c r="C49" s="55"/>
       <c r="D49" s="55"/>
       <c r="E49" s="55" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="F49" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="G49" s="55" t="s">
-        <v>646</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="G49" s="55"/>
       <c r="H49" s="55">
-        <v>603</v>
+        <v>802</v>
       </c>
       <c r="I49" s="55" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="J49" s="55" t="s">
         <v>83</v>
@@ -10032,61 +10037,41 @@
       <c r="K49" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L49" s="56">
-        <v>3490</v>
-      </c>
+      <c r="L49" s="56"/>
       <c r="M49" s="56">
-        <v>25539814</v>
+        <v>36581707</v>
       </c>
       <c r="N49" s="56">
         <v>1</v>
       </c>
       <c r="O49" s="56">
-        <v>3490</v>
-      </c>
-      <c r="P49" s="56">
-        <v>430</v>
-      </c>
-      <c r="Q49" s="58">
-        <v>33700</v>
-      </c>
+        <v>4107</v>
+      </c>
+      <c r="P49" s="56"/>
+      <c r="Q49" s="56"/>
       <c r="R49" s="55"/>
       <c r="S49" s="55"/>
-      <c r="T49" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="U49" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="V49" s="66" t="s">
-        <v>851</v>
-      </c>
-      <c r="W49" s="66" t="s">
-        <v>643</v>
-      </c>
-      <c r="X49" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y49" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Z49" s="55"/>
-      <c r="AA49" s="55" t="s">
-        <v>19</v>
-      </c>
+      <c r="T49" s="55"/>
+      <c r="U49" s="55"/>
+      <c r="V49" s="66"/>
+      <c r="W49" s="66"/>
+      <c r="X49" s="55"/>
+      <c r="Y49" s="55"/>
+      <c r="Z49" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA49" s="55"/>
       <c r="AB49" s="55" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="AC49" s="55" t="s">
-        <v>643</v>
-      </c>
-      <c r="AD49" s="55" t="s">
-        <v>649</v>
-      </c>
+        <v>650</v>
+      </c>
+      <c r="AD49" s="55"/>
       <c r="AE49" s="55"/>
       <c r="AF49" s="55"/>
       <c r="AG49" s="55" t="s">
-        <v>642</v>
+        <v>646</v>
       </c>
       <c r="AH49" s="55"/>
       <c r="AI49" s="55"/>
@@ -10104,12 +10089,8 @@
       <c r="AU49" s="55"/>
       <c r="AV49" s="55"/>
       <c r="AW49" s="55"/>
-      <c r="AX49" s="56" t="s">
-        <v>650</v>
-      </c>
-      <c r="AY49" s="55" t="s">
-        <v>504</v>
-      </c>
+      <c r="AX49" s="56"/>
+      <c r="AY49" s="55"/>
       <c r="AZ49" s="57"/>
     </row>
     <row r="50" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -10117,20 +10098,22 @@
         <v>651</v>
       </c>
       <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
+      <c r="C50" s="55" t="s">
+        <v>652</v>
+      </c>
       <c r="D50" s="55"/>
       <c r="E50" s="55" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="F50" s="55" t="s">
-        <v>210</v>
+        <v>80</v>
       </c>
       <c r="G50" s="55"/>
       <c r="H50" s="55">
-        <v>802</v>
+        <v>978</v>
       </c>
       <c r="I50" s="55" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="J50" s="55" t="s">
         <v>83</v>
@@ -10140,13 +10123,13 @@
       </c>
       <c r="L50" s="56"/>
       <c r="M50" s="56">
-        <v>36581707</v>
+        <v>36581712</v>
       </c>
       <c r="N50" s="56">
         <v>1</v>
       </c>
       <c r="O50" s="56">
-        <v>4107</v>
+        <v>4219</v>
       </c>
       <c r="P50" s="56"/>
       <c r="Q50" s="56"/>
@@ -10159,14 +10142,14 @@
       <c r="X50" s="55"/>
       <c r="Y50" s="55"/>
       <c r="Z50" s="55" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="AA50" s="55"/>
       <c r="AB50" s="55" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="AC50" s="55" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="AD50" s="55"/>
       <c r="AE50" s="55"/>
@@ -10190,31 +10173,37 @@
       <c r="AU50" s="55"/>
       <c r="AV50" s="55"/>
       <c r="AW50" s="55"/>
-      <c r="AX50" s="56"/>
-      <c r="AY50" s="55"/>
+      <c r="AX50" s="56" t="s">
+        <v>657</v>
+      </c>
+      <c r="AY50" s="55" t="s">
+        <v>658</v>
+      </c>
       <c r="AZ50" s="57"/>
     </row>
     <row r="51" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="54" t="s">
-        <v>656</v>
-      </c>
-      <c r="B51" s="55"/>
+        <v>659</v>
+      </c>
+      <c r="B51" s="55" t="s">
+        <v>660</v>
+      </c>
       <c r="C51" s="55" t="s">
-        <v>657</v>
+        <v>661</v>
       </c>
       <c r="D51" s="55"/>
       <c r="E51" s="55" t="s">
-        <v>658</v>
+        <v>662</v>
       </c>
       <c r="F51" s="55" t="s">
-        <v>80</v>
+        <v>210</v>
       </c>
       <c r="G51" s="55"/>
       <c r="H51" s="55">
-        <v>978</v>
-      </c>
-      <c r="I51" s="55" t="s">
-        <v>659</v>
+        <v>802</v>
+      </c>
+      <c r="I51" s="55">
+        <v>5753</v>
       </c>
       <c r="J51" s="55" t="s">
         <v>83</v>
@@ -10224,13 +10213,13 @@
       </c>
       <c r="L51" s="56"/>
       <c r="M51" s="56">
-        <v>36581712</v>
+        <v>36581713</v>
       </c>
       <c r="N51" s="56">
         <v>1</v>
       </c>
       <c r="O51" s="56">
-        <v>4219</v>
+        <v>4283</v>
       </c>
       <c r="P51" s="56"/>
       <c r="Q51" s="56"/>
@@ -10243,20 +10232,20 @@
       <c r="X51" s="55"/>
       <c r="Y51" s="55"/>
       <c r="Z51" s="55" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="AA51" s="55"/>
       <c r="AB51" s="55" t="s">
+        <v>663</v>
+      </c>
+      <c r="AC51" s="55" t="s">
         <v>660</v>
-      </c>
-      <c r="AC51" s="55" t="s">
-        <v>661</v>
       </c>
       <c r="AD51" s="55"/>
       <c r="AE51" s="55"/>
       <c r="AF51" s="55"/>
       <c r="AG51" s="55" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="AH51" s="55"/>
       <c r="AI51" s="55"/>
@@ -10274,12 +10263,8 @@
       <c r="AU51" s="55"/>
       <c r="AV51" s="55"/>
       <c r="AW51" s="55"/>
-      <c r="AX51" s="56" t="s">
-        <v>662</v>
-      </c>
-      <c r="AY51" s="55" t="s">
-        <v>663</v>
-      </c>
+      <c r="AX51" s="56"/>
+      <c r="AY51" s="55"/>
       <c r="AZ51" s="57"/>
     </row>
     <row r="52" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -10294,17 +10279,19 @@
       </c>
       <c r="D52" s="55"/>
       <c r="E52" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F52" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="G52" s="55" t="s">
         <v>667</v>
       </c>
-      <c r="F52" s="55" t="s">
-        <v>210</v>
-      </c>
-      <c r="G52" s="55"/>
       <c r="H52" s="55">
-        <v>802</v>
-      </c>
-      <c r="I52" s="55">
-        <v>5753</v>
+        <v>617</v>
+      </c>
+      <c r="I52" s="55" t="s">
+        <v>668</v>
       </c>
       <c r="J52" s="55" t="s">
         <v>83</v>
@@ -10312,38 +10299,64 @@
       <c r="K52" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L52" s="56"/>
+      <c r="L52" s="56">
+        <v>4935</v>
+      </c>
       <c r="M52" s="56">
-        <v>36581713</v>
+        <v>25539869</v>
       </c>
       <c r="N52" s="56">
         <v>1</v>
       </c>
       <c r="O52" s="56">
-        <v>4283</v>
-      </c>
-      <c r="P52" s="56"/>
-      <c r="Q52" s="56"/>
-      <c r="R52" s="55"/>
-      <c r="S52" s="55"/>
-      <c r="T52" s="55"/>
-      <c r="U52" s="55"/>
-      <c r="V52" s="66"/>
-      <c r="W52" s="66"/>
-      <c r="X52" s="55"/>
-      <c r="Y52" s="55"/>
+        <v>4935</v>
+      </c>
+      <c r="P52" s="56">
+        <v>412</v>
+      </c>
+      <c r="Q52" s="58">
+        <v>31565</v>
+      </c>
+      <c r="R52" s="55" t="s">
+        <v>669</v>
+      </c>
+      <c r="S52" s="55" t="s">
+        <v>665</v>
+      </c>
+      <c r="T52" s="55" t="s">
+        <v>669</v>
+      </c>
+      <c r="U52" s="55" t="s">
+        <v>670</v>
+      </c>
+      <c r="V52" s="66" t="s">
+        <v>669</v>
+      </c>
+      <c r="W52" s="66" t="s">
+        <v>665</v>
+      </c>
+      <c r="X52" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y52" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="Z52" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA52" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="AA52" s="55" t="s">
+        <v>19</v>
+      </c>
       <c r="AB52" s="55" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="AC52" s="55" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
       <c r="AD52" s="55"/>
-      <c r="AE52" s="55"/>
+      <c r="AE52" s="55" t="s">
+        <v>673</v>
+      </c>
       <c r="AF52" s="55"/>
       <c r="AG52" s="55" t="s">
         <v>664</v>
@@ -10358,41 +10371,47 @@
       <c r="AO52" s="55"/>
       <c r="AP52" s="55"/>
       <c r="AQ52" s="55"/>
-      <c r="AR52" s="55"/>
+      <c r="AR52" s="59">
+        <v>85.404166666666669</v>
+      </c>
       <c r="AS52" s="55"/>
-      <c r="AT52" s="55"/>
+      <c r="AT52" s="55" t="s">
+        <v>545</v>
+      </c>
       <c r="AU52" s="55"/>
       <c r="AV52" s="55"/>
       <c r="AW52" s="55"/>
-      <c r="AX52" s="56"/>
+      <c r="AX52" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="AY52" s="55"/>
       <c r="AZ52" s="57"/>
     </row>
     <row r="53" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="54" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="B53" s="55" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="C53" s="55" t="s">
-        <v>671</v>
+        <v>676</v>
       </c>
       <c r="D53" s="55"/>
       <c r="E53" s="55" t="s">
-        <v>244</v>
+        <v>677</v>
       </c>
       <c r="F53" s="55" t="s">
-        <v>80</v>
+        <v>210</v>
       </c>
       <c r="G53" s="55" t="s">
-        <v>672</v>
+        <v>678</v>
       </c>
       <c r="H53" s="55">
-        <v>617</v>
+        <v>802</v>
       </c>
       <c r="I53" s="55" t="s">
-        <v>673</v>
+        <v>679</v>
       </c>
       <c r="J53" s="55" t="s">
         <v>83</v>
@@ -10400,71 +10419,51 @@
       <c r="K53" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L53" s="56">
-        <v>4935</v>
-      </c>
+      <c r="L53" s="56"/>
       <c r="M53" s="56">
-        <v>25539869</v>
+        <v>36581740</v>
       </c>
       <c r="N53" s="56">
         <v>1</v>
       </c>
       <c r="O53" s="56">
-        <v>4935</v>
-      </c>
-      <c r="P53" s="56">
-        <v>412</v>
-      </c>
-      <c r="Q53" s="58">
-        <v>31565</v>
-      </c>
-      <c r="R53" s="55" t="s">
-        <v>674</v>
-      </c>
-      <c r="S53" s="55" t="s">
-        <v>670</v>
-      </c>
-      <c r="T53" s="55" t="s">
-        <v>674</v>
-      </c>
-      <c r="U53" s="55" t="s">
+        <v>5008</v>
+      </c>
+      <c r="P53" s="56"/>
+      <c r="Q53" s="56"/>
+      <c r="R53" s="55"/>
+      <c r="S53" s="55"/>
+      <c r="T53" s="55"/>
+      <c r="U53" s="55"/>
+      <c r="V53" s="66" t="s">
+        <v>847</v>
+      </c>
+      <c r="W53" s="66" t="s">
         <v>675</v>
       </c>
-      <c r="V53" s="66" t="s">
-        <v>674</v>
-      </c>
-      <c r="W53" s="66" t="s">
-        <v>670</v>
-      </c>
-      <c r="X53" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y53" s="55" t="s">
-        <v>85</v>
-      </c>
+      <c r="X53" s="55"/>
+      <c r="Y53" s="55"/>
       <c r="Z53" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA53" s="55" t="s">
-        <v>19</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="AA53" s="55"/>
       <c r="AB53" s="55" t="s">
-        <v>676</v>
+        <v>680</v>
       </c>
       <c r="AC53" s="55" t="s">
-        <v>677</v>
+        <v>681</v>
       </c>
       <c r="AD53" s="55"/>
-      <c r="AE53" s="55" t="s">
-        <v>678</v>
-      </c>
+      <c r="AE53" s="55"/>
       <c r="AF53" s="55"/>
       <c r="AG53" s="55" t="s">
-        <v>669</v>
+        <v>674</v>
       </c>
       <c r="AH53" s="55"/>
       <c r="AI53" s="55"/>
-      <c r="AJ53" s="55"/>
+      <c r="AJ53" s="55" t="s">
+        <v>682</v>
+      </c>
       <c r="AK53" s="55"/>
       <c r="AL53" s="55"/>
       <c r="AM53" s="55"/>
@@ -10472,48 +10471,32 @@
       <c r="AO53" s="55"/>
       <c r="AP53" s="55"/>
       <c r="AQ53" s="55"/>
-      <c r="AR53" s="59">
-        <v>85.404166666666669</v>
-      </c>
+      <c r="AR53" s="55"/>
       <c r="AS53" s="55"/>
-      <c r="AT53" s="55" t="s">
-        <v>545</v>
-      </c>
+      <c r="AT53" s="55"/>
       <c r="AU53" s="55"/>
       <c r="AV53" s="55"/>
       <c r="AW53" s="55"/>
       <c r="AX53" s="56" t="s">
-        <v>97</v>
+        <v>416</v>
       </c>
       <c r="AY53" s="55"/>
       <c r="AZ53" s="57"/>
     </row>
     <row r="54" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="54" t="s">
-        <v>679</v>
-      </c>
-      <c r="B54" s="55" t="s">
-        <v>680</v>
-      </c>
-      <c r="C54" s="55" t="s">
-        <v>681</v>
-      </c>
+        <v>683</v>
+      </c>
+      <c r="B54" s="55"/>
+      <c r="C54" s="55"/>
       <c r="D54" s="55"/>
-      <c r="E54" s="55" t="s">
-        <v>682</v>
-      </c>
-      <c r="F54" s="55" t="s">
-        <v>210</v>
-      </c>
-      <c r="G54" s="55" t="s">
-        <v>683</v>
-      </c>
+      <c r="E54" s="55"/>
+      <c r="F54" s="55"/>
+      <c r="G54" s="55"/>
       <c r="H54" s="55">
-        <v>802</v>
-      </c>
-      <c r="I54" s="55" t="s">
-        <v>684</v>
-      </c>
+        <v>518</v>
+      </c>
+      <c r="I54" s="55"/>
       <c r="J54" s="55" t="s">
         <v>83</v>
       </c>
@@ -10522,13 +10505,13 @@
       </c>
       <c r="L54" s="56"/>
       <c r="M54" s="56">
-        <v>36581740</v>
+        <v>36581764</v>
       </c>
       <c r="N54" s="56">
         <v>1</v>
       </c>
       <c r="O54" s="56">
-        <v>5008</v>
+        <v>5930</v>
       </c>
       <c r="P54" s="56"/>
       <c r="Q54" s="56"/>
@@ -10536,35 +10519,25 @@
       <c r="S54" s="55"/>
       <c r="T54" s="55"/>
       <c r="U54" s="55"/>
-      <c r="V54" s="66" t="s">
-        <v>852</v>
-      </c>
-      <c r="W54" s="66" t="s">
-        <v>680</v>
-      </c>
+      <c r="V54" s="66"/>
+      <c r="W54" s="66"/>
       <c r="X54" s="55"/>
       <c r="Y54" s="55"/>
       <c r="Z54" s="55" t="s">
         <v>124</v>
       </c>
       <c r="AA54" s="55"/>
-      <c r="AB54" s="55" t="s">
-        <v>685</v>
-      </c>
-      <c r="AC54" s="55" t="s">
-        <v>686</v>
-      </c>
+      <c r="AB54" s="55"/>
+      <c r="AC54" s="55"/>
       <c r="AD54" s="55"/>
       <c r="AE54" s="55"/>
       <c r="AF54" s="55"/>
       <c r="AG54" s="55" t="s">
-        <v>679</v>
+        <v>683</v>
       </c>
       <c r="AH54" s="55"/>
       <c r="AI54" s="55"/>
-      <c r="AJ54" s="55" t="s">
-        <v>687</v>
-      </c>
+      <c r="AJ54" s="55"/>
       <c r="AK54" s="55"/>
       <c r="AL54" s="55"/>
       <c r="AM54" s="55"/>
@@ -10578,63 +10551,93 @@
       <c r="AU54" s="55"/>
       <c r="AV54" s="55"/>
       <c r="AW54" s="55"/>
-      <c r="AX54" s="56" t="s">
-        <v>416</v>
-      </c>
+      <c r="AX54" s="56"/>
       <c r="AY54" s="55"/>
       <c r="AZ54" s="57"/>
     </row>
     <row r="55" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="54" t="s">
-        <v>688</v>
-      </c>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
+        <v>684</v>
+      </c>
+      <c r="B55" s="55" t="s">
+        <v>685</v>
+      </c>
+      <c r="C55" s="55" t="s">
+        <v>686</v>
+      </c>
       <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="55"/>
+      <c r="E55" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F55" s="55" t="s">
+        <v>80</v>
+      </c>
       <c r="G55" s="55"/>
       <c r="H55" s="55">
-        <v>518</v>
-      </c>
-      <c r="I55" s="55"/>
+        <v>617</v>
+      </c>
+      <c r="I55" s="55" t="s">
+        <v>687</v>
+      </c>
       <c r="J55" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K55" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L55" s="56"/>
+      <c r="L55" s="56">
+        <v>6442</v>
+      </c>
       <c r="M55" s="56">
-        <v>36581764</v>
+        <v>26089251</v>
       </c>
       <c r="N55" s="56">
         <v>1</v>
       </c>
       <c r="O55" s="56">
-        <v>5930</v>
+        <v>6442</v>
       </c>
       <c r="P55" s="56"/>
       <c r="Q55" s="56"/>
       <c r="R55" s="55"/>
       <c r="S55" s="55"/>
-      <c r="T55" s="55"/>
-      <c r="U55" s="55"/>
-      <c r="V55" s="66"/>
-      <c r="W55" s="66"/>
-      <c r="X55" s="55"/>
-      <c r="Y55" s="55"/>
+      <c r="T55" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="U55" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="V55" s="66" t="s">
+        <v>848</v>
+      </c>
+      <c r="W55" s="66" t="s">
+        <v>685</v>
+      </c>
+      <c r="X55" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y55" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="Z55" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="AA55" s="55"/>
-      <c r="AB55" s="55"/>
-      <c r="AC55" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="AA55" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB55" s="55" t="s">
+        <v>688</v>
+      </c>
+      <c r="AC55" s="55" t="s">
+        <v>689</v>
+      </c>
       <c r="AD55" s="55"/>
-      <c r="AE55" s="55"/>
+      <c r="AE55" s="55" t="s">
+        <v>690</v>
+      </c>
       <c r="AF55" s="55"/>
       <c r="AG55" s="55" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="AH55" s="55"/>
       <c r="AI55" s="55"/>
@@ -10653,92 +10656,62 @@
       <c r="AV55" s="55"/>
       <c r="AW55" s="55"/>
       <c r="AX55" s="56"/>
-      <c r="AY55" s="55"/>
+      <c r="AY55" s="55" t="s">
+        <v>691</v>
+      </c>
       <c r="AZ55" s="57"/>
     </row>
     <row r="56" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="54" t="s">
-        <v>689</v>
-      </c>
-      <c r="B56" s="55" t="s">
-        <v>690</v>
-      </c>
-      <c r="C56" s="55" t="s">
-        <v>691</v>
-      </c>
+        <v>692</v>
+      </c>
+      <c r="B56" s="55"/>
+      <c r="C56" s="55"/>
       <c r="D56" s="55"/>
-      <c r="E56" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="F56" s="55" t="s">
-        <v>80</v>
-      </c>
+      <c r="E56" s="55"/>
+      <c r="F56" s="55"/>
       <c r="G56" s="55"/>
       <c r="H56" s="55">
-        <v>617</v>
-      </c>
-      <c r="I56" s="55" t="s">
-        <v>692</v>
-      </c>
+        <v>508</v>
+      </c>
+      <c r="I56" s="55"/>
       <c r="J56" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K56" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L56" s="56">
-        <v>6442</v>
-      </c>
+      <c r="L56" s="56"/>
       <c r="M56" s="56">
-        <v>26089251</v>
+        <v>36581786</v>
       </c>
       <c r="N56" s="56">
         <v>1</v>
       </c>
       <c r="O56" s="56">
-        <v>6442</v>
+        <v>6562</v>
       </c>
       <c r="P56" s="56"/>
       <c r="Q56" s="56"/>
       <c r="R56" s="55"/>
       <c r="S56" s="55"/>
-      <c r="T56" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="U56" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="V56" s="66" t="s">
-        <v>853</v>
-      </c>
-      <c r="W56" s="66" t="s">
-        <v>690</v>
-      </c>
-      <c r="X56" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y56" s="55" t="s">
-        <v>85</v>
-      </c>
+      <c r="T56" s="55"/>
+      <c r="U56" s="55"/>
+      <c r="V56" s="66"/>
+      <c r="W56" s="66"/>
+      <c r="X56" s="55"/>
+      <c r="Y56" s="55"/>
       <c r="Z56" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA56" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB56" s="55" t="s">
-        <v>693</v>
-      </c>
-      <c r="AC56" s="55" t="s">
-        <v>694</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="AA56" s="55"/>
+      <c r="AB56" s="55"/>
+      <c r="AC56" s="55"/>
       <c r="AD56" s="55"/>
-      <c r="AE56" s="55" t="s">
-        <v>695</v>
-      </c>
+      <c r="AE56" s="55"/>
       <c r="AF56" s="55"/>
       <c r="AG56" s="55" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="AH56" s="55"/>
       <c r="AI56" s="55"/>
@@ -10758,61 +10731,95 @@
       <c r="AW56" s="55"/>
       <c r="AX56" s="56"/>
       <c r="AY56" s="55" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="AZ56" s="57"/>
     </row>
     <row r="57" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="54" t="s">
-        <v>697</v>
-      </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
+        <v>694</v>
+      </c>
+      <c r="B57" s="55" t="s">
+        <v>695</v>
+      </c>
+      <c r="C57" s="55" t="s">
+        <v>696</v>
+      </c>
       <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
+      <c r="E57" s="55" t="s">
+        <v>403</v>
+      </c>
+      <c r="F57" s="55" t="s">
+        <v>133</v>
+      </c>
       <c r="G57" s="55"/>
       <c r="H57" s="55">
-        <v>508</v>
-      </c>
-      <c r="I57" s="55"/>
+        <v>203</v>
+      </c>
+      <c r="I57" s="55" t="s">
+        <v>697</v>
+      </c>
       <c r="J57" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K57" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L57" s="56"/>
+      <c r="L57" s="56">
+        <v>6586</v>
+      </c>
       <c r="M57" s="56">
-        <v>36581786</v>
+        <v>26089256</v>
       </c>
       <c r="N57" s="56">
         <v>1</v>
       </c>
       <c r="O57" s="56">
-        <v>6562</v>
+        <v>6586</v>
       </c>
       <c r="P57" s="56"/>
       <c r="Q57" s="56"/>
-      <c r="R57" s="55"/>
-      <c r="S57" s="55"/>
-      <c r="T57" s="55"/>
-      <c r="U57" s="55"/>
-      <c r="V57" s="66"/>
-      <c r="W57" s="66"/>
-      <c r="X57" s="55"/>
-      <c r="Y57" s="55"/>
+      <c r="R57" s="55" t="s">
+        <v>698</v>
+      </c>
+      <c r="S57" s="55" t="s">
+        <v>695</v>
+      </c>
+      <c r="T57" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="U57" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="V57" s="66" t="s">
+        <v>698</v>
+      </c>
+      <c r="W57" s="66" t="s">
+        <v>695</v>
+      </c>
+      <c r="X57" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y57" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="Z57" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="AA57" s="55"/>
-      <c r="AB57" s="55"/>
-      <c r="AC57" s="55"/>
+      <c r="AA57" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB57" s="55" t="s">
+        <v>698</v>
+      </c>
+      <c r="AC57" s="55" t="s">
+        <v>695</v>
+      </c>
       <c r="AD57" s="55"/>
       <c r="AE57" s="55"/>
       <c r="AF57" s="55"/>
       <c r="AG57" s="55" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="AH57" s="55"/>
       <c r="AI57" s="55"/>
@@ -10824,41 +10831,45 @@
       <c r="AO57" s="55"/>
       <c r="AP57" s="55"/>
       <c r="AQ57" s="55"/>
-      <c r="AR57" s="55"/>
+      <c r="AR57" s="55" t="s">
+        <v>699</v>
+      </c>
       <c r="AS57" s="55"/>
       <c r="AT57" s="55"/>
       <c r="AU57" s="55"/>
       <c r="AV57" s="55"/>
       <c r="AW57" s="55"/>
-      <c r="AX57" s="56"/>
-      <c r="AY57" s="55" t="s">
-        <v>698</v>
-      </c>
+      <c r="AX57" s="56" t="s">
+        <v>416</v>
+      </c>
+      <c r="AY57" s="55"/>
       <c r="AZ57" s="57"/>
     </row>
     <row r="58" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="54" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B58" s="55" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C58" s="55" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="D58" s="55"/>
       <c r="E58" s="55" t="s">
-        <v>403</v>
+        <v>703</v>
       </c>
       <c r="F58" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="G58" s="55"/>
+        <v>704</v>
+      </c>
+      <c r="G58" s="55" t="s">
+        <v>705</v>
+      </c>
       <c r="H58" s="55">
-        <v>203</v>
+        <v>301</v>
       </c>
       <c r="I58" s="55" t="s">
-        <v>702</v>
+        <v>706</v>
       </c>
       <c r="J58" s="55" t="s">
         <v>83</v>
@@ -10867,43 +10878,37 @@
         <v>83</v>
       </c>
       <c r="L58" s="56">
-        <v>6586</v>
+        <v>0</v>
       </c>
       <c r="M58" s="56">
-        <v>26089256</v>
+        <v>26173198</v>
       </c>
       <c r="N58" s="56">
         <v>1</v>
       </c>
       <c r="O58" s="56">
-        <v>6586</v>
-      </c>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="56"/>
+        <v>0</v>
+      </c>
+      <c r="P58" s="56">
+        <v>0</v>
+      </c>
+      <c r="Q58" s="58">
+        <v>41760</v>
+      </c>
       <c r="R58" s="55" t="s">
-        <v>703</v>
-      </c>
-      <c r="S58" s="55" t="s">
-        <v>700</v>
-      </c>
-      <c r="T58" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="U58" s="55" t="s">
-        <v>85</v>
-      </c>
+        <v>707</v>
+      </c>
+      <c r="S58" s="55"/>
+      <c r="T58" s="55"/>
+      <c r="U58" s="55"/>
       <c r="V58" s="66" t="s">
-        <v>703</v>
+        <v>849</v>
       </c>
       <c r="W58" s="66" t="s">
-        <v>700</v>
-      </c>
-      <c r="X58" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y58" s="55" t="s">
-        <v>85</v>
-      </c>
+        <v>701</v>
+      </c>
+      <c r="X58" s="55"/>
+      <c r="Y58" s="55"/>
       <c r="Z58" s="55" t="s">
         <v>124</v>
       </c>
@@ -10911,16 +10916,18 @@
         <v>124</v>
       </c>
       <c r="AB58" s="55" t="s">
-        <v>703</v>
+        <v>708</v>
       </c>
       <c r="AC58" s="55" t="s">
-        <v>700</v>
-      </c>
-      <c r="AD58" s="55"/>
+        <v>709</v>
+      </c>
+      <c r="AD58" s="55" t="s">
+        <v>709</v>
+      </c>
       <c r="AE58" s="55"/>
       <c r="AF58" s="55"/>
       <c r="AG58" s="55" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="AH58" s="55"/>
       <c r="AI58" s="55"/>
@@ -10932,45 +10939,39 @@
       <c r="AO58" s="55"/>
       <c r="AP58" s="55"/>
       <c r="AQ58" s="55"/>
-      <c r="AR58" s="55" t="s">
-        <v>704</v>
-      </c>
+      <c r="AR58" s="55"/>
       <c r="AS58" s="55"/>
       <c r="AT58" s="55"/>
       <c r="AU58" s="55"/>
       <c r="AV58" s="55"/>
       <c r="AW58" s="55"/>
-      <c r="AX58" s="56" t="s">
-        <v>416</v>
-      </c>
+      <c r="AX58" s="56"/>
       <c r="AY58" s="55"/>
       <c r="AZ58" s="57"/>
     </row>
     <row r="59" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="54" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="B59" s="55" t="s">
-        <v>706</v>
+        <v>711</v>
       </c>
       <c r="C59" s="55" t="s">
-        <v>707</v>
+        <v>712</v>
       </c>
       <c r="D59" s="55"/>
       <c r="E59" s="55" t="s">
-        <v>708</v>
+        <v>606</v>
       </c>
       <c r="F59" s="55" t="s">
-        <v>709</v>
-      </c>
-      <c r="G59" s="55" t="s">
-        <v>710</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G59" s="55"/>
       <c r="H59" s="55">
-        <v>301</v>
+        <v>860</v>
       </c>
       <c r="I59" s="55" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="J59" s="55" t="s">
         <v>83</v>
@@ -10979,56 +10980,58 @@
         <v>83</v>
       </c>
       <c r="L59" s="56">
-        <v>0</v>
+        <v>7508</v>
       </c>
       <c r="M59" s="56">
-        <v>26173198</v>
+        <v>26089281</v>
       </c>
       <c r="N59" s="56">
         <v>1</v>
       </c>
       <c r="O59" s="56">
-        <v>0</v>
-      </c>
-      <c r="P59" s="56">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="58">
-        <v>41760</v>
-      </c>
-      <c r="R59" s="55" t="s">
-        <v>712</v>
-      </c>
+        <v>7508</v>
+      </c>
+      <c r="P59" s="56"/>
+      <c r="Q59" s="56"/>
+      <c r="R59" s="55"/>
       <c r="S59" s="55"/>
-      <c r="T59" s="55"/>
-      <c r="U59" s="55"/>
+      <c r="T59" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="U59" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="V59" s="66" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="W59" s="66" t="s">
-        <v>706</v>
-      </c>
-      <c r="X59" s="55"/>
-      <c r="Y59" s="55"/>
+        <v>711</v>
+      </c>
+      <c r="X59" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y59" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="Z59" s="55" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="AA59" s="55" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="AB59" s="55" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="AC59" s="55" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="AD59" s="55" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="AE59" s="55"/>
       <c r="AF59" s="55"/>
       <c r="AG59" s="55" t="s">
-        <v>705</v>
+        <v>710</v>
       </c>
       <c r="AH59" s="55"/>
       <c r="AI59" s="55"/>
@@ -11046,34 +11049,28 @@
       <c r="AU59" s="55"/>
       <c r="AV59" s="55"/>
       <c r="AW59" s="55"/>
-      <c r="AX59" s="56"/>
-      <c r="AY59" s="55"/>
+      <c r="AX59" s="56" t="s">
+        <v>717</v>
+      </c>
+      <c r="AY59" s="55" t="s">
+        <v>504</v>
+      </c>
       <c r="AZ59" s="57"/>
     </row>
     <row r="60" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="54" t="s">
-        <v>715</v>
-      </c>
-      <c r="B60" s="55" t="s">
-        <v>716</v>
-      </c>
-      <c r="C60" s="55" t="s">
-        <v>717</v>
-      </c>
+        <v>718</v>
+      </c>
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
       <c r="D60" s="55"/>
-      <c r="E60" s="55" t="s">
-        <v>606</v>
-      </c>
-      <c r="F60" s="55" t="s">
-        <v>133</v>
-      </c>
+      <c r="E60" s="55"/>
+      <c r="F60" s="55"/>
       <c r="G60" s="55"/>
       <c r="H60" s="55">
-        <v>860</v>
-      </c>
-      <c r="I60" s="55" t="s">
-        <v>718</v>
-      </c>
+        <v>800</v>
+      </c>
+      <c r="I60" s="55"/>
       <c r="J60" s="55" t="s">
         <v>83</v>
       </c>
@@ -11081,19 +11078,23 @@
         <v>83</v>
       </c>
       <c r="L60" s="56">
-        <v>7508</v>
+        <v>679</v>
       </c>
       <c r="M60" s="56">
-        <v>26089281</v>
+        <v>26089120</v>
       </c>
       <c r="N60" s="56">
         <v>1</v>
       </c>
       <c r="O60" s="56">
-        <v>7508</v>
-      </c>
-      <c r="P60" s="56"/>
-      <c r="Q60" s="56"/>
+        <v>679</v>
+      </c>
+      <c r="P60" s="56">
+        <v>269</v>
+      </c>
+      <c r="Q60" s="58">
+        <v>26087</v>
+      </c>
       <c r="R60" s="55"/>
       <c r="S60" s="55"/>
       <c r="T60" s="55" t="s">
@@ -11102,12 +11103,8 @@
       <c r="U60" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V60" s="66" t="s">
-        <v>855</v>
-      </c>
-      <c r="W60" s="66" t="s">
-        <v>716</v>
-      </c>
+      <c r="V60" s="66"/>
+      <c r="W60" s="66"/>
       <c r="X60" s="55" t="s">
         <v>85</v>
       </c>
@@ -11115,24 +11112,18 @@
         <v>85</v>
       </c>
       <c r="Z60" s="55" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="AA60" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB60" s="55" t="s">
-        <v>719</v>
-      </c>
-      <c r="AC60" s="55" t="s">
-        <v>720</v>
-      </c>
-      <c r="AD60" s="55" t="s">
-        <v>721</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="AB60" s="55"/>
+      <c r="AC60" s="55"/>
+      <c r="AD60" s="55"/>
       <c r="AE60" s="55"/>
       <c r="AF60" s="55"/>
       <c r="AG60" s="55" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="AH60" s="55"/>
       <c r="AI60" s="55"/>
@@ -11151,27 +11142,35 @@
       <c r="AV60" s="55"/>
       <c r="AW60" s="55"/>
       <c r="AX60" s="56" t="s">
-        <v>722</v>
-      </c>
-      <c r="AY60" s="55" t="s">
-        <v>504</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="AY60" s="55"/>
       <c r="AZ60" s="57"/>
     </row>
     <row r="61" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="54" t="s">
-        <v>723</v>
-      </c>
-      <c r="B61" s="55"/>
-      <c r="C61" s="55"/>
+        <v>719</v>
+      </c>
+      <c r="B61" s="55" t="s">
+        <v>720</v>
+      </c>
+      <c r="C61" s="55" t="s">
+        <v>721</v>
+      </c>
       <c r="D61" s="55"/>
-      <c r="E61" s="55"/>
-      <c r="F61" s="55"/>
+      <c r="E61" s="55" t="s">
+        <v>722</v>
+      </c>
+      <c r="F61" s="55" t="s">
+        <v>133</v>
+      </c>
       <c r="G61" s="55"/>
       <c r="H61" s="55">
-        <v>800</v>
-      </c>
-      <c r="I61" s="55"/>
+        <v>860</v>
+      </c>
+      <c r="I61" s="55" t="s">
+        <v>723</v>
+      </c>
       <c r="J61" s="55" t="s">
         <v>83</v>
       </c>
@@ -11179,23 +11178,19 @@
         <v>83</v>
       </c>
       <c r="L61" s="56">
-        <v>679</v>
+        <v>2690</v>
       </c>
       <c r="M61" s="56">
-        <v>26089120</v>
+        <v>26089160</v>
       </c>
       <c r="N61" s="56">
         <v>1</v>
       </c>
       <c r="O61" s="56">
-        <v>679</v>
-      </c>
-      <c r="P61" s="56">
-        <v>269</v>
-      </c>
-      <c r="Q61" s="58">
-        <v>26087</v>
-      </c>
+        <v>2690</v>
+      </c>
+      <c r="P61" s="56"/>
+      <c r="Q61" s="56"/>
       <c r="R61" s="55"/>
       <c r="S61" s="55"/>
       <c r="T61" s="55" t="s">
@@ -11204,8 +11199,12 @@
       <c r="U61" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="V61" s="66"/>
-      <c r="W61" s="66"/>
+      <c r="V61" s="66" t="s">
+        <v>851</v>
+      </c>
+      <c r="W61" s="66" t="s">
+        <v>720</v>
+      </c>
       <c r="X61" s="55" t="s">
         <v>85</v>
       </c>
@@ -11213,18 +11212,22 @@
         <v>85</v>
       </c>
       <c r="Z61" s="55" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="AA61" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB61" s="55"/>
-      <c r="AC61" s="55"/>
+        <v>19</v>
+      </c>
+      <c r="AB61" s="55" t="s">
+        <v>724</v>
+      </c>
+      <c r="AC61" s="55" t="s">
+        <v>725</v>
+      </c>
       <c r="AD61" s="55"/>
       <c r="AE61" s="55"/>
       <c r="AF61" s="55"/>
       <c r="AG61" s="55" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="AH61" s="55"/>
       <c r="AI61" s="55"/>
@@ -11243,92 +11246,64 @@
       <c r="AV61" s="55"/>
       <c r="AW61" s="55"/>
       <c r="AX61" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY61" s="55"/>
+        <v>726</v>
+      </c>
+      <c r="AY61" s="55" t="s">
+        <v>727</v>
+      </c>
       <c r="AZ61" s="57"/>
     </row>
     <row r="62" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="54" t="s">
-        <v>724</v>
-      </c>
-      <c r="B62" s="55" t="s">
-        <v>725</v>
-      </c>
-      <c r="C62" s="55" t="s">
-        <v>726</v>
-      </c>
+        <v>728</v>
+      </c>
+      <c r="B62" s="55"/>
+      <c r="C62" s="55"/>
       <c r="D62" s="55"/>
-      <c r="E62" s="55" t="s">
-        <v>727</v>
-      </c>
-      <c r="F62" s="55" t="s">
-        <v>133</v>
-      </c>
+      <c r="E62" s="55"/>
+      <c r="F62" s="55"/>
       <c r="G62" s="55"/>
       <c r="H62" s="55">
-        <v>860</v>
-      </c>
-      <c r="I62" s="55" t="s">
-        <v>728</v>
-      </c>
+        <v>978</v>
+      </c>
+      <c r="I62" s="55"/>
       <c r="J62" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K62" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L62" s="56">
-        <v>2690</v>
-      </c>
+      <c r="L62" s="56"/>
       <c r="M62" s="56">
-        <v>26089160</v>
+        <v>36581702</v>
       </c>
       <c r="N62" s="56">
         <v>1</v>
       </c>
       <c r="O62" s="56">
-        <v>2690</v>
+        <v>3894</v>
       </c>
       <c r="P62" s="56"/>
       <c r="Q62" s="56"/>
       <c r="R62" s="55"/>
       <c r="S62" s="55"/>
-      <c r="T62" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="U62" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="V62" s="66" t="s">
-        <v>856</v>
-      </c>
-      <c r="W62" s="66" t="s">
-        <v>725</v>
-      </c>
-      <c r="X62" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y62" s="55" t="s">
-        <v>85</v>
-      </c>
+      <c r="T62" s="55"/>
+      <c r="U62" s="55"/>
+      <c r="V62" s="66"/>
+      <c r="W62" s="66"/>
+      <c r="X62" s="55"/>
+      <c r="Y62" s="55"/>
       <c r="Z62" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA62" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB62" s="55" t="s">
-        <v>729</v>
-      </c>
-      <c r="AC62" s="55" t="s">
-        <v>730</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="AA62" s="55"/>
+      <c r="AB62" s="55"/>
+      <c r="AC62" s="55"/>
       <c r="AD62" s="55"/>
       <c r="AE62" s="55"/>
       <c r="AF62" s="55"/>
       <c r="AG62" s="55" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="AH62" s="55"/>
       <c r="AI62" s="55"/>
@@ -11346,65 +11321,101 @@
       <c r="AU62" s="55"/>
       <c r="AV62" s="55"/>
       <c r="AW62" s="55"/>
-      <c r="AX62" s="56" t="s">
-        <v>731</v>
-      </c>
-      <c r="AY62" s="55" t="s">
-        <v>732</v>
-      </c>
+      <c r="AX62" s="56"/>
+      <c r="AY62" s="55"/>
       <c r="AZ62" s="57"/>
     </row>
     <row r="63" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="54" t="s">
+        <v>729</v>
+      </c>
+      <c r="B63" s="55" t="s">
+        <v>730</v>
+      </c>
+      <c r="C63" s="55" t="s">
+        <v>731</v>
+      </c>
+      <c r="D63" s="55"/>
+      <c r="E63" s="55" t="s">
+        <v>732</v>
+      </c>
+      <c r="F63" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="G63" s="55" t="s">
         <v>733</v>
       </c>
-      <c r="B63" s="55"/>
-      <c r="C63" s="55"/>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
-      <c r="F63" s="55"/>
-      <c r="G63" s="55"/>
       <c r="H63" s="55">
-        <v>978</v>
-      </c>
-      <c r="I63" s="55"/>
+        <v>508</v>
+      </c>
+      <c r="I63" s="55" t="s">
+        <v>734</v>
+      </c>
       <c r="J63" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K63" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L63" s="56"/>
+      <c r="L63" s="56">
+        <v>6550</v>
+      </c>
       <c r="M63" s="56">
-        <v>36581702</v>
+        <v>25540051</v>
       </c>
       <c r="N63" s="56">
         <v>1</v>
       </c>
       <c r="O63" s="56">
-        <v>3894</v>
-      </c>
-      <c r="P63" s="56"/>
-      <c r="Q63" s="56"/>
-      <c r="R63" s="55"/>
-      <c r="S63" s="55"/>
-      <c r="T63" s="55"/>
-      <c r="U63" s="55"/>
-      <c r="V63" s="66"/>
-      <c r="W63" s="66"/>
-      <c r="X63" s="55"/>
-      <c r="Y63" s="55"/>
+        <v>6550</v>
+      </c>
+      <c r="P63" s="56">
+        <v>391</v>
+      </c>
+      <c r="Q63" s="58">
+        <v>30438</v>
+      </c>
+      <c r="R63" s="55" t="s">
+        <v>735</v>
+      </c>
+      <c r="S63" s="55" t="s">
+        <v>730</v>
+      </c>
+      <c r="T63" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="U63" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="V63" s="66" t="s">
+        <v>735</v>
+      </c>
+      <c r="W63" s="66" t="s">
+        <v>730</v>
+      </c>
+      <c r="X63" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y63" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="Z63" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="AA63" s="55"/>
-      <c r="AB63" s="55"/>
-      <c r="AC63" s="55"/>
+      <c r="AA63" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB63" s="55" t="s">
+        <v>736</v>
+      </c>
+      <c r="AC63" s="55" t="s">
+        <v>737</v>
+      </c>
       <c r="AD63" s="55"/>
       <c r="AE63" s="55"/>
       <c r="AF63" s="55"/>
       <c r="AG63" s="55" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="AH63" s="55"/>
       <c r="AI63" s="55"/>
@@ -11418,7 +11429,9 @@
       <c r="AQ63" s="55"/>
       <c r="AR63" s="55"/>
       <c r="AS63" s="55"/>
-      <c r="AT63" s="55"/>
+      <c r="AT63" s="55">
+        <v>2013</v>
+      </c>
       <c r="AU63" s="55"/>
       <c r="AV63" s="55"/>
       <c r="AW63" s="55"/>
@@ -11428,29 +11441,27 @@
     </row>
     <row r="64" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="54" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="B64" s="55" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
       <c r="C64" s="55" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="D64" s="55"/>
       <c r="E64" s="55" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="F64" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="G64" s="55" t="s">
-        <v>738</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G64" s="55"/>
       <c r="H64" s="55">
-        <v>508</v>
+        <v>203</v>
       </c>
       <c r="I64" s="55" t="s">
-        <v>739</v>
+        <v>743</v>
       </c>
       <c r="J64" s="55" t="s">
         <v>83</v>
@@ -11459,29 +11470,21 @@
         <v>83</v>
       </c>
       <c r="L64" s="56">
-        <v>6550</v>
+        <v>4728</v>
       </c>
       <c r="M64" s="56">
-        <v>25540051</v>
+        <v>26089200</v>
       </c>
       <c r="N64" s="56">
         <v>1</v>
       </c>
       <c r="O64" s="56">
-        <v>6550</v>
-      </c>
-      <c r="P64" s="56">
-        <v>391</v>
-      </c>
-      <c r="Q64" s="58">
-        <v>30438</v>
-      </c>
-      <c r="R64" s="55" t="s">
-        <v>740</v>
-      </c>
-      <c r="S64" s="55" t="s">
-        <v>735</v>
-      </c>
+        <v>4728</v>
+      </c>
+      <c r="P64" s="56"/>
+      <c r="Q64" s="56"/>
+      <c r="R64" s="55"/>
+      <c r="S64" s="55"/>
       <c r="T64" s="55" t="s">
         <v>85</v>
       </c>
@@ -11489,10 +11492,10 @@
         <v>85</v>
       </c>
       <c r="V64" s="66" t="s">
+        <v>744</v>
+      </c>
+      <c r="W64" s="66" t="s">
         <v>740</v>
-      </c>
-      <c r="W64" s="66" t="s">
-        <v>735</v>
       </c>
       <c r="X64" s="55" t="s">
         <v>85</v>
@@ -11501,22 +11504,24 @@
         <v>85</v>
       </c>
       <c r="Z64" s="55" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="AA64" s="55" t="s">
-        <v>124</v>
+        <v>19</v>
       </c>
       <c r="AB64" s="55" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
       <c r="AC64" s="55" t="s">
-        <v>742</v>
-      </c>
-      <c r="AD64" s="55"/>
+        <v>740</v>
+      </c>
+      <c r="AD64" s="55" t="s">
+        <v>745</v>
+      </c>
       <c r="AE64" s="55"/>
       <c r="AF64" s="55"/>
       <c r="AG64" s="55" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
       <c r="AH64" s="55"/>
       <c r="AI64" s="55"/>
@@ -11530,39 +11535,43 @@
       <c r="AQ64" s="55"/>
       <c r="AR64" s="55"/>
       <c r="AS64" s="55"/>
-      <c r="AT64" s="55">
-        <v>2013</v>
-      </c>
+      <c r="AT64" s="55"/>
       <c r="AU64" s="55"/>
       <c r="AV64" s="55"/>
       <c r="AW64" s="55"/>
-      <c r="AX64" s="56"/>
-      <c r="AY64" s="55"/>
+      <c r="AX64" s="56" t="s">
+        <v>746</v>
+      </c>
+      <c r="AY64" s="55" t="s">
+        <v>636</v>
+      </c>
       <c r="AZ64" s="57"/>
     </row>
     <row r="65" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="54" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="B65" s="55" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="C65" s="55" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="D65" s="55"/>
       <c r="E65" s="55" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="F65" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="G65" s="55"/>
+        <v>102</v>
+      </c>
+      <c r="G65" s="55" t="s">
+        <v>751</v>
+      </c>
       <c r="H65" s="55">
-        <v>203</v>
+        <v>401</v>
       </c>
       <c r="I65" s="55" t="s">
-        <v>748</v>
+        <v>752</v>
       </c>
       <c r="J65" s="55" t="s">
         <v>83</v>
@@ -11571,21 +11580,29 @@
         <v>83</v>
       </c>
       <c r="L65" s="56">
-        <v>4728</v>
+        <v>5938</v>
       </c>
       <c r="M65" s="56">
-        <v>26089200</v>
+        <v>25540013</v>
       </c>
       <c r="N65" s="56">
         <v>1</v>
       </c>
       <c r="O65" s="56">
-        <v>4728</v>
-      </c>
-      <c r="P65" s="56"/>
-      <c r="Q65" s="56"/>
-      <c r="R65" s="55"/>
-      <c r="S65" s="55"/>
+        <v>5938</v>
+      </c>
+      <c r="P65" s="56">
+        <v>203</v>
+      </c>
+      <c r="Q65" s="58">
+        <v>25332</v>
+      </c>
+      <c r="R65" s="55" t="s">
+        <v>753</v>
+      </c>
+      <c r="S65" s="55" t="s">
+        <v>748</v>
+      </c>
       <c r="T65" s="55" t="s">
         <v>85</v>
       </c>
@@ -11593,10 +11610,10 @@
         <v>85</v>
       </c>
       <c r="V65" s="66" t="s">
-        <v>749</v>
+        <v>753</v>
       </c>
       <c r="W65" s="66" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="X65" s="55" t="s">
         <v>85</v>
@@ -11611,18 +11628,16 @@
         <v>19</v>
       </c>
       <c r="AB65" s="55" t="s">
-        <v>749</v>
+        <v>754</v>
       </c>
       <c r="AC65" s="55" t="s">
-        <v>745</v>
-      </c>
-      <c r="AD65" s="55" t="s">
-        <v>750</v>
-      </c>
+        <v>755</v>
+      </c>
+      <c r="AD65" s="55"/>
       <c r="AE65" s="55"/>
       <c r="AF65" s="55"/>
       <c r="AG65" s="55" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="AH65" s="55"/>
       <c r="AI65" s="55"/>
@@ -11634,45 +11649,45 @@
       <c r="AO65" s="55"/>
       <c r="AP65" s="55"/>
       <c r="AQ65" s="55"/>
-      <c r="AR65" s="55"/>
+      <c r="AR65" s="55">
+        <v>2019</v>
+      </c>
       <c r="AS65" s="55"/>
       <c r="AT65" s="55"/>
       <c r="AU65" s="55"/>
       <c r="AV65" s="55"/>
       <c r="AW65" s="55"/>
       <c r="AX65" s="56" t="s">
-        <v>751</v>
-      </c>
-      <c r="AY65" s="55" t="s">
-        <v>641</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="AY65" s="55"/>
       <c r="AZ65" s="57"/>
     </row>
     <row r="66" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="54" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="B66" s="55" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="C66" s="55" t="s">
-        <v>754</v>
+        <v>758</v>
       </c>
       <c r="D66" s="55"/>
       <c r="E66" s="55" t="s">
-        <v>755</v>
+        <v>722</v>
       </c>
       <c r="F66" s="55" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
       <c r="G66" s="55" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
       <c r="H66" s="55">
-        <v>401</v>
-      </c>
-      <c r="I66" s="55" t="s">
-        <v>757</v>
+        <v>860</v>
+      </c>
+      <c r="I66" s="55">
+        <v>6117</v>
       </c>
       <c r="J66" s="55" t="s">
         <v>83</v>
@@ -11681,64 +11696,48 @@
         <v>83</v>
       </c>
       <c r="L66" s="56">
-        <v>5938</v>
+        <v>6178</v>
       </c>
       <c r="M66" s="56">
-        <v>25540013</v>
+        <v>25539914</v>
       </c>
       <c r="N66" s="56">
         <v>1</v>
       </c>
       <c r="O66" s="56">
-        <v>5938</v>
-      </c>
-      <c r="P66" s="56">
-        <v>203</v>
-      </c>
-      <c r="Q66" s="58">
-        <v>25332</v>
-      </c>
+        <v>6178</v>
+      </c>
+      <c r="P66" s="56"/>
+      <c r="Q66" s="56"/>
       <c r="R66" s="55" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="S66" s="55" t="s">
-        <v>753</v>
-      </c>
-      <c r="T66" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="U66" s="55" t="s">
-        <v>85</v>
-      </c>
+        <v>761</v>
+      </c>
+      <c r="T66" s="55"/>
+      <c r="U66" s="55"/>
       <c r="V66" s="66" t="s">
-        <v>758</v>
+        <v>852</v>
       </c>
       <c r="W66" s="66" t="s">
-        <v>753</v>
-      </c>
-      <c r="X66" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y66" s="55" t="s">
-        <v>85</v>
-      </c>
+        <v>757</v>
+      </c>
+      <c r="X66" s="55"/>
+      <c r="Y66" s="55"/>
       <c r="Z66" s="55" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="AA66" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB66" s="55" t="s">
-        <v>759</v>
-      </c>
-      <c r="AC66" s="55" t="s">
-        <v>760</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="AB66" s="55"/>
+      <c r="AC66" s="55"/>
       <c r="AD66" s="55"/>
       <c r="AE66" s="55"/>
       <c r="AF66" s="55"/>
       <c r="AG66" s="55" t="s">
-        <v>752</v>
+        <v>756</v>
       </c>
       <c r="AH66" s="55"/>
       <c r="AI66" s="55"/>
@@ -11750,45 +11749,39 @@
       <c r="AO66" s="55"/>
       <c r="AP66" s="55"/>
       <c r="AQ66" s="55"/>
-      <c r="AR66" s="55">
-        <v>2019</v>
-      </c>
+      <c r="AR66" s="55"/>
       <c r="AS66" s="55"/>
       <c r="AT66" s="55"/>
       <c r="AU66" s="55"/>
       <c r="AV66" s="55"/>
       <c r="AW66" s="55"/>
-      <c r="AX66" s="56" t="s">
-        <v>97</v>
-      </c>
+      <c r="AX66" s="56"/>
       <c r="AY66" s="55"/>
       <c r="AZ66" s="57"/>
     </row>
     <row r="67" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="54" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B67" s="55" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C67" s="55" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D67" s="55"/>
       <c r="E67" s="55" t="s">
-        <v>727</v>
+        <v>765</v>
       </c>
       <c r="F67" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="G67" s="55" t="s">
-        <v>764</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="G67" s="55"/>
       <c r="H67" s="55">
-        <v>860</v>
-      </c>
-      <c r="I67" s="55">
-        <v>6117</v>
+        <v>800</v>
+      </c>
+      <c r="I67" s="55" t="s">
+        <v>766</v>
       </c>
       <c r="J67" s="55" t="s">
         <v>83</v>
@@ -11797,48 +11790,56 @@
         <v>83</v>
       </c>
       <c r="L67" s="56">
-        <v>6178</v>
+        <v>6607</v>
       </c>
       <c r="M67" s="56">
-        <v>25539914</v>
+        <v>26089258</v>
       </c>
       <c r="N67" s="56">
         <v>1</v>
       </c>
       <c r="O67" s="56">
-        <v>6178</v>
+        <v>6607</v>
       </c>
       <c r="P67" s="56"/>
       <c r="Q67" s="56"/>
-      <c r="R67" s="55" t="s">
-        <v>765</v>
-      </c>
-      <c r="S67" s="55" t="s">
-        <v>766</v>
-      </c>
-      <c r="T67" s="55"/>
-      <c r="U67" s="55"/>
+      <c r="R67" s="55"/>
+      <c r="S67" s="55"/>
+      <c r="T67" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="U67" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="V67" s="66" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="W67" s="66" t="s">
-        <v>762</v>
-      </c>
-      <c r="X67" s="55"/>
-      <c r="Y67" s="55"/>
+        <v>763</v>
+      </c>
+      <c r="X67" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y67" s="55" t="s">
+        <v>85</v>
+      </c>
       <c r="Z67" s="55" t="s">
         <v>124</v>
       </c>
       <c r="AA67" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="AB67" s="55"/>
-      <c r="AC67" s="55"/>
+      <c r="AB67" s="55" t="s">
+        <v>767</v>
+      </c>
+      <c r="AC67" s="55" t="s">
+        <v>768</v>
+      </c>
       <c r="AD67" s="55"/>
       <c r="AE67" s="55"/>
       <c r="AF67" s="55"/>
       <c r="AG67" s="55" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="AH67" s="55"/>
       <c r="AI67" s="55"/>
@@ -11856,33 +11857,37 @@
       <c r="AU67" s="55"/>
       <c r="AV67" s="55"/>
       <c r="AW67" s="55"/>
-      <c r="AX67" s="56"/>
+      <c r="AX67" s="56" t="s">
+        <v>769</v>
+      </c>
       <c r="AY67" s="55"/>
       <c r="AZ67" s="57"/>
     </row>
     <row r="68" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="54" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="B68" s="55" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="C68" s="55" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="D68" s="55"/>
       <c r="E68" s="55" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="F68" s="55" t="s">
-        <v>293</v>
-      </c>
-      <c r="G68" s="55"/>
+        <v>80</v>
+      </c>
+      <c r="G68" s="55" t="s">
+        <v>774</v>
+      </c>
       <c r="H68" s="55">
-        <v>800</v>
+        <v>781</v>
       </c>
       <c r="I68" s="55" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="J68" s="55" t="s">
         <v>83</v>
@@ -11891,21 +11896,29 @@
         <v>83</v>
       </c>
       <c r="L68" s="56">
-        <v>6607</v>
+        <v>7911</v>
       </c>
       <c r="M68" s="56">
-        <v>26089258</v>
+        <v>25540115</v>
       </c>
       <c r="N68" s="56">
         <v>1</v>
       </c>
       <c r="O68" s="56">
-        <v>6607</v>
-      </c>
-      <c r="P68" s="56"/>
-      <c r="Q68" s="56"/>
-      <c r="R68" s="55"/>
-      <c r="S68" s="55"/>
+        <v>7911</v>
+      </c>
+      <c r="P68" s="56">
+        <v>424</v>
+      </c>
+      <c r="Q68" s="58">
+        <v>32258</v>
+      </c>
+      <c r="R68" s="55" t="s">
+        <v>776</v>
+      </c>
+      <c r="S68" s="55" t="s">
+        <v>771</v>
+      </c>
       <c r="T68" s="55" t="s">
         <v>85</v>
       </c>
@@ -11913,10 +11926,10 @@
         <v>85</v>
       </c>
       <c r="V68" s="66" t="s">
-        <v>858</v>
+        <v>776</v>
       </c>
       <c r="W68" s="66" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="X68" s="55" t="s">
         <v>85</v>
@@ -11931,64 +11944,86 @@
         <v>124</v>
       </c>
       <c r="AB68" s="55" t="s">
-        <v>772</v>
+        <v>777</v>
       </c>
       <c r="AC68" s="55" t="s">
-        <v>773</v>
+        <v>778</v>
       </c>
       <c r="AD68" s="55"/>
-      <c r="AE68" s="55"/>
+      <c r="AE68" s="55" t="s">
+        <v>779</v>
+      </c>
       <c r="AF68" s="55"/>
       <c r="AG68" s="55" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
       <c r="AH68" s="55"/>
       <c r="AI68" s="55"/>
-      <c r="AJ68" s="55"/>
-      <c r="AK68" s="55"/>
-      <c r="AL68" s="55"/>
-      <c r="AM68" s="55"/>
-      <c r="AN68" s="55"/>
-      <c r="AO68" s="55"/>
-      <c r="AP68" s="55"/>
-      <c r="AQ68" s="55"/>
-      <c r="AR68" s="55"/>
-      <c r="AS68" s="55"/>
+      <c r="AJ68" s="55" t="s">
+        <v>780</v>
+      </c>
+      <c r="AK68" s="55" t="s">
+        <v>781</v>
+      </c>
+      <c r="AL68" s="55" t="s">
+        <v>782</v>
+      </c>
+      <c r="AM68" s="55" t="s">
+        <v>783</v>
+      </c>
+      <c r="AN68" s="55" t="s">
+        <v>784</v>
+      </c>
+      <c r="AO68" s="55" t="s">
+        <v>785</v>
+      </c>
+      <c r="AP68" s="55" t="s">
+        <v>786</v>
+      </c>
+      <c r="AQ68" s="55" t="s">
+        <v>787</v>
+      </c>
+      <c r="AR68" s="55" t="s">
+        <v>788</v>
+      </c>
+      <c r="AS68" s="55">
+        <v>2013</v>
+      </c>
       <c r="AT68" s="55"/>
       <c r="AU68" s="55"/>
       <c r="AV68" s="55"/>
       <c r="AW68" s="55"/>
       <c r="AX68" s="56" t="s">
-        <v>774</v>
-      </c>
-      <c r="AY68" s="55"/>
+        <v>789</v>
+      </c>
+      <c r="AY68" s="55">
+        <v>2016</v>
+      </c>
       <c r="AZ68" s="57"/>
     </row>
     <row r="69" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="54" t="s">
-        <v>775</v>
+        <v>790</v>
       </c>
       <c r="B69" s="55" t="s">
-        <v>776</v>
+        <v>791</v>
       </c>
       <c r="C69" s="55" t="s">
-        <v>777</v>
+        <v>792</v>
       </c>
       <c r="D69" s="55"/>
       <c r="E69" s="55" t="s">
-        <v>778</v>
+        <v>793</v>
       </c>
       <c r="F69" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="G69" s="55" t="s">
-        <v>779</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="G69" s="55"/>
       <c r="H69" s="55">
-        <v>781</v>
+        <v>860</v>
       </c>
       <c r="I69" s="55" t="s">
-        <v>780</v>
+        <v>794</v>
       </c>
       <c r="J69" s="55" t="s">
         <v>83</v>
@@ -11997,29 +12032,21 @@
         <v>83</v>
       </c>
       <c r="L69" s="56">
-        <v>7911</v>
+        <v>7920</v>
       </c>
       <c r="M69" s="56">
-        <v>25540115</v>
+        <v>26089292</v>
       </c>
       <c r="N69" s="56">
         <v>1</v>
       </c>
       <c r="O69" s="56">
-        <v>7911</v>
-      </c>
-      <c r="P69" s="56">
-        <v>424</v>
-      </c>
-      <c r="Q69" s="58">
-        <v>32258</v>
-      </c>
-      <c r="R69" s="55" t="s">
-        <v>781</v>
-      </c>
-      <c r="S69" s="55" t="s">
-        <v>776</v>
-      </c>
+        <v>7920</v>
+      </c>
+      <c r="P69" s="56"/>
+      <c r="Q69" s="56"/>
+      <c r="R69" s="55"/>
+      <c r="S69" s="55"/>
       <c r="T69" s="55" t="s">
         <v>85</v>
       </c>
@@ -12027,16 +12054,16 @@
         <v>85</v>
       </c>
       <c r="V69" s="66" t="s">
-        <v>781</v>
+        <v>854</v>
       </c>
       <c r="W69" s="66" t="s">
-        <v>776</v>
+        <v>791</v>
       </c>
       <c r="X69" s="55" t="s">
-        <v>85</v>
+        <v>795</v>
       </c>
       <c r="Y69" s="55" t="s">
-        <v>85</v>
+        <v>796</v>
       </c>
       <c r="Z69" s="55" t="s">
         <v>124</v>
@@ -12045,86 +12072,70 @@
         <v>124</v>
       </c>
       <c r="AB69" s="55" t="s">
-        <v>782</v>
+        <v>797</v>
       </c>
       <c r="AC69" s="55" t="s">
-        <v>783</v>
-      </c>
-      <c r="AD69" s="55"/>
+        <v>798</v>
+      </c>
+      <c r="AD69" s="55">
+        <v>8606852046</v>
+      </c>
       <c r="AE69" s="55" t="s">
-        <v>784</v>
+        <v>799</v>
       </c>
       <c r="AF69" s="55"/>
       <c r="AG69" s="55" t="s">
-        <v>775</v>
+        <v>790</v>
       </c>
       <c r="AH69" s="55"/>
       <c r="AI69" s="55"/>
       <c r="AJ69" s="55" t="s">
-        <v>785</v>
-      </c>
-      <c r="AK69" s="55" t="s">
-        <v>786</v>
-      </c>
-      <c r="AL69" s="55" t="s">
-        <v>787</v>
-      </c>
-      <c r="AM69" s="55" t="s">
-        <v>788</v>
-      </c>
-      <c r="AN69" s="55" t="s">
-        <v>789</v>
-      </c>
-      <c r="AO69" s="55" t="s">
-        <v>790</v>
-      </c>
-      <c r="AP69" s="55" t="s">
-        <v>791</v>
-      </c>
-      <c r="AQ69" s="55" t="s">
-        <v>792</v>
-      </c>
-      <c r="AR69" s="55" t="s">
-        <v>793</v>
-      </c>
+        <v>800</v>
+      </c>
+      <c r="AK69" s="55"/>
+      <c r="AL69" s="55"/>
+      <c r="AM69" s="55"/>
+      <c r="AN69" s="55"/>
+      <c r="AO69" s="55"/>
+      <c r="AP69" s="55"/>
+      <c r="AQ69" s="55"/>
+      <c r="AR69" s="55"/>
       <c r="AS69" s="55">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="AT69" s="55"/>
       <c r="AU69" s="55"/>
       <c r="AV69" s="55"/>
       <c r="AW69" s="55"/>
       <c r="AX69" s="56" t="s">
-        <v>794</v>
-      </c>
-      <c r="AY69" s="55">
-        <v>2016</v>
-      </c>
+        <v>801</v>
+      </c>
+      <c r="AY69" s="55"/>
       <c r="AZ69" s="57"/>
     </row>
     <row r="70" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="54" t="s">
-        <v>795</v>
+        <v>802</v>
       </c>
       <c r="B70" s="55" t="s">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="C70" s="55" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="D70" s="55"/>
       <c r="E70" s="55" t="s">
-        <v>798</v>
+        <v>805</v>
       </c>
       <c r="F70" s="55" t="s">
         <v>133</v>
       </c>
       <c r="G70" s="55"/>
       <c r="H70" s="55">
-        <v>860</v>
+        <v>877</v>
       </c>
       <c r="I70" s="55" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
       <c r="J70" s="55" t="s">
         <v>83</v>
@@ -12133,16 +12144,16 @@
         <v>83</v>
       </c>
       <c r="L70" s="56">
-        <v>7920</v>
+        <v>8028</v>
       </c>
       <c r="M70" s="56">
-        <v>26089292</v>
+        <v>26089294</v>
       </c>
       <c r="N70" s="56">
         <v>1</v>
       </c>
       <c r="O70" s="56">
-        <v>7920</v>
+        <v>8028</v>
       </c>
       <c r="P70" s="56"/>
       <c r="Q70" s="56"/>
@@ -12155,16 +12166,16 @@
         <v>85</v>
       </c>
       <c r="V70" s="66" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="W70" s="66" t="s">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="X70" s="55" t="s">
-        <v>800</v>
+        <v>85</v>
       </c>
       <c r="Y70" s="55" t="s">
-        <v>801</v>
+        <v>85</v>
       </c>
       <c r="Z70" s="55" t="s">
         <v>124</v>
@@ -12173,26 +12184,20 @@
         <v>124</v>
       </c>
       <c r="AB70" s="55" t="s">
-        <v>802</v>
+        <v>807</v>
       </c>
       <c r="AC70" s="55" t="s">
-        <v>803</v>
-      </c>
-      <c r="AD70" s="55">
-        <v>8606852046</v>
-      </c>
-      <c r="AE70" s="55" t="s">
-        <v>804</v>
-      </c>
+        <v>808</v>
+      </c>
+      <c r="AD70" s="55"/>
+      <c r="AE70" s="55"/>
       <c r="AF70" s="55"/>
       <c r="AG70" s="55" t="s">
-        <v>795</v>
+        <v>802</v>
       </c>
       <c r="AH70" s="55"/>
       <c r="AI70" s="55"/>
-      <c r="AJ70" s="55" t="s">
-        <v>805</v>
-      </c>
+      <c r="AJ70" s="55"/>
       <c r="AK70" s="55"/>
       <c r="AL70" s="55"/>
       <c r="AM70" s="55"/>
@@ -12201,100 +12206,68 @@
       <c r="AP70" s="55"/>
       <c r="AQ70" s="55"/>
       <c r="AR70" s="55"/>
-      <c r="AS70" s="55">
-        <v>2016</v>
-      </c>
+      <c r="AS70" s="55"/>
       <c r="AT70" s="55"/>
       <c r="AU70" s="55"/>
       <c r="AV70" s="55"/>
       <c r="AW70" s="55"/>
       <c r="AX70" s="56" t="s">
-        <v>806</v>
+        <v>416</v>
       </c>
       <c r="AY70" s="55"/>
       <c r="AZ70" s="57"/>
     </row>
     <row r="71" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="54" t="s">
-        <v>807</v>
-      </c>
-      <c r="B71" s="55" t="s">
-        <v>808</v>
-      </c>
-      <c r="C71" s="55" t="s">
         <v>809</v>
       </c>
+      <c r="B71" s="55"/>
+      <c r="C71" s="55"/>
       <c r="D71" s="55"/>
-      <c r="E71" s="55" t="s">
-        <v>810</v>
-      </c>
-      <c r="F71" s="55" t="s">
-        <v>133</v>
-      </c>
+      <c r="E71" s="55"/>
+      <c r="F71" s="55"/>
       <c r="G71" s="55"/>
       <c r="H71" s="55">
-        <v>877</v>
-      </c>
-      <c r="I71" s="55" t="s">
-        <v>811</v>
-      </c>
+        <v>413</v>
+      </c>
+      <c r="I71" s="55"/>
       <c r="J71" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K71" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L71" s="56">
-        <v>8028</v>
-      </c>
+      <c r="L71" s="56"/>
       <c r="M71" s="56">
-        <v>26089294</v>
+        <v>36581819</v>
       </c>
       <c r="N71" s="56">
         <v>1</v>
       </c>
       <c r="O71" s="56">
-        <v>8028</v>
+        <v>8085</v>
       </c>
       <c r="P71" s="56"/>
       <c r="Q71" s="56"/>
       <c r="R71" s="55"/>
       <c r="S71" s="55"/>
-      <c r="T71" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="U71" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="V71" s="66" t="s">
-        <v>860</v>
-      </c>
-      <c r="W71" s="66" t="s">
-        <v>808</v>
-      </c>
-      <c r="X71" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y71" s="55" t="s">
-        <v>85</v>
-      </c>
+      <c r="T71" s="55"/>
+      <c r="U71" s="55"/>
+      <c r="V71" s="66"/>
+      <c r="W71" s="66"/>
+      <c r="X71" s="55"/>
+      <c r="Y71" s="55"/>
       <c r="Z71" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="AA71" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB71" s="55" t="s">
-        <v>812</v>
-      </c>
-      <c r="AC71" s="55" t="s">
-        <v>813</v>
-      </c>
+      <c r="AA71" s="55"/>
+      <c r="AB71" s="55"/>
+      <c r="AC71" s="55"/>
       <c r="AD71" s="55"/>
       <c r="AE71" s="55"/>
       <c r="AF71" s="55"/>
       <c r="AG71" s="55" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="AH71" s="55"/>
       <c r="AI71" s="55"/>
@@ -12312,41 +12285,53 @@
       <c r="AU71" s="55"/>
       <c r="AV71" s="55"/>
       <c r="AW71" s="55"/>
-      <c r="AX71" s="56" t="s">
-        <v>416</v>
-      </c>
+      <c r="AX71" s="56"/>
       <c r="AY71" s="55"/>
       <c r="AZ71" s="57"/>
     </row>
     <row r="72" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="54" t="s">
+        <v>810</v>
+      </c>
+      <c r="B72" s="55" t="s">
+        <v>811</v>
+      </c>
+      <c r="C72" s="55" t="s">
+        <v>812</v>
+      </c>
+      <c r="D72" s="55"/>
+      <c r="E72" s="55" t="s">
+        <v>813</v>
+      </c>
+      <c r="F72" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="G72" s="55" t="s">
         <v>814</v>
       </c>
-      <c r="B72" s="55"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="55"/>
-      <c r="E72" s="55"/>
-      <c r="F72" s="55"/>
-      <c r="G72" s="55"/>
       <c r="H72" s="55">
         <v>413</v>
       </c>
-      <c r="I72" s="55"/>
+      <c r="I72" s="55" t="s">
+        <v>815</v>
+      </c>
       <c r="J72" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K72" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L72" s="56"/>
+      <c r="L72" s="56">
+        <v>8253</v>
+      </c>
       <c r="M72" s="56">
-        <v>36581819</v>
+        <v>29345753</v>
       </c>
       <c r="N72" s="56">
         <v>1</v>
       </c>
       <c r="O72" s="56">
-        <v>8085</v>
+        <v>8253</v>
       </c>
       <c r="P72" s="56"/>
       <c r="Q72" s="56"/>
@@ -12354,21 +12339,29 @@
       <c r="S72" s="55"/>
       <c r="T72" s="55"/>
       <c r="U72" s="55"/>
-      <c r="V72" s="66"/>
-      <c r="W72" s="66"/>
+      <c r="V72" s="66" t="s">
+        <v>816</v>
+      </c>
+      <c r="W72" s="66" t="s">
+        <v>811</v>
+      </c>
       <c r="X72" s="55"/>
       <c r="Y72" s="55"/>
-      <c r="Z72" s="55" t="s">
-        <v>124</v>
-      </c>
+      <c r="Z72" s="55"/>
       <c r="AA72" s="55"/>
-      <c r="AB72" s="55"/>
-      <c r="AC72" s="55"/>
-      <c r="AD72" s="55"/>
+      <c r="AB72" s="55" t="s">
+        <v>816</v>
+      </c>
+      <c r="AC72" s="55" t="s">
+        <v>811</v>
+      </c>
+      <c r="AD72" s="55" t="s">
+        <v>817</v>
+      </c>
       <c r="AE72" s="55"/>
       <c r="AF72" s="55"/>
       <c r="AG72" s="55" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="AH72" s="55"/>
       <c r="AI72" s="55"/>
@@ -12386,53 +12379,41 @@
       <c r="AU72" s="55"/>
       <c r="AV72" s="55"/>
       <c r="AW72" s="55"/>
-      <c r="AX72" s="56"/>
+      <c r="AX72" s="56" t="s">
+        <v>97</v>
+      </c>
       <c r="AY72" s="55"/>
       <c r="AZ72" s="57"/>
     </row>
     <row r="73" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="54" t="s">
-        <v>815</v>
-      </c>
-      <c r="B73" s="55" t="s">
-        <v>816</v>
-      </c>
-      <c r="C73" s="55" t="s">
-        <v>817</v>
-      </c>
+        <v>818</v>
+      </c>
+      <c r="B73" s="55"/>
+      <c r="C73" s="55"/>
       <c r="D73" s="55"/>
-      <c r="E73" s="55" t="s">
-        <v>818</v>
-      </c>
-      <c r="F73" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="G73" s="55" t="s">
-        <v>819</v>
-      </c>
+      <c r="E73" s="55"/>
+      <c r="F73" s="55"/>
+      <c r="G73" s="55"/>
       <c r="H73" s="55">
-        <v>413</v>
-      </c>
-      <c r="I73" s="55" t="s">
-        <v>820</v>
-      </c>
+        <v>508</v>
+      </c>
+      <c r="I73" s="55"/>
       <c r="J73" s="55" t="s">
         <v>83</v>
       </c>
       <c r="K73" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="L73" s="56">
-        <v>8253</v>
-      </c>
+      <c r="L73" s="56"/>
       <c r="M73" s="56">
-        <v>29345753</v>
+        <v>36581834</v>
       </c>
       <c r="N73" s="56">
         <v>1</v>
       </c>
       <c r="O73" s="56">
-        <v>8253</v>
+        <v>8415</v>
       </c>
       <c r="P73" s="56"/>
       <c r="Q73" s="56"/>
@@ -12440,29 +12421,21 @@
       <c r="S73" s="55"/>
       <c r="T73" s="55"/>
       <c r="U73" s="55"/>
-      <c r="V73" s="66" t="s">
-        <v>821</v>
-      </c>
-      <c r="W73" s="66" t="s">
-        <v>816</v>
-      </c>
+      <c r="V73" s="66"/>
+      <c r="W73" s="66"/>
       <c r="X73" s="55"/>
       <c r="Y73" s="55"/>
-      <c r="Z73" s="55"/>
+      <c r="Z73" s="55" t="s">
+        <v>19</v>
+      </c>
       <c r="AA73" s="55"/>
-      <c r="AB73" s="55" t="s">
-        <v>821</v>
-      </c>
-      <c r="AC73" s="55" t="s">
-        <v>816</v>
-      </c>
-      <c r="AD73" s="55" t="s">
-        <v>822</v>
-      </c>
+      <c r="AB73" s="55"/>
+      <c r="AC73" s="55"/>
+      <c r="AD73" s="55"/>
       <c r="AE73" s="55"/>
       <c r="AF73" s="55"/>
       <c r="AG73" s="55" t="s">
-        <v>815</v>
+        <v>818</v>
       </c>
       <c r="AH73" s="55"/>
       <c r="AI73" s="55"/>
@@ -12480,85 +12453,65 @@
       <c r="AU73" s="55"/>
       <c r="AV73" s="55"/>
       <c r="AW73" s="55"/>
-      <c r="AX73" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="AY73" s="55"/>
+      <c r="AX73" s="56"/>
+      <c r="AY73" s="55" t="s">
+        <v>819</v>
+      </c>
       <c r="AZ73" s="57"/>
     </row>
-    <row r="74" spans="1:52" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="54" t="s">
-        <v>823</v>
-      </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="55"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="55"/>
-      <c r="H74" s="55">
-        <v>508</v>
-      </c>
-      <c r="I74" s="55"/>
-      <c r="J74" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="K74" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="L74" s="56"/>
-      <c r="M74" s="56">
-        <v>36581834</v>
-      </c>
-      <c r="N74" s="56">
-        <v>1</v>
-      </c>
-      <c r="O74" s="56">
-        <v>8415</v>
-      </c>
-      <c r="P74" s="56"/>
-      <c r="Q74" s="56"/>
-      <c r="R74" s="55"/>
-      <c r="S74" s="55"/>
-      <c r="T74" s="55"/>
-      <c r="U74" s="55"/>
-      <c r="V74" s="66"/>
-      <c r="W74" s="66"/>
-      <c r="X74" s="55"/>
-      <c r="Y74" s="55"/>
-      <c r="Z74" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA74" s="55"/>
-      <c r="AB74" s="55"/>
-      <c r="AC74" s="55"/>
-      <c r="AD74" s="55"/>
-      <c r="AE74" s="55"/>
-      <c r="AF74" s="55"/>
-      <c r="AG74" s="55" t="s">
-        <v>823</v>
-      </c>
-      <c r="AH74" s="55"/>
-      <c r="AI74" s="55"/>
-      <c r="AJ74" s="55"/>
-      <c r="AK74" s="55"/>
-      <c r="AL74" s="55"/>
-      <c r="AM74" s="55"/>
-      <c r="AN74" s="55"/>
-      <c r="AO74" s="55"/>
-      <c r="AP74" s="55"/>
-      <c r="AQ74" s="55"/>
-      <c r="AR74" s="55"/>
-      <c r="AS74" s="55"/>
-      <c r="AT74" s="55"/>
-      <c r="AU74" s="55"/>
-      <c r="AV74" s="55"/>
-      <c r="AW74" s="55"/>
-      <c r="AX74" s="56"/>
-      <c r="AY74" s="55" t="s">
-        <v>824</v>
-      </c>
-      <c r="AZ74" s="57"/>
+    <row r="74" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="4"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="4"/>
+      <c r="L74" s="4"/>
+      <c r="M74" s="4"/>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="4"/>
+      <c r="S74" s="4"/>
+      <c r="T74" s="4"/>
+      <c r="U74" s="4"/>
+      <c r="V74" s="4"/>
+      <c r="W74" s="4"/>
+      <c r="X74" s="4"/>
+      <c r="Y74" s="4"/>
+      <c r="Z74" s="4"/>
+      <c r="AA74" s="4"/>
+      <c r="AB74" s="4"/>
+      <c r="AC74" s="4"/>
+      <c r="AD74" s="4"/>
+      <c r="AE74" s="4"/>
+      <c r="AF74" s="4"/>
+      <c r="AG74" s="4"/>
+      <c r="AH74" s="4"/>
+      <c r="AI74" s="4"/>
+      <c r="AJ74" s="4"/>
+      <c r="AK74" s="4"/>
+      <c r="AL74" s="4"/>
+      <c r="AM74" s="4"/>
+      <c r="AN74" s="4"/>
+      <c r="AO74" s="4"/>
+      <c r="AP74" s="4"/>
+      <c r="AQ74" s="4"/>
+      <c r="AR74" s="4"/>
+      <c r="AS74" s="4"/>
+      <c r="AT74" s="4"/>
+      <c r="AU74" s="4"/>
+      <c r="AV74" s="4"/>
+      <c r="AW74" s="4"/>
+      <c r="AX74" s="4"/>
+      <c r="AY74" s="4"/>
+      <c r="AZ74" s="4"/>
     </row>
     <row r="75" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4"/>
@@ -62510,60 +62463,6 @@
       <c r="AY999" s="4"/>
       <c r="AZ999" s="4"/>
     </row>
-    <row r="1000" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1000" s="4"/>
-      <c r="B1000" s="4"/>
-      <c r="C1000" s="4"/>
-      <c r="D1000" s="4"/>
-      <c r="E1000" s="4"/>
-      <c r="F1000" s="4"/>
-      <c r="G1000" s="4"/>
-      <c r="H1000" s="4"/>
-      <c r="I1000" s="4"/>
-      <c r="J1000" s="4"/>
-      <c r="K1000" s="4"/>
-      <c r="L1000" s="4"/>
-      <c r="M1000" s="4"/>
-      <c r="N1000" s="4"/>
-      <c r="O1000" s="4"/>
-      <c r="P1000" s="4"/>
-      <c r="Q1000" s="4"/>
-      <c r="R1000" s="4"/>
-      <c r="S1000" s="4"/>
-      <c r="T1000" s="4"/>
-      <c r="U1000" s="4"/>
-      <c r="V1000" s="4"/>
-      <c r="W1000" s="4"/>
-      <c r="X1000" s="4"/>
-      <c r="Y1000" s="4"/>
-      <c r="Z1000" s="4"/>
-      <c r="AA1000" s="4"/>
-      <c r="AB1000" s="4"/>
-      <c r="AC1000" s="4"/>
-      <c r="AD1000" s="4"/>
-      <c r="AE1000" s="4"/>
-      <c r="AF1000" s="4"/>
-      <c r="AG1000" s="4"/>
-      <c r="AH1000" s="4"/>
-      <c r="AI1000" s="4"/>
-      <c r="AJ1000" s="4"/>
-      <c r="AK1000" s="4"/>
-      <c r="AL1000" s="4"/>
-      <c r="AM1000" s="4"/>
-      <c r="AN1000" s="4"/>
-      <c r="AO1000" s="4"/>
-      <c r="AP1000" s="4"/>
-      <c r="AQ1000" s="4"/>
-      <c r="AR1000" s="4"/>
-      <c r="AS1000" s="4"/>
-      <c r="AT1000" s="4"/>
-      <c r="AU1000" s="4"/>
-      <c r="AV1000" s="4"/>
-      <c r="AW1000" s="4"/>
-      <c r="AX1000" s="4"/>
-      <c r="AY1000" s="4"/>
-      <c r="AZ1000" s="4"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="AC4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>

</xml_diff>

<commit_message>
Move functional code from playground to main area
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E67F1B9-E239-6544-8A32-D86F55B61DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9999BA5F-5D47-0E47-8E85-66F9A37F5979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4547,10 +4547,10 @@
   <dimension ref="A1:AZ999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AH2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI18" sqref="AI18"/>
+      <selection pane="bottomRight" activeCell="AH28" sqref="AH28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add current code to playground for testing
I am now testing out the new code for Updating the ‘Custom Field Data - Chapter Reports’ Column (Not Concerning Ourselves with Color Coding Yet).
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9999BA5F-5D47-0E47-8E85-66F9A37F5979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33811DA0-8DEA-5346-AC5E-B5B9D256F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-1360" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="-860" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Overview" sheetId="1" r:id="rId1"/>
@@ -3347,7 +3347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4547,10 +4549,10 @@
   <dimension ref="A1:AZ999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AW2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AH28" sqref="AH28"/>
+      <selection pane="bottomRight" activeCell="BA22" sqref="BA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add a docstring to `update_record`
</commit_message>
<xml_diff>
--- a/Zone 1 Activity.xlsx
+++ b/Zone 1 Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180BFF75-546B-A741-8B2F-21EA7F499E13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B490B6-9358-6C49-AF6B-8F2E14464A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Overview" sheetId="1" r:id="rId1"/>
@@ -4411,15 +4411,15 @@
   <dimension ref="A1:AZ999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AK2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AF20" sqref="AF20"/>
+      <selection pane="bottomRight" activeCell="AL30" sqref="AL30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.1640625" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" customWidth="1"/>
     <col min="4" max="4" width="45.33203125" customWidth="1"/>
@@ -4452,11 +4452,9 @@
     <col min="32" max="32" width="54" customWidth="1"/>
     <col min="33" max="33" width="61.1640625" customWidth="1"/>
     <col min="34" max="34" width="70.33203125" customWidth="1"/>
-    <col min="35" max="35" width="74.6640625" customWidth="1"/>
-    <col min="36" max="36" width="75.1640625" customWidth="1"/>
-    <col min="37" max="37" width="75" customWidth="1"/>
-    <col min="38" max="38" width="70.33203125" customWidth="1"/>
-    <col min="39" max="39" width="70.1640625" customWidth="1"/>
+    <col min="35" max="35" width="53" customWidth="1"/>
+    <col min="36" max="37" width="57" customWidth="1"/>
+    <col min="38" max="39" width="53.33203125" customWidth="1"/>
     <col min="40" max="40" width="70.33203125" customWidth="1"/>
     <col min="41" max="41" width="70.1640625" customWidth="1"/>
     <col min="42" max="42" width="135.83203125" customWidth="1"/>

</xml_diff>